<commit_message>
TD ML = 1200
</commit_message>
<xml_diff>
--- a/webserver/model_data/TrainingData_ml.xlsx
+++ b/webserver/model_data/TrainingData_ml.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12622" uniqueCount="1947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13157" uniqueCount="2032">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -5471,9 +5471,6 @@
     <t>Dort machen sie dann auch Erfahrungen mit Menschen anderer Herkunft, die sie selbst dort prägen, wo sie nicht positiv sind.</t>
   </si>
   <si>
-    <t>0.0.2</t>
-  </si>
-  <si>
     <t>ZeitGeistGestörter</t>
   </si>
   <si>
@@ -5868,6 +5865,264 @@
   </si>
   <si>
     <t>Björn van Zwoll</t>
+  </si>
+  <si>
+    <t>Mit Leuten wie Borjans geht sowas gar nicht</t>
+  </si>
+  <si>
+    <t>Waere hoechste Zeit fuer eine solche Reform.</t>
+  </si>
+  <si>
+    <t>Heike-Doreen Ehling</t>
+  </si>
+  <si>
+    <t>SJ hat wirklich in vielen Rollen brilliert</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/kultur/film/2020-02/scarlett-johansson-oscar-verleihung-nomierung-film/seite-2</t>
+  </si>
+  <si>
+    <t>Tobmal</t>
+  </si>
+  <si>
+    <t>Die Bandbreite der Genres ist groß</t>
+  </si>
+  <si>
+    <t>Sie hat es wirklich verdient!</t>
+  </si>
+  <si>
+    <t>Sorry, aber da fällt mir erstmal Isabelle Huppert ein</t>
+  </si>
+  <si>
+    <t>prinzessin.leia</t>
+  </si>
+  <si>
+    <t>Wahnsinnig schön, vielseitig und x-fach ausgezeichnet</t>
+  </si>
+  <si>
+    <t>Marriage Story ist wirklich ein hervorragender Film.</t>
+  </si>
+  <si>
+    <t>stadtmutter</t>
+  </si>
+  <si>
+    <t>Lohnt sich.</t>
+  </si>
+  <si>
+    <t>Vielleicht für Frauen.</t>
+  </si>
+  <si>
+    <t>Ich als Mann kann mich der Meinung nur anschließen und den Film uneingeschränkt empfehlen.</t>
+  </si>
+  <si>
+    <t>Ich konnte beide Partnern der Ehe sehr gut mitfühlen.</t>
+  </si>
+  <si>
+    <t>Adam Drive und Scarlett Johansson spielen ihre Rollen wirklich sehr authentisch und nahbar.</t>
+  </si>
+  <si>
+    <t>Zwar toll gespielt, aber die Story hat ihre Schwächen und unnötige Längen.</t>
+  </si>
+  <si>
+    <t>Heinrich der Föwler</t>
+  </si>
+  <si>
+    <t>DM aus K</t>
+  </si>
+  <si>
+    <t>Fanfähnchen</t>
+  </si>
+  <si>
+    <t>Scarlett Johansson ist eine absolut grandiose Schauspielerin!</t>
+  </si>
+  <si>
+    <t>Xy-ungelöst</t>
+  </si>
+  <si>
+    <t>Leider mag ich viele ihrer Filme nicht, was allerdings nie an ihr liegt</t>
+  </si>
+  <si>
+    <t>Zweifelsohne eine gute Schauspielerin</t>
+  </si>
+  <si>
+    <t>Einen Film mit Scarlett Johansson unbedingt in der Originalfassung ansehen/anhören.</t>
+  </si>
+  <si>
+    <t>elfotografo</t>
+  </si>
+  <si>
+    <t>Ihre Stimme ist noch einmal genauso sexy wie Ihr Aussehen, Ihre Ausstrahlung.</t>
+  </si>
+  <si>
+    <t>Glauben Sie ernsthaft, Ihr Vorredner kommt über den Trailer hinaus?</t>
+  </si>
+  <si>
+    <t>astor131</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>Die CDU sollte sich auf Ihrer Werte besinnen und auf das C das sie im Namen trägt.</t>
+  </si>
+  <si>
+    <t>jgbk</t>
+  </si>
+  <si>
+    <t>Mit dem U und besonders dem D haben die aber auch so ihre Probleme.</t>
+  </si>
+  <si>
+    <t>cnlzeitonline</t>
+  </si>
+  <si>
+    <t>Welche Werte? Wann war die CDU" Christlich", außer das sie das C im Namen trägt?</t>
+  </si>
+  <si>
+    <t>selten dämliche Überschrift</t>
+  </si>
+  <si>
+    <t>riennevaplus</t>
+  </si>
+  <si>
+    <t>Valerian I</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/politik/deutschland/2020-02/cdu-nachfolge-jens-spahn-armin-laschet-friedrich-merz</t>
+  </si>
+  <si>
+    <t>Ich hätte gern mal jemand junges</t>
+  </si>
+  <si>
+    <t>Arisaka</t>
+  </si>
+  <si>
+    <t>Vielleicht fliegt man damit auf die Nase, aber ich würde es gerne ausprobieren.</t>
+  </si>
+  <si>
+    <t>Nein ernsthaft: Die jüngeren können sich nicht durchsetzen</t>
+  </si>
+  <si>
+    <t>Slackovic</t>
+  </si>
+  <si>
+    <t>Na gut, dann halt Laschet als kleinstes Übel.</t>
+  </si>
+  <si>
+    <t>Was für eine dürftige Auswahl:</t>
+  </si>
+  <si>
+    <t>Friedrich Merz, der das Auslaufmodell Neoliberalismus der 80er Jahre wieder zurück haben will</t>
+  </si>
+  <si>
+    <t>Armin Laschet, der es nicht mal geschafft hat, in seinem Bundesland ein Waldstück in den Griff zu bekommen</t>
+  </si>
+  <si>
+    <t>Jens Spahn, der zwar als einziger der Unions-Minister fleißig und professionell arbeitet, aber das Image des ewigen Karrieristen nicht los wird.</t>
+  </si>
+  <si>
+    <t>Gut finde ich das nicht</t>
+  </si>
+  <si>
+    <t>Sommerrolle</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/politik/deutschland/2020-02/annegret-kramp-karrenbauer-ruecktritt-cdu</t>
+  </si>
+  <si>
+    <t>ich befürchte, dass die Zeit der großen Volksparteien dem Ende entgegen geht.</t>
+  </si>
+  <si>
+    <t>Und auf Verhältnisse wie die in Italien zusteuern.</t>
+  </si>
+  <si>
+    <t>Ich hielt Merz immer für ein Grossmaul ohne viel dahinter, und ich kann nicht sehen dass sich daran viel geändert hat.</t>
+  </si>
+  <si>
+    <t>Die sichere Wahl für die CDU ist Laschet, die mutige Wahl Spahn.</t>
+  </si>
+  <si>
+    <t>HKaspar</t>
+  </si>
+  <si>
+    <t>das ist das beste was den Grünen passieren kann</t>
+  </si>
+  <si>
+    <t>Direkte Demokratie 1</t>
+  </si>
+  <si>
+    <t>Ganz Deutschrap left the CHAT</t>
+  </si>
+  <si>
+    <t>Gülcan Kara</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LgFQS4u--H0</t>
+  </si>
+  <si>
+    <t>Was ist das für ne sprache denkt sich jeder mero fan :))</t>
+  </si>
+  <si>
+    <t>Hadii Bakaliim</t>
+  </si>
+  <si>
+    <t>Das ist rap Punkt und jeder der damals schon deutschrap gehört hat weiß das</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Man kann sagen was man will, aber Bushidos Stimme ist für so Shit wie gemacht.</t>
+  </si>
+  <si>
+    <t>Hisoka</t>
+  </si>
+  <si>
+    <t>Brett.. Warte schon auf Sonny Black 2</t>
+  </si>
+  <si>
+    <t>Dr Dodi</t>
+  </si>
+  <si>
+    <t>Guter Beat, guter Texzt! CCN 4 einfach ein Meisterwerk</t>
+  </si>
+  <si>
+    <t>P****HanneZ CCN4</t>
+  </si>
+  <si>
+    <t>Ich finde es nice dass du den alten beats treu bleibst</t>
+  </si>
+  <si>
+    <t>DJ_DBM Music</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>Das Album wird sich jetzt gegönnt</t>
+  </si>
+  <si>
+    <t>Beste line</t>
+  </si>
+  <si>
+    <t>M2ilfschnitte</t>
+  </si>
+  <si>
+    <t>Sachlich gesehen ist der Rap schon geil</t>
+  </si>
+  <si>
+    <t>Florian Harings</t>
+  </si>
+  <si>
+    <t>Bushido ist der beste und bleibt auch der beste</t>
+  </si>
+  <si>
+    <t>Volkan Erisoglu</t>
+  </si>
+  <si>
+    <t>Guter stuff. Auch stimmlich gute Combo.</t>
+  </si>
+  <si>
+    <t>Patrick Fame</t>
   </si>
 </sst>
 </file>
@@ -6227,12 +6482,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1150"/>
+  <dimension ref="A1:W1200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="158" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1133" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1189" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="M1150" sqref="M1150:N1150"/>
+      <selection pane="bottomLeft" activeCell="M1197" sqref="M1197:N1200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -61368,7 +61623,7 @@
         <v>18</v>
       </c>
       <c r="R1078" t="s">
-        <v>1814</v>
+        <v>250</v>
       </c>
       <c r="S1078">
         <v>0.28000000000000003</v>
@@ -61391,16 +61646,16 @@
         <v>1234</v>
       </c>
       <c r="L1079" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="M1079" t="s">
         <v>1034</v>
       </c>
       <c r="N1079" t="s">
+        <v>1815</v>
+      </c>
+      <c r="P1079" t="s">
         <v>1816</v>
-      </c>
-      <c r="P1079" t="s">
-        <v>1817</v>
       </c>
       <c r="Q1079" t="s">
         <v>17</v>
@@ -61429,16 +61684,16 @@
         <v>1235</v>
       </c>
       <c r="L1080" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="M1080" t="s">
         <v>1034</v>
       </c>
       <c r="N1080" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="P1080" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="Q1080" t="s">
         <v>19</v>
@@ -61467,16 +61722,16 @@
         <v>1236</v>
       </c>
       <c r="L1081" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="M1081" t="s">
         <v>1034</v>
       </c>
       <c r="N1081" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="P1081" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="Q1081" t="s">
         <v>20</v>
@@ -61505,16 +61760,16 @@
         <v>1237</v>
       </c>
       <c r="L1082" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="M1082" t="s">
         <v>1034</v>
       </c>
       <c r="N1082" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="P1082" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="Q1082" t="s">
         <v>20</v>
@@ -61543,16 +61798,16 @@
         <v>1238</v>
       </c>
       <c r="L1083" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="M1083" t="s">
         <v>1034</v>
       </c>
       <c r="N1083" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="P1083" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="Q1083" t="s">
         <v>16</v>
@@ -61581,16 +61836,16 @@
         <v>1239</v>
       </c>
       <c r="L1084" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="M1084" t="s">
         <v>123</v>
       </c>
       <c r="N1084" t="s">
+        <v>1824</v>
+      </c>
+      <c r="P1084" t="s">
         <v>1825</v>
-      </c>
-      <c r="P1084" t="s">
-        <v>1826</v>
       </c>
       <c r="Q1084" t="s">
         <v>20</v>
@@ -61619,16 +61874,16 @@
         <v>1240</v>
       </c>
       <c r="L1085" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="M1085" t="s">
         <v>123</v>
       </c>
       <c r="N1085" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1085" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="Q1085" t="s">
         <v>20</v>
@@ -61657,16 +61912,16 @@
         <v>1241</v>
       </c>
       <c r="L1086" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="M1086" t="s">
         <v>123</v>
       </c>
       <c r="N1086" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1086" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="Q1086" t="s">
         <v>19</v>
@@ -61695,16 +61950,16 @@
         <v>1242</v>
       </c>
       <c r="L1087" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="M1087" t="s">
         <v>123</v>
       </c>
       <c r="N1087" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1087" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="Q1087" t="s">
         <v>17</v>
@@ -61733,16 +61988,16 @@
         <v>1243</v>
       </c>
       <c r="L1088" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="M1088" t="s">
         <v>123</v>
       </c>
       <c r="N1088" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1088" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="Q1088" t="s">
         <v>20</v>
@@ -61771,16 +62026,16 @@
         <v>1244</v>
       </c>
       <c r="L1089" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="M1089" t="s">
         <v>123</v>
       </c>
       <c r="N1089" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1089" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="Q1089" t="s">
         <v>19</v>
@@ -61809,16 +62064,16 @@
         <v>1245</v>
       </c>
       <c r="L1090" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="M1090" t="s">
         <v>123</v>
       </c>
       <c r="N1090" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1090" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="Q1090" t="s">
         <v>18</v>
@@ -61847,16 +62102,16 @@
         <v>1246</v>
       </c>
       <c r="L1091" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="M1091" t="s">
         <v>123</v>
       </c>
       <c r="N1091" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1091" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="Q1091" t="s">
         <v>17</v>
@@ -61885,16 +62140,16 @@
         <v>1247</v>
       </c>
       <c r="L1092" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="M1092" t="s">
         <v>123</v>
       </c>
       <c r="N1092" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1092" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="Q1092" t="s">
         <v>17</v>
@@ -61923,16 +62178,16 @@
         <v>1248</v>
       </c>
       <c r="L1093" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="M1093" t="s">
         <v>123</v>
       </c>
       <c r="N1093" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1093" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="Q1093" t="s">
         <v>17</v>
@@ -61961,16 +62216,16 @@
         <v>1249</v>
       </c>
       <c r="L1094" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="M1094" t="s">
         <v>123</v>
       </c>
       <c r="N1094" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1094" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="Q1094" t="s">
         <v>17</v>
@@ -61999,16 +62254,16 @@
         <v>1250</v>
       </c>
       <c r="L1095" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="M1095" t="s">
         <v>123</v>
       </c>
       <c r="N1095" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1095" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="Q1095" t="s">
         <v>17</v>
@@ -62037,16 +62292,16 @@
         <v>1251</v>
       </c>
       <c r="L1096" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="M1096" t="s">
         <v>123</v>
       </c>
       <c r="N1096" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="P1096" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="Q1096" t="s">
         <v>20</v>
@@ -62075,16 +62330,16 @@
         <v>1252</v>
       </c>
       <c r="L1097" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="M1097" t="s">
         <v>62</v>
       </c>
       <c r="N1097" t="s">
+        <v>1845</v>
+      </c>
+      <c r="P1097" t="s">
         <v>1846</v>
-      </c>
-      <c r="P1097" t="s">
-        <v>1847</v>
       </c>
       <c r="Q1097" t="s">
         <v>18</v>
@@ -62119,10 +62374,10 @@
         <v>62</v>
       </c>
       <c r="N1098" t="s">
+        <v>1847</v>
+      </c>
+      <c r="P1098" t="s">
         <v>1848</v>
-      </c>
-      <c r="P1098" t="s">
-        <v>1849</v>
       </c>
       <c r="Q1098" t="s">
         <v>17</v>
@@ -62151,16 +62406,16 @@
         <v>1254</v>
       </c>
       <c r="L1099" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="M1099" t="s">
         <v>62</v>
       </c>
       <c r="N1099" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1099" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="Q1099" t="s">
         <v>17</v>
@@ -62189,16 +62444,16 @@
         <v>1255</v>
       </c>
       <c r="L1100" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="M1100" t="s">
         <v>62</v>
       </c>
       <c r="N1100" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1100" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="Q1100" t="s">
         <v>17</v>
@@ -62227,16 +62482,16 @@
         <v>1256</v>
       </c>
       <c r="L1101" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="M1101" t="s">
         <v>62</v>
       </c>
       <c r="N1101" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1101" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="Q1101" t="s">
         <v>19</v>
@@ -62265,16 +62520,16 @@
         <v>1257</v>
       </c>
       <c r="L1102" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="M1102" t="s">
         <v>62</v>
       </c>
       <c r="N1102" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1102" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="Q1102" t="s">
         <v>19</v>
@@ -62309,10 +62564,10 @@
         <v>62</v>
       </c>
       <c r="N1103" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1103" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="Q1103" t="s">
         <v>20</v>
@@ -62347,10 +62602,10 @@
         <v>62</v>
       </c>
       <c r="N1104" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1104" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="Q1104" t="s">
         <v>16</v>
@@ -62379,16 +62634,16 @@
         <v>1260</v>
       </c>
       <c r="L1105" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="M1105" t="s">
         <v>62</v>
       </c>
       <c r="N1105" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1105" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="Q1105" t="s">
         <v>20</v>
@@ -62417,16 +62672,16 @@
         <v>1261</v>
       </c>
       <c r="L1106" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="M1106" t="s">
         <v>62</v>
       </c>
       <c r="N1106" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1106" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="Q1106" t="s">
         <v>19</v>
@@ -62455,16 +62710,16 @@
         <v>1262</v>
       </c>
       <c r="L1107" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="M1107" t="s">
         <v>62</v>
       </c>
       <c r="N1107" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1107" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="Q1107" t="s">
         <v>17</v>
@@ -62493,16 +62748,16 @@
         <v>1263</v>
       </c>
       <c r="L1108" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="M1108" t="s">
         <v>62</v>
       </c>
       <c r="N1108" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1108" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="Q1108" t="s">
         <v>19</v>
@@ -62531,16 +62786,16 @@
         <v>1264</v>
       </c>
       <c r="L1109" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="M1109" t="s">
         <v>62</v>
       </c>
       <c r="N1109" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1109" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="Q1109" t="s">
         <v>20</v>
@@ -62569,16 +62824,16 @@
         <v>1265</v>
       </c>
       <c r="L1110" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="M1110" t="s">
         <v>62</v>
       </c>
       <c r="N1110" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="P1110" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="Q1110" t="s">
         <v>17</v>
@@ -62607,16 +62862,16 @@
         <v>1266</v>
       </c>
       <c r="L1111" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="M1111" t="s">
         <v>62</v>
       </c>
       <c r="N1111" t="s">
+        <v>1867</v>
+      </c>
+      <c r="P1111" t="s">
         <v>1868</v>
-      </c>
-      <c r="P1111" t="s">
-        <v>1869</v>
       </c>
       <c r="Q1111" t="s">
         <v>20</v>
@@ -62645,16 +62900,16 @@
         <v>1267</v>
       </c>
       <c r="L1112" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="M1112" t="s">
         <v>62</v>
       </c>
       <c r="N1112" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="P1112" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="Q1112" t="s">
         <v>16</v>
@@ -62683,16 +62938,16 @@
         <v>1268</v>
       </c>
       <c r="L1113" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="M1113" t="s">
         <v>62</v>
       </c>
       <c r="N1113" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="P1113" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="Q1113" t="s">
         <v>17</v>
@@ -62721,16 +62976,16 @@
         <v>1269</v>
       </c>
       <c r="L1114" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="M1114" t="s">
         <v>62</v>
       </c>
       <c r="N1114" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="P1114" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="Q1114" t="s">
         <v>20</v>
@@ -62759,16 +63014,16 @@
         <v>1270</v>
       </c>
       <c r="L1115" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="M1115" t="s">
         <v>62</v>
       </c>
       <c r="N1115" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="P1115" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="Q1115" t="s">
         <v>18</v>
@@ -62797,16 +63052,16 @@
         <v>1271</v>
       </c>
       <c r="L1116" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="M1116" t="s">
         <v>62</v>
       </c>
       <c r="N1116" t="s">
+        <v>1878</v>
+      </c>
+      <c r="P1116" t="s">
         <v>1879</v>
-      </c>
-      <c r="P1116" t="s">
-        <v>1880</v>
       </c>
       <c r="Q1116" t="s">
         <v>18</v>
@@ -62835,16 +63090,16 @@
         <v>1272</v>
       </c>
       <c r="L1117" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="M1117" t="s">
         <v>62</v>
       </c>
       <c r="N1117" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="P1117" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="Q1117" t="s">
         <v>18</v>
@@ -62873,16 +63128,16 @@
         <v>1273</v>
       </c>
       <c r="L1118" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="M1118" t="s">
         <v>62</v>
       </c>
       <c r="N1118" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="P1118" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="Q1118" t="s">
         <v>18</v>
@@ -62911,16 +63166,16 @@
         <v>1274</v>
       </c>
       <c r="L1119" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="M1119" t="s">
         <v>62</v>
       </c>
       <c r="N1119" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="P1119" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="Q1119" t="s">
         <v>19</v>
@@ -62949,16 +63204,16 @@
         <v>1275</v>
       </c>
       <c r="L1120" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="M1120" t="s">
         <v>62</v>
       </c>
       <c r="N1120" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="P1120" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="Q1120" t="s">
         <v>16</v>
@@ -62987,16 +63242,16 @@
         <v>1276</v>
       </c>
       <c r="L1121" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="M1121" t="s">
         <v>62</v>
       </c>
       <c r="N1121" t="s">
+        <v>1887</v>
+      </c>
+      <c r="P1121" t="s">
         <v>1888</v>
-      </c>
-      <c r="P1121" t="s">
-        <v>1889</v>
       </c>
       <c r="Q1121" t="s">
         <v>19</v>
@@ -63025,16 +63280,16 @@
         <v>1277</v>
       </c>
       <c r="L1122" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="M1122" t="s">
         <v>62</v>
       </c>
       <c r="N1122" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="P1122" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="Q1122" t="s">
         <v>19</v>
@@ -63063,16 +63318,16 @@
         <v>1278</v>
       </c>
       <c r="L1123" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="M1123" t="s">
         <v>62</v>
       </c>
       <c r="N1123" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="P1123" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="Q1123" t="s">
         <v>20</v>
@@ -63101,16 +63356,16 @@
         <v>1279</v>
       </c>
       <c r="L1124" t="s">
+        <v>1892</v>
+      </c>
+      <c r="M1124" t="s">
         <v>1893</v>
       </c>
-      <c r="M1124" t="s">
+      <c r="N1124" t="s">
         <v>1894</v>
       </c>
-      <c r="N1124" t="s">
+      <c r="P1124" t="s">
         <v>1895</v>
-      </c>
-      <c r="P1124" t="s">
-        <v>1896</v>
       </c>
       <c r="Q1124" t="s">
         <v>17</v>
@@ -63139,16 +63394,16 @@
         <v>1280</v>
       </c>
       <c r="L1125" t="s">
+        <v>1892</v>
+      </c>
+      <c r="M1125" t="s">
         <v>1893</v>
       </c>
-      <c r="M1125" t="s">
-        <v>1894</v>
-      </c>
       <c r="N1125" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1125" t="s">
         <v>1897</v>
-      </c>
-      <c r="P1125" t="s">
-        <v>1898</v>
       </c>
       <c r="Q1125" t="s">
         <v>17</v>
@@ -63177,16 +63432,16 @@
         <v>1281</v>
       </c>
       <c r="L1126" t="s">
+        <v>1898</v>
+      </c>
+      <c r="M1126" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1126" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1126" t="s">
         <v>1899</v>
-      </c>
-      <c r="M1126" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1126" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1126" t="s">
-        <v>1900</v>
       </c>
       <c r="Q1126" t="s">
         <v>19</v>
@@ -63215,16 +63470,16 @@
         <v>1282</v>
       </c>
       <c r="L1127" t="s">
+        <v>1900</v>
+      </c>
+      <c r="M1127" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1127" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1127" t="s">
         <v>1901</v>
-      </c>
-      <c r="M1127" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1127" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1127" t="s">
-        <v>1902</v>
       </c>
       <c r="Q1127" t="s">
         <v>17</v>
@@ -63253,16 +63508,16 @@
         <v>1283</v>
       </c>
       <c r="L1128" t="s">
+        <v>1902</v>
+      </c>
+      <c r="M1128" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1128" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1128" t="s">
         <v>1903</v>
-      </c>
-      <c r="M1128" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1128" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1128" t="s">
-        <v>1904</v>
       </c>
       <c r="Q1128" t="s">
         <v>20</v>
@@ -63291,16 +63546,16 @@
         <v>1284</v>
       </c>
       <c r="L1129" t="s">
+        <v>1904</v>
+      </c>
+      <c r="M1129" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1129" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1129" t="s">
         <v>1905</v>
-      </c>
-      <c r="M1129" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1129" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1129" t="s">
-        <v>1906</v>
       </c>
       <c r="Q1129" t="s">
         <v>17</v>
@@ -63329,16 +63584,16 @@
         <v>1285</v>
       </c>
       <c r="L1130" t="s">
+        <v>1906</v>
+      </c>
+      <c r="M1130" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1130" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1130" t="s">
         <v>1907</v>
-      </c>
-      <c r="M1130" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1130" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1130" t="s">
-        <v>1908</v>
       </c>
       <c r="Q1130" t="s">
         <v>17</v>
@@ -63367,16 +63622,16 @@
         <v>1286</v>
       </c>
       <c r="L1131" t="s">
+        <v>1908</v>
+      </c>
+      <c r="M1131" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1131" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1131" t="s">
         <v>1909</v>
-      </c>
-      <c r="M1131" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1131" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1131" t="s">
-        <v>1910</v>
       </c>
       <c r="Q1131" t="s">
         <v>16</v>
@@ -63405,16 +63660,16 @@
         <v>1287</v>
       </c>
       <c r="L1132" t="s">
+        <v>1910</v>
+      </c>
+      <c r="M1132" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1132" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1132" t="s">
         <v>1911</v>
-      </c>
-      <c r="M1132" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1132" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1132" t="s">
-        <v>1912</v>
       </c>
       <c r="Q1132" t="s">
         <v>17</v>
@@ -63443,16 +63698,16 @@
         <v>1288</v>
       </c>
       <c r="L1133" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="M1133" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="N1133" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="P1133" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="Q1133" t="s">
         <v>17</v>
@@ -63481,16 +63736,16 @@
         <v>1289</v>
       </c>
       <c r="L1134" t="s">
+        <v>1913</v>
+      </c>
+      <c r="M1134" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1134" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1134" t="s">
         <v>1914</v>
-      </c>
-      <c r="M1134" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1134" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1134" t="s">
-        <v>1915</v>
       </c>
       <c r="Q1134" t="s">
         <v>19</v>
@@ -63519,16 +63774,16 @@
         <v>1290</v>
       </c>
       <c r="L1135" t="s">
+        <v>1915</v>
+      </c>
+      <c r="M1135" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1135" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1135" t="s">
         <v>1916</v>
-      </c>
-      <c r="M1135" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1135" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1135" t="s">
-        <v>1917</v>
       </c>
       <c r="Q1135" t="s">
         <v>19</v>
@@ -63557,16 +63812,16 @@
         <v>1291</v>
       </c>
       <c r="L1136" t="s">
+        <v>1917</v>
+      </c>
+      <c r="M1136" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1136" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1136" t="s">
         <v>1918</v>
-      </c>
-      <c r="M1136" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1136" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1136" t="s">
-        <v>1919</v>
       </c>
       <c r="Q1136" t="s">
         <v>17</v>
@@ -63595,16 +63850,16 @@
         <v>1292</v>
       </c>
       <c r="L1137" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="M1137" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="N1137" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="P1137" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="Q1137" t="s">
         <v>20</v>
@@ -63633,16 +63888,16 @@
         <v>1293</v>
       </c>
       <c r="L1138" t="s">
+        <v>1920</v>
+      </c>
+      <c r="M1138" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1138" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1138" t="s">
         <v>1921</v>
-      </c>
-      <c r="M1138" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1138" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1138" t="s">
-        <v>1922</v>
       </c>
       <c r="Q1138" t="s">
         <v>16</v>
@@ -63671,16 +63926,16 @@
         <v>1294</v>
       </c>
       <c r="L1139" t="s">
+        <v>1922</v>
+      </c>
+      <c r="M1139" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1139" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1139" t="s">
         <v>1923</v>
-      </c>
-      <c r="M1139" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1139" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1139" t="s">
-        <v>1924</v>
       </c>
       <c r="Q1139" t="s">
         <v>17</v>
@@ -63709,16 +63964,16 @@
         <v>1295</v>
       </c>
       <c r="L1140" t="s">
+        <v>1924</v>
+      </c>
+      <c r="M1140" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1140" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1140" t="s">
         <v>1925</v>
-      </c>
-      <c r="M1140" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1140" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1140" t="s">
-        <v>1926</v>
       </c>
       <c r="Q1140" t="s">
         <v>17</v>
@@ -63747,16 +64002,16 @@
         <v>1296</v>
       </c>
       <c r="L1141" t="s">
+        <v>1926</v>
+      </c>
+      <c r="M1141" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1141" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1141" t="s">
         <v>1927</v>
-      </c>
-      <c r="M1141" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1141" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1141" t="s">
-        <v>1928</v>
       </c>
       <c r="Q1141" t="s">
         <v>17</v>
@@ -63785,16 +64040,16 @@
         <v>1297</v>
       </c>
       <c r="L1142" t="s">
+        <v>1928</v>
+      </c>
+      <c r="M1142" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1142" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1142" t="s">
         <v>1929</v>
-      </c>
-      <c r="M1142" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1142" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1142" t="s">
-        <v>1930</v>
       </c>
       <c r="Q1142" t="s">
         <v>17</v>
@@ -63823,16 +64078,16 @@
         <v>1298</v>
       </c>
       <c r="L1143" t="s">
+        <v>1930</v>
+      </c>
+      <c r="M1143" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1143" t="s">
+        <v>1896</v>
+      </c>
+      <c r="P1143" t="s">
         <v>1931</v>
-      </c>
-      <c r="M1143" t="s">
-        <v>1894</v>
-      </c>
-      <c r="N1143" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P1143" t="s">
-        <v>1932</v>
       </c>
       <c r="Q1143" t="s">
         <v>17</v>
@@ -63861,19 +64116,34 @@
         <v>1299</v>
       </c>
       <c r="L1144" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="M1144" t="s">
         <v>123</v>
       </c>
       <c r="N1144" t="s">
+        <v>1933</v>
+      </c>
+      <c r="P1144" t="s">
         <v>1934</v>
-      </c>
-      <c r="P1144" t="s">
-        <v>1935</v>
       </c>
       <c r="Q1144" t="s">
         <v>17</v>
+      </c>
+      <c r="R1144" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1144" t="s">
+        <v>1669</v>
+      </c>
+      <c r="T1144" t="s">
+        <v>165</v>
+      </c>
+      <c r="U1144" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1144" t="s">
+        <v>455</v>
       </c>
       <c r="W1144" t="s">
         <v>32</v>
@@ -63884,19 +64154,34 @@
         <v>1300</v>
       </c>
       <c r="L1145" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="M1145" t="s">
         <v>123</v>
       </c>
       <c r="N1145" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="P1145" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="Q1145" t="s">
         <v>17</v>
+      </c>
+      <c r="R1145" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1145" t="s">
+        <v>907</v>
+      </c>
+      <c r="T1145" t="s">
+        <v>165</v>
+      </c>
+      <c r="U1145" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1145" t="s">
+        <v>102</v>
       </c>
       <c r="W1145" t="s">
         <v>32</v>
@@ -63907,19 +64192,34 @@
         <v>1301</v>
       </c>
       <c r="L1146" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="M1146" t="s">
         <v>123</v>
       </c>
       <c r="N1146" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="P1146" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="Q1146" t="s">
         <v>20</v>
+      </c>
+      <c r="R1146" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1146" t="s">
+        <v>102</v>
+      </c>
+      <c r="T1146" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1146" t="s">
+        <v>211</v>
+      </c>
+      <c r="V1146" t="s">
+        <v>542</v>
       </c>
       <c r="W1146" t="s">
         <v>32</v>
@@ -63930,73 +64230,1733 @@
         <v>1302</v>
       </c>
       <c r="L1147" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="M1147" t="s">
         <v>123</v>
       </c>
       <c r="N1147" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="P1147" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="Q1147" t="s">
         <v>20</v>
       </c>
+      <c r="R1147" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1147" t="s">
+        <v>160</v>
+      </c>
+      <c r="T1147" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1147" t="s">
+        <v>165</v>
+      </c>
+      <c r="V1147" t="s">
+        <v>613</v>
+      </c>
       <c r="W1147" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="1148" spans="1:23" x14ac:dyDescent="0.2">
       <c r="L1148" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="M1148" t="s">
         <v>62</v>
       </c>
       <c r="N1148" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="P1148" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="Q1148" t="s">
         <v>16</v>
       </c>
+      <c r="R1148" t="s">
+        <v>542</v>
+      </c>
+      <c r="S1148" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1148" t="s">
+        <v>102</v>
+      </c>
+      <c r="U1148" t="s">
+        <v>141</v>
+      </c>
+      <c r="V1148" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="1149" spans="1:23" x14ac:dyDescent="0.2">
       <c r="L1149" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="M1149" t="s">
         <v>62</v>
       </c>
       <c r="N1149" t="s">
+        <v>1941</v>
+      </c>
+      <c r="P1149" t="s">
         <v>1942</v>
-      </c>
-      <c r="P1149" t="s">
-        <v>1943</v>
       </c>
       <c r="Q1149" t="s">
         <v>17</v>
       </c>
+      <c r="R1149" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1149" t="s">
+        <v>1635</v>
+      </c>
+      <c r="T1149" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1149" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1149" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="1150" spans="1:23" x14ac:dyDescent="0.2">
       <c r="L1150" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="M1150" t="s">
         <v>62</v>
       </c>
       <c r="N1150" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="P1150" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="Q1150" t="s">
         <v>18</v>
+      </c>
+      <c r="R1150" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1150" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1150" t="s">
+        <v>635</v>
+      </c>
+      <c r="U1150" t="s">
+        <v>101</v>
+      </c>
+      <c r="V1150" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="L1151" t="s">
+        <v>1945</v>
+      </c>
+      <c r="M1151" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1151" t="s">
+        <v>1941</v>
+      </c>
+      <c r="P1151" t="s">
+        <v>1946</v>
+      </c>
+      <c r="Q1151" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1151" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1151" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1151" t="s">
+        <v>613</v>
+      </c>
+      <c r="U1151" t="s">
+        <v>142</v>
+      </c>
+      <c r="V1151" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="L1152" t="s">
+        <v>1948</v>
+      </c>
+      <c r="M1152" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1152" t="s">
+        <v>1941</v>
+      </c>
+      <c r="P1152" t="s">
+        <v>1947</v>
+      </c>
+      <c r="Q1152" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1152" t="s">
+        <v>709</v>
+      </c>
+      <c r="S1152" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1152" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1152" t="s">
+        <v>211</v>
+      </c>
+      <c r="V1152" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="1153" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1153" t="s">
+        <v>1951</v>
+      </c>
+      <c r="M1153" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1153" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1153" t="s">
+        <v>1949</v>
+      </c>
+      <c r="Q1153" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1153" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1153" t="s">
+        <v>106</v>
+      </c>
+      <c r="T1153" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1153" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1153" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="1154" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1154" t="s">
+        <v>1951</v>
+      </c>
+      <c r="M1154" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1154" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1154" t="s">
+        <v>1952</v>
+      </c>
+      <c r="Q1154" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1154" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1154" t="s">
+        <v>102</v>
+      </c>
+      <c r="T1154" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1154" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1154" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="1155" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1155" t="s">
+        <v>1951</v>
+      </c>
+      <c r="M1155" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1155" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1155" t="s">
+        <v>1953</v>
+      </c>
+      <c r="Q1155" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1155" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1155" t="s">
+        <v>1635</v>
+      </c>
+      <c r="T1155" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1155" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1155" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1156" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1156" t="s">
+        <v>1955</v>
+      </c>
+      <c r="M1156" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1156" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1156" t="s">
+        <v>1954</v>
+      </c>
+      <c r="Q1156" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1156" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1156" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1156" t="s">
+        <v>228</v>
+      </c>
+      <c r="U1156" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1156" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1157" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1157" t="s">
+        <v>1955</v>
+      </c>
+      <c r="M1157" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1157" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1157" t="s">
+        <v>1956</v>
+      </c>
+      <c r="Q1157" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1157" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1157" t="s">
+        <v>1669</v>
+      </c>
+      <c r="T1157" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1157" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1157" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="1158" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1158" t="s">
+        <v>1958</v>
+      </c>
+      <c r="M1158" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1158" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1158" t="s">
+        <v>1957</v>
+      </c>
+      <c r="Q1158" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1158" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1158" t="s">
+        <v>1353</v>
+      </c>
+      <c r="T1158" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1158" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1158" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="1159" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1159" t="s">
+        <v>1958</v>
+      </c>
+      <c r="M1159" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1159" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1159" t="s">
+        <v>1959</v>
+      </c>
+      <c r="Q1159" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1159" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1159" t="s">
+        <v>530</v>
+      </c>
+      <c r="T1159" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1159" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1159" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="1160" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1160" t="s">
+        <v>1965</v>
+      </c>
+      <c r="M1160" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1160" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1160" t="s">
+        <v>1960</v>
+      </c>
+      <c r="Q1160" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1160" t="s">
+        <v>99</v>
+      </c>
+      <c r="S1160" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1160" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1160" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1160" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="1161" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1161" t="s">
+        <v>1966</v>
+      </c>
+      <c r="M1161" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1161" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1161" t="s">
+        <v>1961</v>
+      </c>
+      <c r="Q1161" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1161" t="s">
+        <v>222</v>
+      </c>
+      <c r="S1161" t="s">
+        <v>106</v>
+      </c>
+      <c r="T1161" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1161" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1161" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="1162" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1162" t="s">
+        <v>1966</v>
+      </c>
+      <c r="M1162" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1162" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1162" t="s">
+        <v>1962</v>
+      </c>
+      <c r="Q1162" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1162" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1162" t="s">
+        <v>106</v>
+      </c>
+      <c r="T1162" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1162" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1162" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="1163" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1163" t="s">
+        <v>1966</v>
+      </c>
+      <c r="M1163" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1163" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1163" t="s">
+        <v>1963</v>
+      </c>
+      <c r="Q1163" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1163" t="s">
+        <v>165</v>
+      </c>
+      <c r="S1163" t="s">
+        <v>1669</v>
+      </c>
+      <c r="T1163" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1163" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1163" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1164" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1164" t="s">
+        <v>1967</v>
+      </c>
+      <c r="M1164" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1164" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1164" t="s">
+        <v>1964</v>
+      </c>
+      <c r="Q1164" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1164" t="s">
+        <v>95</v>
+      </c>
+      <c r="S1164" t="s">
+        <v>305</v>
+      </c>
+      <c r="T1164" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1164" t="s">
+        <v>635</v>
+      </c>
+      <c r="V1164" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1165" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1165" t="s">
+        <v>1969</v>
+      </c>
+      <c r="M1165" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1165" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1165" t="s">
+        <v>1968</v>
+      </c>
+      <c r="Q1165" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1165" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1165" t="s">
+        <v>1977</v>
+      </c>
+      <c r="T1165" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1165" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1165" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1166" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1166" t="s">
+        <v>1969</v>
+      </c>
+      <c r="M1166" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1166" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1166" t="s">
+        <v>1970</v>
+      </c>
+      <c r="Q1166" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1166" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1166" t="s">
+        <v>152</v>
+      </c>
+      <c r="T1166" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1166" t="s">
+        <v>185</v>
+      </c>
+      <c r="V1166" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1167" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1167" t="s">
+        <v>1969</v>
+      </c>
+      <c r="M1167" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1167" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1167" t="s">
+        <v>1971</v>
+      </c>
+      <c r="Q1167" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1167" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1167" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1167" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1167" t="s">
+        <v>211</v>
+      </c>
+      <c r="V1167" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="1168" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1168" t="s">
+        <v>1973</v>
+      </c>
+      <c r="M1168" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1168" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1168" t="s">
+        <v>1972</v>
+      </c>
+      <c r="Q1168" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1168" t="s">
+        <v>366</v>
+      </c>
+      <c r="S1168" t="s">
+        <v>160</v>
+      </c>
+      <c r="T1168" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1168" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1168" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="1169" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1169" t="s">
+        <v>1973</v>
+      </c>
+      <c r="M1169" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1169" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1169" t="s">
+        <v>1974</v>
+      </c>
+      <c r="Q1169" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1169" t="s">
+        <v>207</v>
+      </c>
+      <c r="S1169" t="s">
+        <v>1353</v>
+      </c>
+      <c r="T1169" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1169" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1169" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="1170" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1170" t="s">
+        <v>1976</v>
+      </c>
+      <c r="M1170" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1170" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P1170" t="s">
+        <v>1975</v>
+      </c>
+      <c r="Q1170" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1170" t="s">
+        <v>185</v>
+      </c>
+      <c r="S1170" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1170" t="s">
+        <v>542</v>
+      </c>
+      <c r="U1170" t="s">
+        <v>350</v>
+      </c>
+      <c r="V1170" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="1171" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1171" t="s">
+        <v>1979</v>
+      </c>
+      <c r="M1171" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1171" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1171" t="s">
+        <v>1978</v>
+      </c>
+      <c r="Q1171" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1171" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1171" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1171" t="s">
+        <v>986</v>
+      </c>
+      <c r="U1171" t="s">
+        <v>877</v>
+      </c>
+      <c r="V1171" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1172" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1172" t="s">
+        <v>1981</v>
+      </c>
+      <c r="M1172" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1172" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1172" t="s">
+        <v>1980</v>
+      </c>
+      <c r="Q1172" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1172" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1172" t="s">
+        <v>159</v>
+      </c>
+      <c r="T1172" t="s">
+        <v>552</v>
+      </c>
+      <c r="U1172" t="s">
+        <v>613</v>
+      </c>
+      <c r="V1172" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="1173" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1173" t="s">
+        <v>1985</v>
+      </c>
+      <c r="M1173" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1173" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1173" t="s">
+        <v>1982</v>
+      </c>
+      <c r="Q1173" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1173" t="s">
+        <v>240</v>
+      </c>
+      <c r="S1173" t="s">
+        <v>159</v>
+      </c>
+      <c r="T1173" t="s">
+        <v>101</v>
+      </c>
+      <c r="U1173" t="s">
+        <v>542</v>
+      </c>
+      <c r="V1173" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="1174" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1174" t="s">
+        <v>1984</v>
+      </c>
+      <c r="M1174" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1174" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1174" t="s">
+        <v>1983</v>
+      </c>
+      <c r="Q1174" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1174" t="s">
+        <v>228</v>
+      </c>
+      <c r="S1174" t="s">
+        <v>165</v>
+      </c>
+      <c r="T1174" t="s">
+        <v>986</v>
+      </c>
+      <c r="U1174" t="s">
+        <v>530</v>
+      </c>
+      <c r="V1174" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="1175" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1175" t="s">
+        <v>1988</v>
+      </c>
+      <c r="M1175" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1175" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1175" t="s">
+        <v>1987</v>
+      </c>
+      <c r="Q1175" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1175" t="s">
+        <v>165</v>
+      </c>
+      <c r="S1175" t="s">
+        <v>452</v>
+      </c>
+      <c r="T1175" t="s">
+        <v>165</v>
+      </c>
+      <c r="U1175" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1175" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1176" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1176" t="s">
+        <v>1988</v>
+      </c>
+      <c r="M1176" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1176" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1176" t="s">
+        <v>1989</v>
+      </c>
+      <c r="Q1176" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1176" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1176" t="s">
+        <v>240</v>
+      </c>
+      <c r="T1176" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1176" t="s">
+        <v>202</v>
+      </c>
+      <c r="V1176" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="1177" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1177" t="s">
+        <v>1991</v>
+      </c>
+      <c r="M1177" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1177" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1177" t="s">
+        <v>1990</v>
+      </c>
+      <c r="Q1177" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1177" t="s">
+        <v>111</v>
+      </c>
+      <c r="S1177" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1177" t="s">
+        <v>141</v>
+      </c>
+      <c r="U1177" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1177" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1178" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1178" t="s">
+        <v>1028</v>
+      </c>
+      <c r="M1178" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1178" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1178" t="s">
+        <v>1992</v>
+      </c>
+      <c r="Q1178" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1178" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1178" t="s">
+        <v>844</v>
+      </c>
+      <c r="T1178" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1178" t="s">
+        <v>141</v>
+      </c>
+      <c r="V1178" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="1179" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1179" t="s">
+        <v>1869</v>
+      </c>
+      <c r="M1179" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1179" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1179" t="s">
+        <v>1993</v>
+      </c>
+      <c r="Q1179" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1179" t="s">
+        <v>228</v>
+      </c>
+      <c r="S1179" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1179" t="s">
+        <v>65</v>
+      </c>
+      <c r="U1179" t="s">
+        <v>530</v>
+      </c>
+      <c r="V1179" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="1180" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1180" t="s">
+        <v>1869</v>
+      </c>
+      <c r="M1180" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1180" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1180" t="s">
+        <v>1994</v>
+      </c>
+      <c r="Q1180" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1180" t="s">
+        <v>825</v>
+      </c>
+      <c r="S1180" t="s">
+        <v>202</v>
+      </c>
+      <c r="T1180" t="s">
+        <v>542</v>
+      </c>
+      <c r="U1180" t="s">
+        <v>552</v>
+      </c>
+      <c r="V1180" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1181" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1181" t="s">
+        <v>1869</v>
+      </c>
+      <c r="M1181" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1181" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1181" t="s">
+        <v>1995</v>
+      </c>
+      <c r="Q1181" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1181" t="s">
+        <v>825</v>
+      </c>
+      <c r="S1181" t="s">
+        <v>165</v>
+      </c>
+      <c r="T1181" t="s">
+        <v>141</v>
+      </c>
+      <c r="U1181" t="s">
+        <v>613</v>
+      </c>
+      <c r="V1181" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1182" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1182" t="s">
+        <v>1869</v>
+      </c>
+      <c r="M1182" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1182" t="s">
+        <v>1986</v>
+      </c>
+      <c r="P1182" t="s">
+        <v>1996</v>
+      </c>
+      <c r="Q1182" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1182" t="s">
+        <v>884</v>
+      </c>
+      <c r="S1182" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1182" t="s">
+        <v>240</v>
+      </c>
+      <c r="U1182" t="s">
+        <v>575</v>
+      </c>
+      <c r="V1182" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="1183" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1183" t="s">
+        <v>1998</v>
+      </c>
+      <c r="M1183" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1183" t="s">
+        <v>1999</v>
+      </c>
+      <c r="P1183" t="s">
+        <v>1997</v>
+      </c>
+      <c r="Q1183" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1183" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1183" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1183" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1183" t="s">
+        <v>907</v>
+      </c>
+      <c r="V1183" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1184" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1184" t="s">
+        <v>1998</v>
+      </c>
+      <c r="M1184" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1184" t="s">
+        <v>1999</v>
+      </c>
+      <c r="P1184" t="s">
+        <v>2000</v>
+      </c>
+      <c r="Q1184" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1184" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1184" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1184" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1184" t="s">
+        <v>552</v>
+      </c>
+      <c r="V1184" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="1185" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1185" t="s">
+        <v>1998</v>
+      </c>
+      <c r="M1185" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1185" t="s">
+        <v>1999</v>
+      </c>
+      <c r="P1185" t="s">
+        <v>2001</v>
+      </c>
+      <c r="Q1185" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1185" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1185" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1185" t="s">
+        <v>542</v>
+      </c>
+      <c r="U1185" t="s">
+        <v>552</v>
+      </c>
+      <c r="V1185" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1186" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1186" t="s">
+        <v>2004</v>
+      </c>
+      <c r="M1186" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1186" t="s">
+        <v>1999</v>
+      </c>
+      <c r="P1186" t="s">
+        <v>2002</v>
+      </c>
+      <c r="Q1186" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1186" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1186" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1186" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1186" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1186" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1187" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1187" t="s">
+        <v>2004</v>
+      </c>
+      <c r="M1187" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1187" t="s">
+        <v>1999</v>
+      </c>
+      <c r="P1187" t="s">
+        <v>2003</v>
+      </c>
+      <c r="Q1187" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1187" t="s">
+        <v>613</v>
+      </c>
+      <c r="S1187" t="s">
+        <v>189</v>
+      </c>
+      <c r="T1187" t="s">
+        <v>185</v>
+      </c>
+      <c r="U1187" t="s">
+        <v>654</v>
+      </c>
+      <c r="V1187" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="1188" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1188" t="s">
+        <v>2006</v>
+      </c>
+      <c r="M1188" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1188" t="s">
+        <v>1999</v>
+      </c>
+      <c r="P1188" t="s">
+        <v>2005</v>
+      </c>
+      <c r="Q1188" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1188" t="s">
+        <v>111</v>
+      </c>
+      <c r="S1188" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1188" t="s">
+        <v>588</v>
+      </c>
+      <c r="U1188" t="s">
+        <v>236</v>
+      </c>
+      <c r="V1188" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1189" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1189" t="s">
+        <v>2008</v>
+      </c>
+      <c r="M1189" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1189" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1189" t="s">
+        <v>2007</v>
+      </c>
+      <c r="Q1189" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1189" t="s">
+        <v>185</v>
+      </c>
+      <c r="S1189" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1189" t="s">
+        <v>613</v>
+      </c>
+      <c r="U1189" t="s">
+        <v>240</v>
+      </c>
+      <c r="V1189" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1190" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1190" t="s">
+        <v>2011</v>
+      </c>
+      <c r="M1190" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1190" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1190" t="s">
+        <v>2010</v>
+      </c>
+      <c r="Q1190" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1190" t="s">
+        <v>189</v>
+      </c>
+      <c r="S1190" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1190" t="s">
+        <v>530</v>
+      </c>
+      <c r="U1190" t="s">
+        <v>240</v>
+      </c>
+      <c r="V1190" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1191" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1191" t="s">
+        <v>2013</v>
+      </c>
+      <c r="M1191" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1191" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1191" t="s">
+        <v>2012</v>
+      </c>
+      <c r="Q1191" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1191" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1191" t="s">
+        <v>530</v>
+      </c>
+      <c r="T1191" t="s">
+        <v>142</v>
+      </c>
+      <c r="U1191" t="s">
+        <v>211</v>
+      </c>
+      <c r="V1191" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1192" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1192" t="s">
+        <v>2015</v>
+      </c>
+      <c r="M1192" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1192" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1192" t="s">
+        <v>2014</v>
+      </c>
+      <c r="Q1192" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1192" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1192" t="s">
+        <v>402</v>
+      </c>
+      <c r="T1192" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1192" t="s">
+        <v>159</v>
+      </c>
+      <c r="V1192" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="1193" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1193" t="s">
+        <v>2017</v>
+      </c>
+      <c r="M1193" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1193" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1193" t="s">
+        <v>2016</v>
+      </c>
+      <c r="Q1193" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1193" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1193" t="s">
+        <v>530</v>
+      </c>
+      <c r="T1193" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1193" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1193" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1194" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1194" t="s">
+        <v>2019</v>
+      </c>
+      <c r="M1194" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1194" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1194" t="s">
+        <v>2018</v>
+      </c>
+      <c r="Q1194" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1194" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1194" t="s">
+        <v>1669</v>
+      </c>
+      <c r="T1194" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1194" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1194" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1195" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1195" t="s">
+        <v>2021</v>
+      </c>
+      <c r="M1195" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1195" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1195" t="s">
+        <v>2020</v>
+      </c>
+      <c r="Q1195" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1195" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1195" t="s">
+        <v>2022</v>
+      </c>
+      <c r="T1195" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1195" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1195" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="1196" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1196" t="s">
+        <v>2021</v>
+      </c>
+      <c r="M1196" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1196" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1196" t="s">
+        <v>2023</v>
+      </c>
+      <c r="Q1196" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1196" t="s">
+        <v>85</v>
+      </c>
+      <c r="S1196" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1196" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1196" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1196" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="1197" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1197" t="s">
+        <v>2025</v>
+      </c>
+      <c r="M1197" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1197" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1197" t="s">
+        <v>2024</v>
+      </c>
+      <c r="Q1197" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1197" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1197" t="s">
+        <v>907</v>
+      </c>
+      <c r="T1197" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1197" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1197" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="1198" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1198" t="s">
+        <v>2027</v>
+      </c>
+      <c r="M1198" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1198" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1198" t="s">
+        <v>2026</v>
+      </c>
+      <c r="Q1198" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1198" t="s">
+        <v>240</v>
+      </c>
+      <c r="S1198" t="s">
+        <v>613</v>
+      </c>
+      <c r="T1198" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1198" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1198" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="1199" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1199" t="s">
+        <v>2029</v>
+      </c>
+      <c r="M1199" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1199" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1199" t="s">
+        <v>2028</v>
+      </c>
+      <c r="Q1199" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1199" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1199" t="s">
+        <v>1353</v>
+      </c>
+      <c r="T1199" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1199" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1199" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1200" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1200" t="s">
+        <v>2031</v>
+      </c>
+      <c r="M1200" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1200" t="s">
+        <v>2009</v>
+      </c>
+      <c r="P1200" t="s">
+        <v>2030</v>
+      </c>
+      <c r="Q1200" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1200" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1200" t="s">
+        <v>1669</v>
+      </c>
+      <c r="T1200" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1200" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1200" t="s">
+        <v>588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TD ML = 1260
</commit_message>
<xml_diff>
--- a/webserver/model_data/TrainingData_ml.xlsx
+++ b/webserver/model_data/TrainingData_ml.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13157" uniqueCount="2032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13630" uniqueCount="2152">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -6123,6 +6123,366 @@
   </si>
   <si>
     <t>Patrick Fame</t>
+  </si>
+  <si>
+    <t>mal an die hier meckern kleiner Tipp von mir macht euern Kopf zu oder hört es auch doch einfach nicht an Hauptsache mal dumm daher gelabbert</t>
+  </si>
+  <si>
+    <t>Herbert Uttrich</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2czABFw6RnE</t>
+  </si>
+  <si>
+    <t>ihr Wichtigtuer</t>
+  </si>
+  <si>
+    <t>Ist zwar nicht meine Musikrichtung, finde den Song aber trotzdem geil!!!</t>
+  </si>
+  <si>
+    <t>Reverend Music</t>
+  </si>
+  <si>
+    <t>Live ist sie immer besser als ihre Videos</t>
+  </si>
+  <si>
+    <t>Wudruff Wildcard</t>
+  </si>
+  <si>
+    <t>Das ist es, was jeden richtig guten Künstler auszeichnet</t>
+  </si>
+  <si>
+    <t>Helene Fischer ist das beste!</t>
+  </si>
+  <si>
+    <t>Marilene Wolf</t>
+  </si>
+  <si>
+    <t>Ich mag sehr gerne!</t>
+  </si>
+  <si>
+    <t>Schön Muzik!</t>
+  </si>
+  <si>
+    <t>So eine schöne stimme</t>
+  </si>
+  <si>
+    <t>JeskesBegurem</t>
+  </si>
+  <si>
+    <t>geiles Video und geile frau</t>
+  </si>
+  <si>
+    <t>Florian Florian</t>
+  </si>
+  <si>
+    <t>ich liebe dich und du hast das Musik sehr gut gemacht</t>
+  </si>
+  <si>
+    <t>das Lied, okay- ich verstehe, warum es ein Hit war.</t>
+  </si>
+  <si>
+    <t>Scrubbini</t>
+  </si>
+  <si>
+    <t>Aber das Video sieht so nach 1-€-Produktion aus..echt nicht gut.</t>
+  </si>
+  <si>
+    <t>Coole Clips, Coole Musik!</t>
+  </si>
+  <si>
+    <t>Ich liebe das Lied.</t>
+  </si>
+  <si>
+    <t>christina tas</t>
+  </si>
+  <si>
+    <t>Ich glaube, dass das bestes Deutsches Lied ist</t>
+  </si>
+  <si>
+    <t>Alte Erinnerungen kommen hoch</t>
+  </si>
+  <si>
+    <t>lyre elain</t>
+  </si>
+  <si>
+    <t>Ich mag immernoch Helene Fischer hab sie auch in real life gesehen</t>
+  </si>
+  <si>
+    <t>geiles lied es ist auf platz 1 meiner top 10 lieblings lieder</t>
+  </si>
+  <si>
+    <t>WolfyNova</t>
+  </si>
+  <si>
+    <t>Sven Brochhagen</t>
+  </si>
+  <si>
+    <t>Helene du bist schön und hast eine tolle Stimme und du hast es ein großes talent</t>
+  </si>
+  <si>
+    <t>Werner Mettlach</t>
+  </si>
+  <si>
+    <t>Helene Fischer bei dir ist einfach alles perfekt</t>
+  </si>
+  <si>
+    <t>Lelolinchen</t>
+  </si>
+  <si>
+    <t>sie kann sehr gut singen das ist klar</t>
+  </si>
+  <si>
+    <t>Steven Sell</t>
+  </si>
+  <si>
+    <t>Die Frau ist wunderbar und macht deutsche Musik attraktive !!!!!!!</t>
+  </si>
+  <si>
+    <t>sifis sidis</t>
+  </si>
+  <si>
+    <t>Hellenen du bist meine Traumfrau</t>
+  </si>
+  <si>
+    <t>Philipp Meyer</t>
+  </si>
+  <si>
+    <t>Sie kann echt gut singen</t>
+  </si>
+  <si>
+    <t>Cemyoo</t>
+  </si>
+  <si>
+    <t>Gänsehaut pur</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Gmo4WVqaU1g</t>
+  </si>
+  <si>
+    <t>Lisa Ru</t>
+  </si>
+  <si>
+    <t>Wundervolle Stimme ihr beiden</t>
+  </si>
+  <si>
+    <t>Jason Enrico Altendorf</t>
+  </si>
+  <si>
+    <t>Mir kommen immer die Tränen</t>
+  </si>
+  <si>
+    <t>Kurz Stier</t>
+  </si>
+  <si>
+    <t>Eines der schönsten Lieder überhaupt</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Xytt5PNC0Wo</t>
+  </si>
+  <si>
+    <t>Mike Hanson</t>
+  </si>
+  <si>
+    <t>Richtiger Ohrwurm-Song bei mir momentan</t>
+  </si>
+  <si>
+    <t>Hendrik B</t>
+  </si>
+  <si>
+    <t>Oh wie ich dieses Video liebe</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8BX70FI7hfI</t>
+  </si>
+  <si>
+    <t>ApertureIntern023</t>
+  </si>
+  <si>
+    <t>Diese beiden Jungs. Welche große Kunst die beiden da machen.</t>
+  </si>
+  <si>
+    <t>Super Lied!</t>
+  </si>
+  <si>
+    <t>Jorg Meguin</t>
+  </si>
+  <si>
+    <t>Immer noch schön, ich weine</t>
+  </si>
+  <si>
+    <t>floomdesk</t>
+  </si>
+  <si>
+    <t>Yeah Baby!</t>
+  </si>
+  <si>
+    <t>Norbert Ketterl</t>
+  </si>
+  <si>
+    <t>Große Liebe!</t>
+  </si>
+  <si>
+    <t>Herr Engels</t>
+  </si>
+  <si>
+    <t>Dirk Amos</t>
+  </si>
+  <si>
+    <t>Cool</t>
+  </si>
+  <si>
+    <t>verfluchte scheisse... der song ist 20 jahre alt...</t>
+  </si>
+  <si>
+    <t>Agares Blight</t>
+  </si>
+  <si>
+    <t>Meine Jugend zieht an meinem inneren Auge vorbei wenn ich das höre .... Gänsehaut !!!</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vZPMJCmBfi4</t>
+  </si>
+  <si>
+    <t>The1Rausch</t>
+  </si>
+  <si>
+    <t>2018 und immer noch mega.</t>
+  </si>
+  <si>
+    <t>Zeitlos!</t>
+  </si>
+  <si>
+    <t>It sounds like Cherry</t>
+  </si>
+  <si>
+    <t>Hamburger schule!!!!</t>
+  </si>
+  <si>
+    <t>toll</t>
+  </si>
+  <si>
+    <t>thomas böge</t>
+  </si>
+  <si>
+    <t>uoeigrono</t>
+  </si>
+  <si>
+    <t>der track ist geil so wie er ist</t>
+  </si>
+  <si>
+    <t>yomanpolanski</t>
+  </si>
+  <si>
+    <t>sehr geil!!!</t>
+  </si>
+  <si>
+    <t>devilshaircut</t>
+  </si>
+  <si>
+    <t>allezhenry</t>
+  </si>
+  <si>
+    <t>ich reg mich blos immerwieder auf wenn ich anfange die dämlichen comments zu lesen</t>
+  </si>
+  <si>
+    <t>ICH LIEBE ES!!!!!!</t>
+  </si>
+  <si>
+    <t>Daggi1234</t>
+  </si>
+  <si>
+    <t>Wer keine Ahnung hat, der sollte den Sabbel halten ;)</t>
+  </si>
+  <si>
+    <t>renethann</t>
+  </si>
+  <si>
+    <t>Recht hast du, tagtraeumer1990!</t>
+  </si>
+  <si>
+    <t>TheCLion</t>
+  </si>
+  <si>
+    <t>Ich freue mich schon auf die Konzerte 2008!!!!!!</t>
+  </si>
+  <si>
+    <t>chechersf</t>
+  </si>
+  <si>
+    <t>eines der schönsten Lieder von Tocotronic!!!</t>
+  </si>
+  <si>
+    <t>das lied is echt ziemlich bis sehr geil</t>
+  </si>
+  <si>
+    <t>Pupa Strav</t>
+  </si>
+  <si>
+    <t>Kann allen nur zustimmen!!Eines der Besten Lider von den Tocos!!</t>
+  </si>
+  <si>
+    <t>frvfl76</t>
+  </si>
+  <si>
+    <t>zeitloses meisterwerk!</t>
+  </si>
+  <si>
+    <t>schwarzemilch</t>
+  </si>
+  <si>
+    <t>also des video hält sich in grenzen, aber.. der text is gut un so</t>
+  </si>
+  <si>
+    <t>Essipnetzak</t>
+  </si>
+  <si>
+    <t>ich finds ziemlich geil....</t>
+  </si>
+  <si>
+    <t>das beste lied was sie je rausgebracht haben!!!</t>
+  </si>
+  <si>
+    <t>reeloop1</t>
+  </si>
+  <si>
+    <t>Feinstes tocotronic!</t>
+  </si>
+  <si>
+    <t>Martin Nö</t>
+  </si>
+  <si>
+    <t>Vergesst alles was ihr kennt und dann wisst ihr endlich das was ihr braucht.</t>
+  </si>
+  <si>
+    <t>pop gegen deutschland</t>
+  </si>
+  <si>
+    <t>ekili11</t>
+  </si>
+  <si>
+    <t>Diese Möchtegernaufrichtigkeit von dir ist ja wohl echt lächerlich!!!</t>
+  </si>
+  <si>
+    <t>Was hat denn das mit nem Nazi zu tun, wenn man sagt, dass das richtig gute deutsche Musik ist!</t>
+  </si>
+  <si>
+    <t>tagtraeumer1990</t>
+  </si>
+  <si>
+    <t>Ehrlich wenn man nicht mal mehr ne Band loben kann, nur weil die aus Deutschland ist, dann ist dir auch nicht mehr zu helfen!</t>
+  </si>
+  <si>
+    <t>du glaubst bestimmt von dir selbst, daß du ein total lockerer und vor allem toleranter typ bist.</t>
+  </si>
+  <si>
+    <t>cycling4ever</t>
+  </si>
+  <si>
+    <t>Typen von Deiner Sorte gibt es zu Hunderten -auch im linken Lager.</t>
+  </si>
+  <si>
+    <t>Ich weiß, das hört Ihr nicht so gerne...</t>
   </si>
 </sst>
 </file>
@@ -6482,12 +6842,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1200"/>
+  <dimension ref="A1:W1266"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1189" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1242" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="M1197" sqref="M1197:N1200"/>
+      <selection pane="bottomLeft" activeCell="M1240" sqref="M1240:N1266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -65959,6 +66319,1557 @@
         <v>588</v>
       </c>
     </row>
+    <row r="1201" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1201" t="s">
+        <v>2033</v>
+      </c>
+      <c r="M1201" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1201" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1201" t="s">
+        <v>2032</v>
+      </c>
+      <c r="Q1201" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1201" t="s">
+        <v>530</v>
+      </c>
+      <c r="S1201" t="s">
+        <v>165</v>
+      </c>
+      <c r="T1201" t="s">
+        <v>128</v>
+      </c>
+      <c r="U1201" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1201" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1202" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1202" t="s">
+        <v>2033</v>
+      </c>
+      <c r="M1202" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1202" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1202" t="s">
+        <v>2035</v>
+      </c>
+      <c r="Q1202" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1202" t="s">
+        <v>142</v>
+      </c>
+      <c r="S1202" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1202" t="s">
+        <v>305</v>
+      </c>
+      <c r="U1202" t="s">
+        <v>1645</v>
+      </c>
+      <c r="V1202" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="1203" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1203" t="s">
+        <v>2037</v>
+      </c>
+      <c r="M1203" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1203" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1203" t="s">
+        <v>2036</v>
+      </c>
+      <c r="Q1203" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1203" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1203" t="s">
+        <v>106</v>
+      </c>
+      <c r="T1203" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1203" t="s">
+        <v>189</v>
+      </c>
+      <c r="V1203" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="1204" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1204" t="s">
+        <v>2039</v>
+      </c>
+      <c r="M1204" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1204" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1204" t="s">
+        <v>2038</v>
+      </c>
+      <c r="Q1204" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1204" t="s">
+        <v>223</v>
+      </c>
+      <c r="S1204" t="s">
+        <v>1645</v>
+      </c>
+      <c r="T1204" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1204" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1204" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="1205" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1205" t="s">
+        <v>2039</v>
+      </c>
+      <c r="M1205" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1205" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1205" t="s">
+        <v>2040</v>
+      </c>
+      <c r="Q1205" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1205" t="s">
+        <v>530</v>
+      </c>
+      <c r="S1205" t="s">
+        <v>102</v>
+      </c>
+      <c r="T1205" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1205" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1205" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1206" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1206" t="s">
+        <v>2042</v>
+      </c>
+      <c r="M1206" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1206" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1206" t="s">
+        <v>2041</v>
+      </c>
+      <c r="Q1206" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1206" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1206" t="s">
+        <v>2022</v>
+      </c>
+      <c r="T1206" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1206" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1206" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="1207" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1207" t="s">
+        <v>2042</v>
+      </c>
+      <c r="M1207" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1207" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1207" t="s">
+        <v>2043</v>
+      </c>
+      <c r="Q1207" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1207" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1207" t="s">
+        <v>588</v>
+      </c>
+      <c r="T1207" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1207" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1207" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="1208" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1208" t="s">
+        <v>2042</v>
+      </c>
+      <c r="M1208" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1208" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1208" t="s">
+        <v>2044</v>
+      </c>
+      <c r="Q1208" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1208" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1208" t="s">
+        <v>1669</v>
+      </c>
+      <c r="T1208" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1208" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1208" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1209" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1209" t="s">
+        <v>2046</v>
+      </c>
+      <c r="M1209" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1209" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1209" t="s">
+        <v>2045</v>
+      </c>
+      <c r="Q1209" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1209" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1209" t="s">
+        <v>1669</v>
+      </c>
+      <c r="T1209" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1209" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1209" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1210" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1210" t="s">
+        <v>2048</v>
+      </c>
+      <c r="M1210" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1210" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1210" t="s">
+        <v>2047</v>
+      </c>
+      <c r="Q1210" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1210" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1210" t="s">
+        <v>1977</v>
+      </c>
+      <c r="T1210" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1210" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1210" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="1211" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="M1211" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1211" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1211" t="s">
+        <v>2049</v>
+      </c>
+      <c r="Q1211" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1211" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1211" t="s">
+        <v>1977</v>
+      </c>
+      <c r="T1211" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1211" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1211" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="1212" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1212" t="s">
+        <v>2051</v>
+      </c>
+      <c r="M1212" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1212" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1212" t="s">
+        <v>2050</v>
+      </c>
+      <c r="Q1212" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1212" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1212" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1212" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1212" t="s">
+        <v>189</v>
+      </c>
+      <c r="V1212" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="1213" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1213" t="s">
+        <v>2051</v>
+      </c>
+      <c r="M1213" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1213" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1213" t="s">
+        <v>2052</v>
+      </c>
+      <c r="Q1213" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1213" t="s">
+        <v>350</v>
+      </c>
+      <c r="S1213" t="s">
+        <v>165</v>
+      </c>
+      <c r="T1213" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1213" t="s">
+        <v>907</v>
+      </c>
+      <c r="V1213" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1214" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="M1214" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1214" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1214" t="s">
+        <v>2053</v>
+      </c>
+      <c r="Q1214" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1214" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1214" t="s">
+        <v>1669</v>
+      </c>
+      <c r="T1214" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1214" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1214" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="1215" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1215" t="s">
+        <v>2055</v>
+      </c>
+      <c r="M1215" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1215" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1215" t="s">
+        <v>2054</v>
+      </c>
+      <c r="Q1215" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1215" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1215" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1215" t="s">
+        <v>86</v>
+      </c>
+      <c r="U1215" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1215" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="1216" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1216" t="s">
+        <v>2055</v>
+      </c>
+      <c r="M1216" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1216" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1216" t="s">
+        <v>2056</v>
+      </c>
+      <c r="Q1216" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1216" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1216" t="s">
+        <v>366</v>
+      </c>
+      <c r="T1216" t="s">
+        <v>189</v>
+      </c>
+      <c r="U1216" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1216" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="1217" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1217" t="s">
+        <v>2058</v>
+      </c>
+      <c r="M1217" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1217" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1217" t="s">
+        <v>2057</v>
+      </c>
+      <c r="Q1217" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1217" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1217" t="s">
+        <v>160</v>
+      </c>
+      <c r="T1217" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1217" t="s">
+        <v>211</v>
+      </c>
+      <c r="V1217" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="1218" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1218" t="s">
+        <v>2061</v>
+      </c>
+      <c r="M1218" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1218" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1218" t="s">
+        <v>2059</v>
+      </c>
+      <c r="Q1218" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1218" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1218" t="s">
+        <v>102</v>
+      </c>
+      <c r="T1218" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1218" t="s">
+        <v>159</v>
+      </c>
+      <c r="V1218" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="1219" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1219" t="s">
+        <v>2062</v>
+      </c>
+      <c r="M1219" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1219" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1219" t="s">
+        <v>2060</v>
+      </c>
+      <c r="Q1219" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1219" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1219" t="s">
+        <v>2022</v>
+      </c>
+      <c r="T1219" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1219" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1219" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="1220" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1220" t="s">
+        <v>2064</v>
+      </c>
+      <c r="M1220" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1220" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1220" t="s">
+        <v>2063</v>
+      </c>
+      <c r="Q1220" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1220" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1220" t="s">
+        <v>1977</v>
+      </c>
+      <c r="T1220" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1220" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1220" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="1221" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1221" t="s">
+        <v>2066</v>
+      </c>
+      <c r="M1221" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1221" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1221" t="s">
+        <v>2065</v>
+      </c>
+      <c r="Q1221" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1221" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1221" t="s">
+        <v>1977</v>
+      </c>
+      <c r="T1221" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1221" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1221" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="1222" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1222" t="s">
+        <v>2068</v>
+      </c>
+      <c r="M1222" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1222" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1222" t="s">
+        <v>2067</v>
+      </c>
+      <c r="Q1222" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1222" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1222" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1222" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1222" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1222" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="1223" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1223" t="s">
+        <v>2070</v>
+      </c>
+      <c r="M1223" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1223" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1223" t="s">
+        <v>2069</v>
+      </c>
+      <c r="Q1223" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1223" t="s">
+        <v>305</v>
+      </c>
+      <c r="S1223" t="s">
+        <v>1645</v>
+      </c>
+      <c r="T1223" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1223" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1223" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1224" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1224" t="s">
+        <v>2072</v>
+      </c>
+      <c r="M1224" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1224" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1224" t="s">
+        <v>2071</v>
+      </c>
+      <c r="Q1224" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1224" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1224" t="s">
+        <v>635</v>
+      </c>
+      <c r="T1224" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1224" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1224" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="1225" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1225" t="s">
+        <v>2074</v>
+      </c>
+      <c r="M1225" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1225" t="s">
+        <v>2034</v>
+      </c>
+      <c r="P1225" t="s">
+        <v>2073</v>
+      </c>
+      <c r="Q1225" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1225" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1225" t="s">
+        <v>366</v>
+      </c>
+      <c r="T1225" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1225" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1225" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="1226" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1226" t="s">
+        <v>2077</v>
+      </c>
+      <c r="M1226" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1226" t="s">
+        <v>2076</v>
+      </c>
+      <c r="P1226" t="s">
+        <v>2075</v>
+      </c>
+      <c r="Q1226" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1226" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1226" t="s">
+        <v>1977</v>
+      </c>
+      <c r="T1226" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1226" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1226" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="1227" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1227" t="s">
+        <v>2079</v>
+      </c>
+      <c r="M1227" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1227" t="s">
+        <v>2076</v>
+      </c>
+      <c r="P1227" t="s">
+        <v>2078</v>
+      </c>
+      <c r="Q1227" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1227" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1227" t="s">
+        <v>2022</v>
+      </c>
+      <c r="T1227" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1227" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1227" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1228" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1228" t="s">
+        <v>2081</v>
+      </c>
+      <c r="M1228" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1228" t="s">
+        <v>2076</v>
+      </c>
+      <c r="P1228" t="s">
+        <v>2080</v>
+      </c>
+      <c r="Q1228" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1228" t="s">
+        <v>85</v>
+      </c>
+      <c r="S1228" t="s">
+        <v>369</v>
+      </c>
+      <c r="T1228" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1228" t="s">
+        <v>211</v>
+      </c>
+      <c r="V1228" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="1229" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1229" t="s">
+        <v>2084</v>
+      </c>
+      <c r="M1229" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1229" t="s">
+        <v>2083</v>
+      </c>
+      <c r="P1229" t="s">
+        <v>2082</v>
+      </c>
+      <c r="Q1229" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1229" t="s">
+        <v>222</v>
+      </c>
+      <c r="S1229" t="s">
+        <v>1977</v>
+      </c>
+      <c r="T1229" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1229" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1229" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="1230" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1230" t="s">
+        <v>2086</v>
+      </c>
+      <c r="M1230" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1230" t="s">
+        <v>2083</v>
+      </c>
+      <c r="P1230" t="s">
+        <v>2085</v>
+      </c>
+      <c r="Q1230" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1231" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1231" t="s">
+        <v>2089</v>
+      </c>
+      <c r="M1231" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1231" t="s">
+        <v>2088</v>
+      </c>
+      <c r="P1231" t="s">
+        <v>2087</v>
+      </c>
+      <c r="Q1231" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1232" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1232" t="s">
+        <v>2089</v>
+      </c>
+      <c r="M1232" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1232" t="s">
+        <v>2088</v>
+      </c>
+      <c r="P1232" t="s">
+        <v>2090</v>
+      </c>
+      <c r="Q1232" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1233" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1233" t="s">
+        <v>2092</v>
+      </c>
+      <c r="M1233" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1233" t="s">
+        <v>2088</v>
+      </c>
+      <c r="P1233" t="s">
+        <v>2091</v>
+      </c>
+      <c r="Q1233" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1234" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1234" t="s">
+        <v>2094</v>
+      </c>
+      <c r="M1234" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1234" t="s">
+        <v>2088</v>
+      </c>
+      <c r="P1234" t="s">
+        <v>2093</v>
+      </c>
+      <c r="Q1234" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1235" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1235" t="s">
+        <v>2096</v>
+      </c>
+      <c r="M1235" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1235" t="s">
+        <v>2088</v>
+      </c>
+      <c r="P1235" t="s">
+        <v>2095</v>
+      </c>
+      <c r="Q1235" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1236" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1236" t="s">
+        <v>2098</v>
+      </c>
+      <c r="M1236" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1236" t="s">
+        <v>2088</v>
+      </c>
+      <c r="P1236" t="s">
+        <v>2097</v>
+      </c>
+      <c r="Q1236" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1237" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1237" t="s">
+        <v>2099</v>
+      </c>
+      <c r="M1237" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1237" t="s">
+        <v>2088</v>
+      </c>
+      <c r="P1237" t="s">
+        <v>2100</v>
+      </c>
+      <c r="Q1237" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1238" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1238" t="s">
+        <v>2102</v>
+      </c>
+      <c r="M1238" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1238" t="s">
+        <v>2088</v>
+      </c>
+      <c r="P1238" t="s">
+        <v>2101</v>
+      </c>
+      <c r="Q1238" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1239" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1239" t="s">
+        <v>2105</v>
+      </c>
+      <c r="M1239" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1239" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1239" t="s">
+        <v>2103</v>
+      </c>
+      <c r="Q1239" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1240" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1240" t="s">
+        <v>2108</v>
+      </c>
+      <c r="M1240" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1240" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1240" t="s">
+        <v>2106</v>
+      </c>
+      <c r="Q1240" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1241" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1241" t="s">
+        <v>2108</v>
+      </c>
+      <c r="M1241" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1241" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1241" t="s">
+        <v>2107</v>
+      </c>
+      <c r="Q1241" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1242" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1242" t="s">
+        <v>2111</v>
+      </c>
+      <c r="M1242" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1242" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1242" t="s">
+        <v>2109</v>
+      </c>
+      <c r="Q1242" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1243" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1243" t="s">
+        <v>2112</v>
+      </c>
+      <c r="M1243" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1243" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1243" t="s">
+        <v>2110</v>
+      </c>
+      <c r="Q1243" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1244" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1244" t="s">
+        <v>2114</v>
+      </c>
+      <c r="M1244" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1244" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1244" t="s">
+        <v>2113</v>
+      </c>
+      <c r="Q1244" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1245" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1245" t="s">
+        <v>2116</v>
+      </c>
+      <c r="M1245" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1245" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1245" t="s">
+        <v>2115</v>
+      </c>
+      <c r="Q1245" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1246" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1246" t="s">
+        <v>2117</v>
+      </c>
+      <c r="M1246" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1246" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1246" t="s">
+        <v>2118</v>
+      </c>
+      <c r="Q1246" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1247" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1247" t="s">
+        <v>2120</v>
+      </c>
+      <c r="M1247" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1247" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1247" t="s">
+        <v>2119</v>
+      </c>
+      <c r="Q1247" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1248" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1248" t="s">
+        <v>2122</v>
+      </c>
+      <c r="M1248" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1248" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1248" t="s">
+        <v>2121</v>
+      </c>
+      <c r="Q1248" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1249" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1249" t="s">
+        <v>2124</v>
+      </c>
+      <c r="M1249" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1249" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1249" t="s">
+        <v>2123</v>
+      </c>
+      <c r="Q1249" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1250" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1250" t="s">
+        <v>2126</v>
+      </c>
+      <c r="M1250" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1250" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1250" t="s">
+        <v>2125</v>
+      </c>
+      <c r="Q1250" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1251" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1251" t="s">
+        <v>2120</v>
+      </c>
+      <c r="M1251" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1251" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1251" t="s">
+        <v>2127</v>
+      </c>
+      <c r="Q1251" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1252" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1252" t="s">
+        <v>2129</v>
+      </c>
+      <c r="M1252" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1252" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1252" t="s">
+        <v>2128</v>
+      </c>
+      <c r="Q1252" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1253" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1253" t="s">
+        <v>2131</v>
+      </c>
+      <c r="M1253" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1253" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1253" t="s">
+        <v>2130</v>
+      </c>
+      <c r="Q1253" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1254" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1254" t="s">
+        <v>2133</v>
+      </c>
+      <c r="M1254" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1254" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1254" t="s">
+        <v>2132</v>
+      </c>
+      <c r="Q1254" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1255" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1255" t="s">
+        <v>2135</v>
+      </c>
+      <c r="M1255" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1255" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1255" t="s">
+        <v>2134</v>
+      </c>
+      <c r="Q1255" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1256" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1256" t="s">
+        <v>2135</v>
+      </c>
+      <c r="M1256" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1256" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1256" t="s">
+        <v>2136</v>
+      </c>
+      <c r="Q1256" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1257" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1257" t="s">
+        <v>2138</v>
+      </c>
+      <c r="M1257" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1257" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1257" t="s">
+        <v>2137</v>
+      </c>
+      <c r="Q1257" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1258" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1258" t="s">
+        <v>2140</v>
+      </c>
+      <c r="M1258" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1258" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1258" t="s">
+        <v>2139</v>
+      </c>
+      <c r="Q1258" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1259" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1259" t="s">
+        <v>2140</v>
+      </c>
+      <c r="M1259" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1259" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1259" t="s">
+        <v>2141</v>
+      </c>
+      <c r="Q1259" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1260" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1260" t="s">
+        <v>2143</v>
+      </c>
+      <c r="M1260" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1260" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1260" t="s">
+        <v>2142</v>
+      </c>
+      <c r="Q1260" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1261" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1261" t="s">
+        <v>2146</v>
+      </c>
+      <c r="M1261" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1261" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1261" t="s">
+        <v>2144</v>
+      </c>
+      <c r="Q1261" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1262" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1262" t="s">
+        <v>2146</v>
+      </c>
+      <c r="M1262" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1262" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1262" t="s">
+        <v>2145</v>
+      </c>
+      <c r="Q1262" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1263" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1263" t="s">
+        <v>2146</v>
+      </c>
+      <c r="M1263" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1263" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1263" t="s">
+        <v>2147</v>
+      </c>
+      <c r="Q1263" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1264" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1264" t="s">
+        <v>2149</v>
+      </c>
+      <c r="M1264" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1264" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1264" t="s">
+        <v>2148</v>
+      </c>
+      <c r="Q1264" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1265" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1265" t="s">
+        <v>2149</v>
+      </c>
+      <c r="M1265" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1265" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1265" t="s">
+        <v>2150</v>
+      </c>
+      <c r="Q1265" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1266" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1266" t="s">
+        <v>2149</v>
+      </c>
+      <c r="M1266" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1266" t="s">
+        <v>2104</v>
+      </c>
+      <c r="P1266" t="s">
+        <v>2151</v>
+      </c>
+      <c r="Q1266" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
TD ML = 1330
</commit_message>
<xml_diff>
--- a/webserver/model_data/TrainingData_ml.xlsx
+++ b/webserver/model_data/TrainingData_ml.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13630" uniqueCount="2152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13955" uniqueCount="2251">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -6483,13 +6483,333 @@
   </si>
   <si>
     <t>Ich weiß, das hört Ihr nicht so gerne...</t>
+  </si>
+  <si>
+    <t>Der spricht mir aus dem Herzen.</t>
+  </si>
+  <si>
+    <t>Applaus fuer den Titel des Beitrags</t>
+  </si>
+  <si>
+    <t>Lukas Werth</t>
+  </si>
+  <si>
+    <t>https://www.faz.net/aktuell/wissen/coronavirus-uebertraeger-die-rache-des-schuppentiers-16622676.html?utm_source=pocket-newtab</t>
+  </si>
+  <si>
+    <t>Und ich will hier keinesfals weiteren Vorurteilen gegenueber der chinesischen Gesellschaft den Mund reden.</t>
+  </si>
+  <si>
+    <t>Doch glaube oder, besser, hoffe ich, dass es diese Rache der Tiere wirklich gibt.</t>
+  </si>
+  <si>
+    <t>Schweine aus der industrialisierten Tierfolter verstopfen unsere Arterien - recht so.</t>
+  </si>
+  <si>
+    <t>Ich hoffe nur, dass Trump Junior, wenn er das naechste Mal auf Grosswildjagd geht, von einem Tier ueber den Haufen gerannt wird.</t>
+  </si>
+  <si>
+    <t>Die Reaktion der Partei war klar</t>
+  </si>
+  <si>
+    <t>CaoKy</t>
+  </si>
+  <si>
+    <t>Die Wahrheit war Kommunisten schon immer egal wenn sie nicht in ihr Programm gepasst hat.</t>
+  </si>
+  <si>
+    <t>Hysterie und Verfolgungswahn wollen wir doch einmal beiseite lassen und festhalten was wir wissen</t>
+  </si>
+  <si>
+    <t>Oliver Gerd Wormer</t>
+  </si>
+  <si>
+    <t>Man kann nur hoffen, dass die jetzige Virus-Katastrophe zu einem radikalen Umdenken der chinesischen Führung ausreicht</t>
+  </si>
+  <si>
+    <t>Peter Krcmar</t>
+  </si>
+  <si>
+    <t>Hoffentlich ändert sich jetzt daran etwas in China.</t>
+  </si>
+  <si>
+    <t>Nina Neumann</t>
+  </si>
+  <si>
+    <t>Das ist irgendwie die Strafe für katastrophalen Umgang mit Tieren und unermessliches Tierleid auf dem Tiermarkt in Wuhan sowie die rücksichtslose Ausbeutung und Ausrottung vieler Tierarten.</t>
+  </si>
+  <si>
+    <t>Gratulation an die Briten, die es im Gegensatz zu uns Deutschen geschafft haben, sich von Frau Merkel zu emanzipieren!</t>
+  </si>
+  <si>
+    <t>Rainer Kyon</t>
+  </si>
+  <si>
+    <t>https://www.faz.net/aktuell/brexit/brexit-vollzogen-johnson-und-die-suche-nach-den-muskeln-16611660.html</t>
+  </si>
+  <si>
+    <t>Beneidenswert frei</t>
+  </si>
+  <si>
+    <t>Da schauen einige durchaus nachdenklich drein...</t>
+  </si>
+  <si>
+    <t>Andreas Martin</t>
+  </si>
+  <si>
+    <t>Nun endlich kann die EU ihren Weg fortsetzen</t>
+  </si>
+  <si>
+    <t>Rainhart Raack</t>
+  </si>
+  <si>
+    <t>Natürlich werden sich die Verhandlungen mit dem neuen Drittstaat, dem Bittsteller Groß Britannien, noch hinziehen.</t>
+  </si>
+  <si>
+    <t>Doch GB hat seine EU-Rechte verloren.</t>
+  </si>
+  <si>
+    <t>Und die EU ist endlich von der ständigen Mäkelei, Quertreiberei und dem Pochen auf Sonderrechte , kurz, vom Klotz am Bein befreit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einfach Danke für die letzten Jahre. </t>
+  </si>
+  <si>
+    <t>FeineSahneFischFilet</t>
+  </si>
+  <si>
+    <t>https://twitter.com/feinesahne/status/1214858502230958080</t>
+  </si>
+  <si>
+    <t>Danke an alle Menschen vor, auf und neben der Bühne.</t>
+  </si>
+  <si>
+    <t>Danke für euer Aktiv sein, für eure Einmischung und die Unterstützung, die wir von euch bekommen haben!</t>
+  </si>
+  <si>
+    <t>Demmin Nazifrei</t>
+  </si>
+  <si>
+    <t>Danke für die Hoffnung, dass wir doch noch nicht komplett im Arsch sind.</t>
+  </si>
+  <si>
+    <t>matzetremonia</t>
+  </si>
+  <si>
+    <t>Danke auch euch und bis demnächst</t>
+  </si>
+  <si>
+    <t>Ron</t>
+  </si>
+  <si>
+    <t>Ich denke, ihr seid toll!</t>
+  </si>
+  <si>
+    <t>Skadi Winter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bin zwar 67, aber was soll's? </t>
+  </si>
+  <si>
+    <t>Es gibt aber auch andere Beispiele in der Gründerszene.</t>
+  </si>
+  <si>
+    <t>https://www.gruenderszene.de/karriere/jobprotokoll-gruender-gehalt?utm_source=pocket-newtab</t>
+  </si>
+  <si>
+    <t>Die ganze Geschichte klingt nach einem Schmarrn.</t>
+  </si>
+  <si>
+    <t>kofiallstar</t>
+  </si>
+  <si>
+    <t>HHeinz</t>
+  </si>
+  <si>
+    <t>Bonuspunkt für den Inhaber hier, denn er bezahlt anscheinend ordentlich und lässt seine Mitarbeiter(innen) zusätzlich am Erfolg teilhaben.</t>
+  </si>
+  <si>
+    <t>Das hier beschriebene Unternehmen ist aber zu anonym um daraus einen Mehrwert zu ziehen, sprich die Geschichte könnte auch frei erfunden sein.</t>
+  </si>
+  <si>
+    <t>Naja, ich sag es mal so</t>
+  </si>
+  <si>
+    <t>Etherion</t>
+  </si>
+  <si>
+    <t>Wenn das Unternehmen Gewinne abwirft und die Mitarbeiter tatsächlich mit Ihrem Arbeitsleben und Gehalt zufrieden sind, warum dann nicht?</t>
+  </si>
+  <si>
+    <t>Ich kenne die Branche des Herren nicht, also kann ich auch nicht beurteilen, ob er überhaupt investieren muss</t>
+  </si>
+  <si>
+    <t>Und dieses Gehalt ist nichtmal extrem.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Darf hier eigentlich jeder </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hanswurst</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Gründer rumprahlen?</t>
+    </r>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Wenn ihr das verdienen wollt, dann spart Geld an, entwickelt eine gute ertragreiche Idee und setzt sie um.</t>
+  </si>
+  <si>
+    <t>Jörg Becker</t>
+  </si>
+  <si>
+    <t>Dann könnt ihr auch so viel Geld verdienen.</t>
+  </si>
+  <si>
+    <t>Bitte um Antwort Dr. Schlauberger.</t>
+  </si>
+  <si>
+    <t>fpstefan</t>
+  </si>
+  <si>
+    <t>https://www.heise.de/forum/heise-online/News-Kommentare/Cryptoleaks-CIA-und-BND-steckten-jahrzehntelang-hinter-Verschluesselungsfirma/Re-Wer-sich-ausspionieren-laesst-ist-selber-Schuld-kwt/posting-36113334/show/</t>
+  </si>
+  <si>
+    <t>Wer sich ausspionieren lässt, ist selber schuld</t>
+  </si>
+  <si>
+    <t>memex666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aber das ist doch seit 25 Jahren bekannt </t>
+  </si>
+  <si>
+    <t>Ulriko</t>
+  </si>
+  <si>
+    <t>Und dass jetzt etliche Medien das wieder bringen, weil ein ZDF-Reporter letztes Jahr "neue Beweise" zugespielt bekam - na gut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit Vollbitverschlüsselung wäre das nicht passiert </t>
+  </si>
+  <si>
+    <t>Cabriofahrer</t>
+  </si>
+  <si>
+    <t>Warum heult alles rum wegen Crypto AG</t>
+  </si>
+  <si>
+    <t>LaMünz</t>
+  </si>
+  <si>
+    <t>Müller Maguhn der linke Klops, der sich so gerne vor den Kameras der Medien damit brüstet ein so toller Typ zu sein, petzt doch alle Nase lang an der Verfassungsschutz und BND.</t>
+  </si>
+  <si>
+    <t>Der Typ ist einfach nur gierig nach Anerkennung.</t>
+  </si>
+  <si>
+    <t>Also schaut lieber auf Euren eigenen Misthaufen anstatt alten Hut zu lesen.</t>
+  </si>
+  <si>
+    <t>Dass der CCC überhaupt noch an diesem Verräter festhält ist echt ein Unikum.</t>
+  </si>
+  <si>
+    <t>Und jeder weiss doch, dass der Vatikan in Wirklichkeit Prostitution mit den politischen Weltmächten betreibt</t>
+  </si>
+  <si>
+    <t>öfit</t>
+  </si>
+  <si>
+    <t>Es gibt hier eine Reihe von interessanten Beiträgen zur Historie diese historischen Events</t>
+  </si>
+  <si>
+    <t>Föhn</t>
+  </si>
+  <si>
+    <t>Ist das blindes Fishing nach Empörung? gehört das wirklich hier her?</t>
+  </si>
+  <si>
+    <t>manchmal sind die Artikel zu Flach</t>
+  </si>
+  <si>
+    <t>aber woran liegt es, dass Heise Artikel immer häufiger nicht aus technisch wissenschaftlicher Sicht kommentiert werden, sondern als Politikbashing misbraucht werden?</t>
+  </si>
+  <si>
+    <t>Kann ich empfehlen.</t>
+  </si>
+  <si>
+    <t>Hursch</t>
+  </si>
+  <si>
+    <t>sagte schon Brecht, das trifft hier in abgewandelter Form auch zu.</t>
+  </si>
+  <si>
+    <t>ganzfaul</t>
+  </si>
+  <si>
+    <t>Aber noch cleverer, denn man kann von den Gewinnen der Firma auch noch das eigentliche Geschäft finanzieren.</t>
+  </si>
+  <si>
+    <t>Ehrlich, was braucht man noch Verschwörungstheorien bei den Machenschaften der Akteure in unserer "Wertegemeinschaft".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok, und wann kommen die technischen Details? </t>
+  </si>
+  <si>
+    <t>Dass das so ist, ist ja jetzt nicht sonderlich überraschend</t>
+  </si>
+  <si>
+    <t>Die NZZ bringt es wieder einmal auf den Punkt!</t>
+  </si>
+  <si>
+    <t>Regi87</t>
+  </si>
+  <si>
+    <t>Von wegen "investigative Recherche" des ZDF .... LOL ..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die TS hat einen schön weichgewaschenen Artikel dazu gebracht... </t>
+  </si>
+  <si>
+    <t>in welchem sie es sorgfältig vermeidet, das Wort "Hintertür" auch nur in den Mund zu nehmen.</t>
+  </si>
+  <si>
+    <t>Auch den Namen "Siemens" vermeidet die Tagesschau akribisch.</t>
+  </si>
+  <si>
+    <t>sou</t>
+  </si>
+  <si>
+    <t>Sowas nennt man auch Framing, die TS ist da ganz groß drin.</t>
+  </si>
+  <si>
+    <t>Weichspüler für's Dummvieh.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6501,6 +6821,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -6842,12 +7170,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1266"/>
+  <dimension ref="A1:W1331"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1242" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1329" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="M1240" sqref="M1240:N1266"/>
+      <selection pane="bottomLeft" activeCell="P1331" sqref="P1331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -67870,7 +68198,1118 @@
         <v>18</v>
       </c>
     </row>
+    <row r="1267" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1267" t="s">
+        <v>2154</v>
+      </c>
+      <c r="M1267" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1267" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1267" t="s">
+        <v>2153</v>
+      </c>
+      <c r="Q1267" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1268" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1268" t="s">
+        <v>2154</v>
+      </c>
+      <c r="M1268" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1268" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1268" t="s">
+        <v>2152</v>
+      </c>
+      <c r="Q1268" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1269" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1269" t="s">
+        <v>2154</v>
+      </c>
+      <c r="M1269" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1269" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1269" t="s">
+        <v>2156</v>
+      </c>
+      <c r="Q1269" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1270" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1270" t="s">
+        <v>2154</v>
+      </c>
+      <c r="M1270" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1270" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1270" t="s">
+        <v>2157</v>
+      </c>
+      <c r="Q1270" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1271" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1271" t="s">
+        <v>2154</v>
+      </c>
+      <c r="M1271" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1271" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1271" t="s">
+        <v>2158</v>
+      </c>
+      <c r="Q1271" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1272" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1272" t="s">
+        <v>2154</v>
+      </c>
+      <c r="M1272" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1272" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1272" t="s">
+        <v>2159</v>
+      </c>
+      <c r="Q1272" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1273" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1273" t="s">
+        <v>2161</v>
+      </c>
+      <c r="M1273" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1273" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1273" t="s">
+        <v>2160</v>
+      </c>
+      <c r="Q1273" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1274" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1274" t="s">
+        <v>2161</v>
+      </c>
+      <c r="M1274" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1274" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1274" t="s">
+        <v>2162</v>
+      </c>
+      <c r="Q1274" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1275" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1275" t="s">
+        <v>2164</v>
+      </c>
+      <c r="M1275" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1275" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1275" t="s">
+        <v>2163</v>
+      </c>
+      <c r="Q1275" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1276" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1276" t="s">
+        <v>2166</v>
+      </c>
+      <c r="M1276" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1276" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1276" t="s">
+        <v>2165</v>
+      </c>
+      <c r="Q1276" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1277" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1277" t="s">
+        <v>2168</v>
+      </c>
+      <c r="M1277" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1277" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1277" t="s">
+        <v>2167</v>
+      </c>
+      <c r="Q1277" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1278" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1278" t="s">
+        <v>2168</v>
+      </c>
+      <c r="M1278" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1278" t="s">
+        <v>2155</v>
+      </c>
+      <c r="P1278" t="s">
+        <v>2169</v>
+      </c>
+      <c r="Q1278" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1279" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1279" t="s">
+        <v>2171</v>
+      </c>
+      <c r="M1279" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1279" t="s">
+        <v>2172</v>
+      </c>
+      <c r="P1279" t="s">
+        <v>2170</v>
+      </c>
+      <c r="Q1279" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1280" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1280" t="s">
+        <v>2171</v>
+      </c>
+      <c r="M1280" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1280" t="s">
+        <v>2172</v>
+      </c>
+      <c r="P1280" t="s">
+        <v>2173</v>
+      </c>
+      <c r="Q1280" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1281" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1281" t="s">
+        <v>2175</v>
+      </c>
+      <c r="M1281" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1281" t="s">
+        <v>2172</v>
+      </c>
+      <c r="P1281" t="s">
+        <v>2174</v>
+      </c>
+      <c r="Q1281" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1282" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1282" t="s">
+        <v>2177</v>
+      </c>
+      <c r="M1282" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1282" t="s">
+        <v>2172</v>
+      </c>
+      <c r="P1282" t="s">
+        <v>2176</v>
+      </c>
+      <c r="Q1282" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1283" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1283" t="s">
+        <v>2177</v>
+      </c>
+      <c r="M1283" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1283" t="s">
+        <v>2172</v>
+      </c>
+      <c r="P1283" t="s">
+        <v>2178</v>
+      </c>
+      <c r="Q1283" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1284" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1284" t="s">
+        <v>2177</v>
+      </c>
+      <c r="M1284" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1284" t="s">
+        <v>2172</v>
+      </c>
+      <c r="P1284" t="s">
+        <v>2179</v>
+      </c>
+      <c r="Q1284" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1285" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1285" t="s">
+        <v>2177</v>
+      </c>
+      <c r="M1285" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1285" t="s">
+        <v>2172</v>
+      </c>
+      <c r="P1285" t="s">
+        <v>2180</v>
+      </c>
+      <c r="Q1285" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1286" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1286" t="s">
+        <v>2182</v>
+      </c>
+      <c r="M1286" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1286" t="s">
+        <v>2183</v>
+      </c>
+      <c r="P1286" t="s">
+        <v>2181</v>
+      </c>
+      <c r="Q1286" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1287" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1287" t="s">
+        <v>2182</v>
+      </c>
+      <c r="M1287" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1287" t="s">
+        <v>2183</v>
+      </c>
+      <c r="P1287" t="s">
+        <v>2184</v>
+      </c>
+      <c r="Q1287" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1288" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1288" t="s">
+        <v>2186</v>
+      </c>
+      <c r="M1288" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1288" t="s">
+        <v>2183</v>
+      </c>
+      <c r="P1288" t="s">
+        <v>2185</v>
+      </c>
+      <c r="Q1288" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1289" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1289" t="s">
+        <v>2188</v>
+      </c>
+      <c r="M1289" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1289" t="s">
+        <v>2183</v>
+      </c>
+      <c r="P1289" t="s">
+        <v>2187</v>
+      </c>
+      <c r="Q1289" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1290" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1290" t="s">
+        <v>2190</v>
+      </c>
+      <c r="M1290" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1290" t="s">
+        <v>2183</v>
+      </c>
+      <c r="P1290" t="s">
+        <v>2189</v>
+      </c>
+      <c r="Q1290" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1291" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1291" t="s">
+        <v>2192</v>
+      </c>
+      <c r="M1291" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1291" t="s">
+        <v>2183</v>
+      </c>
+      <c r="P1291" t="s">
+        <v>2191</v>
+      </c>
+      <c r="Q1291" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1292" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1292" t="s">
+        <v>2192</v>
+      </c>
+      <c r="M1292" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1292" t="s">
+        <v>2183</v>
+      </c>
+      <c r="P1292" t="s">
+        <v>2193</v>
+      </c>
+      <c r="Q1292" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1293" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1293" t="s">
+        <v>2198</v>
+      </c>
+      <c r="M1293" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1293" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1293" t="s">
+        <v>2194</v>
+      </c>
+      <c r="Q1293" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1294" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1294" t="s">
+        <v>2197</v>
+      </c>
+      <c r="M1294" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1294" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1294" t="s">
+        <v>2196</v>
+      </c>
+      <c r="Q1294" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1295" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1295" t="s">
+        <v>2198</v>
+      </c>
+      <c r="M1295" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1295" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1295" t="s">
+        <v>2199</v>
+      </c>
+      <c r="Q1295" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1296" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1296" t="s">
+        <v>2198</v>
+      </c>
+      <c r="M1296" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1296" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1296" t="s">
+        <v>2200</v>
+      </c>
+      <c r="Q1296" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1297" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1297" t="s">
+        <v>2202</v>
+      </c>
+      <c r="M1297" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1297" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1297" t="s">
+        <v>2201</v>
+      </c>
+      <c r="Q1297" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1298" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1298" t="s">
+        <v>2202</v>
+      </c>
+      <c r="M1298" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1298" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1298" t="s">
+        <v>2203</v>
+      </c>
+      <c r="Q1298" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1299" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1299" t="s">
+        <v>2202</v>
+      </c>
+      <c r="M1299" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1299" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1299" t="s">
+        <v>2204</v>
+      </c>
+      <c r="Q1299" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1300" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1300" t="s">
+        <v>2202</v>
+      </c>
+      <c r="M1300" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1300" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1300" t="s">
+        <v>2205</v>
+      </c>
+      <c r="Q1300" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1301" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1301" t="s">
+        <v>2207</v>
+      </c>
+      <c r="M1301" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1301" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1301" t="s">
+        <v>2206</v>
+      </c>
+      <c r="Q1301" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1302" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1302" t="s">
+        <v>2209</v>
+      </c>
+      <c r="M1302" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1302" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1302" t="s">
+        <v>2208</v>
+      </c>
+      <c r="Q1302" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1303" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1303" t="s">
+        <v>2209</v>
+      </c>
+      <c r="M1303" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1303" t="s">
+        <v>2195</v>
+      </c>
+      <c r="P1303" t="s">
+        <v>2210</v>
+      </c>
+      <c r="Q1303" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1304" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1304" t="s">
+        <v>2212</v>
+      </c>
+      <c r="M1304" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1304" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1304" t="s">
+        <v>2211</v>
+      </c>
+      <c r="Q1304" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1305" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1305" t="s">
+        <v>2215</v>
+      </c>
+      <c r="M1305" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1305" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1305" t="s">
+        <v>2214</v>
+      </c>
+      <c r="Q1305" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1306" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1306" t="s">
+        <v>2217</v>
+      </c>
+      <c r="M1306" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1306" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1306" t="s">
+        <v>2216</v>
+      </c>
+      <c r="Q1306" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1307" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1307" t="s">
+        <v>2217</v>
+      </c>
+      <c r="M1307" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1307" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1307" t="s">
+        <v>2218</v>
+      </c>
+      <c r="Q1307" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1308" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1308" t="s">
+        <v>2220</v>
+      </c>
+      <c r="M1308" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1308" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1308" t="s">
+        <v>2219</v>
+      </c>
+      <c r="Q1308" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1309" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1309" t="s">
+        <v>2222</v>
+      </c>
+      <c r="M1309" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1309" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1309" t="s">
+        <v>2221</v>
+      </c>
+      <c r="Q1309" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1310" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1310" t="s">
+        <v>2222</v>
+      </c>
+      <c r="M1310" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1310" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1310" t="s">
+        <v>2223</v>
+      </c>
+      <c r="Q1310" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1311" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1311" t="s">
+        <v>2222</v>
+      </c>
+      <c r="M1311" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1311" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1311" t="s">
+        <v>2224</v>
+      </c>
+      <c r="Q1311" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1312" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1312" t="s">
+        <v>2222</v>
+      </c>
+      <c r="M1312" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1312" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1312" t="s">
+        <v>2225</v>
+      </c>
+      <c r="Q1312" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1313" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1313" t="s">
+        <v>2222</v>
+      </c>
+      <c r="M1313" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1313" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1313" t="s">
+        <v>2226</v>
+      </c>
+      <c r="Q1313" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1314" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1314" t="s">
+        <v>2228</v>
+      </c>
+      <c r="M1314" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1314" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1314" t="s">
+        <v>2227</v>
+      </c>
+      <c r="Q1314" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1315" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1315" t="s">
+        <v>2230</v>
+      </c>
+      <c r="M1315" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1315" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1315" t="s">
+        <v>2229</v>
+      </c>
+      <c r="Q1315" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1316" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1316" t="s">
+        <v>2230</v>
+      </c>
+      <c r="M1316" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1316" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1316" t="s">
+        <v>2231</v>
+      </c>
+      <c r="Q1316" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1317" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1317" t="s">
+        <v>2230</v>
+      </c>
+      <c r="M1317" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1317" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1317" t="s">
+        <v>2232</v>
+      </c>
+      <c r="Q1317" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1318" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1318" t="s">
+        <v>2230</v>
+      </c>
+      <c r="M1318" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1318" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1318" t="s">
+        <v>2233</v>
+      </c>
+      <c r="Q1318" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1319" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1319" t="s">
+        <v>2235</v>
+      </c>
+      <c r="M1319" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1319" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1319" t="s">
+        <v>2234</v>
+      </c>
+      <c r="Q1319" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1320" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1320" t="s">
+        <v>2237</v>
+      </c>
+      <c r="M1320" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1320" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1320" t="s">
+        <v>2236</v>
+      </c>
+      <c r="Q1320" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1321" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1321" t="s">
+        <v>2237</v>
+      </c>
+      <c r="M1321" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1321" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1321" t="s">
+        <v>2238</v>
+      </c>
+      <c r="Q1321" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1322" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1322" t="s">
+        <v>2237</v>
+      </c>
+      <c r="M1322" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1322" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1322" t="s">
+        <v>2239</v>
+      </c>
+      <c r="Q1322" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1323" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1323" t="s">
+        <v>2235</v>
+      </c>
+      <c r="M1323" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1323" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1323" t="s">
+        <v>2240</v>
+      </c>
+      <c r="Q1323" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1324" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1324" t="s">
+        <v>2235</v>
+      </c>
+      <c r="M1324" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1324" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1324" t="s">
+        <v>2241</v>
+      </c>
+      <c r="Q1324" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1325" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1325" t="s">
+        <v>2243</v>
+      </c>
+      <c r="M1325" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1325" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1325" t="s">
+        <v>2242</v>
+      </c>
+      <c r="Q1325" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1326" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1326" t="s">
+        <v>2243</v>
+      </c>
+      <c r="M1326" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1326" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1326" t="s">
+        <v>2244</v>
+      </c>
+      <c r="Q1326" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1327" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1327" t="s">
+        <v>2248</v>
+      </c>
+      <c r="M1327" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1327" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1327" t="s">
+        <v>2245</v>
+      </c>
+      <c r="Q1327" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1328" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1328" t="s">
+        <v>2248</v>
+      </c>
+      <c r="M1328" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1328" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1328" t="s">
+        <v>2246</v>
+      </c>
+      <c r="Q1328" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1329" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1329" t="s">
+        <v>2248</v>
+      </c>
+      <c r="M1329" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1329" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1329" t="s">
+        <v>2247</v>
+      </c>
+      <c r="Q1329" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1330" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1330" t="s">
+        <v>2248</v>
+      </c>
+      <c r="M1330" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1330" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1330" t="s">
+        <v>2249</v>
+      </c>
+      <c r="Q1330" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1331" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1331" t="s">
+        <v>2248</v>
+      </c>
+      <c r="M1331" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1331" t="s">
+        <v>2213</v>
+      </c>
+      <c r="P1331" t="s">
+        <v>2250</v>
+      </c>
+      <c r="Q1331" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P1306" r:id="rId1"/>
+    <hyperlink ref="P1308" r:id="rId2"/>
+    <hyperlink ref="P1323" r:id="rId3"/>
+    <hyperlink ref="P1327" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
TD ML = 1400
</commit_message>
<xml_diff>
--- a/webserver/model_data/TrainingData_ml.xlsx
+++ b/webserver/model_data/TrainingData_ml.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13955" uniqueCount="2251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14330" uniqueCount="2383">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -6803,6 +6803,402 @@
   </si>
   <si>
     <t>Weichspüler für's Dummvieh.</t>
+  </si>
+  <si>
+    <t>Dennoch freue ich mich, dass es Menschen gibt, die sich dieser Angelegenheit annehmen.</t>
+  </si>
+  <si>
+    <t>andenhorn</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/zeit-magazin/essen-trinken/2020-01/nachhaltige-ernaehrung-lebensmittel-restaurant-gemeinschaft-regional/seite-2</t>
+  </si>
+  <si>
+    <t>Nein, die Antwort darf nicht "extensive" Landwirtschaft heißen.</t>
+  </si>
+  <si>
+    <t>Oschnelle</t>
+  </si>
+  <si>
+    <t>Mit Methoden, die früher aus der Not heraus geboren wurden, finden wir keine Antworten auf die Fragen der Zukunft</t>
+  </si>
+  <si>
+    <t>Die Antwort ist sicher aber auch nicht die sog. "Landwirtschaft 4.0".</t>
+  </si>
+  <si>
+    <t>Wir stehen gerade am Anfang eines Erkenntnisprozesses, der die bisher ziemliche hohlen Worte "Mit der Natur arbeiten statt gegen sie" endlich mit Inhalt füllt.</t>
+  </si>
+  <si>
+    <t>Leute von heute</t>
+  </si>
+  <si>
+    <t>Kein Mensch auf dieser Welt muss "Wollhausschweine" oder "Rauwollige Landschafe" und sonstige Tiere essen.</t>
+  </si>
+  <si>
+    <t>zudem tun sich Menschen, egal ob arm, ob reich persönlich etwas Gutes, wenn sie sich fortan pflanzlich ernähren.</t>
+  </si>
+  <si>
+    <t>Ist in jeder Hinsicht das Fortschrittlichste für alle Beteiligten, gerade für diejenigen die nach uns kommen.</t>
+  </si>
+  <si>
+    <t>Das Recht auf tägliches Fleisch und Milch wird gern gepredigt.</t>
+  </si>
+  <si>
+    <t>AGB akzeptiert</t>
+  </si>
+  <si>
+    <t>Ich genieße jedoch weiterhin die Freiheit, die eine Woche vielleicht 5 Mal oder andere Wochen gar kein Fleisch zu essen.</t>
+  </si>
+  <si>
+    <t>Ring Road</t>
+  </si>
+  <si>
+    <t>Für mich wäre das nicht toll.</t>
+  </si>
+  <si>
+    <t>Es wäre zumindest ein Anfang und würde so einige Probleme lösen.</t>
+  </si>
+  <si>
+    <t>Aber man sieht: manche wollen frei sein und ihren Konsum um jeden Preis ausleben.</t>
+  </si>
+  <si>
+    <t>Sie haben den Begriff schon genannt: Freiheit</t>
+  </si>
+  <si>
+    <t>Doch was für eine Freiheit ist das, sich gegenüber anderen Arten von Lebewesen gewalttätig und rücksichtslos zu verhalten und durch diese angebliche Freiheit die Erde und die Biodiversität nachhaltig zu zerstören?</t>
+  </si>
+  <si>
+    <t>Ja, Egoismus ist die Basis allen Übels.</t>
+  </si>
+  <si>
+    <t>Irren ist nunmal menschlich.</t>
+  </si>
+  <si>
+    <t>Mal abgesehen davon, wie realistisch ist Ihr Vorschlag?</t>
+  </si>
+  <si>
+    <t>Wer kontrolliert denn, ob ich zweimal wöchentlich Fleisch esse?</t>
+  </si>
+  <si>
+    <t>Sehen Sie, je mehr man darüber nachdenkt, umso unwirklicher wirkt dieser Gedanke.</t>
+  </si>
+  <si>
+    <t>Warum kontrollieren Sie es denn nicht nicht einfach selbst?</t>
+  </si>
+  <si>
+    <t>seli</t>
+  </si>
+  <si>
+    <t>Wenn Sie nicht auf Ihrem vermeintlichen Freiheitsrecht pochen würden, sondern Einsicht und Rücksicht für die Bedürfnisse der Welt finden könnten, würden solche Fragen überflüssig und ein wenig Utopie würde Wirklichkeit.</t>
+  </si>
+  <si>
+    <t>Gute Entscheidung, wenn ich das mal so unbedarft sagen darf.</t>
+  </si>
+  <si>
+    <t>Daniel-Pascal Zorn</t>
+  </si>
+  <si>
+    <t>https://twitter.com/jholofernes/status/1197188701144657920</t>
+  </si>
+  <si>
+    <t>Persona abwerfen, sich neu entwerfen.</t>
+  </si>
+  <si>
+    <t>Das klingt wunderbar!</t>
+  </si>
+  <si>
+    <t>jasmin schreiber</t>
+  </si>
+  <si>
+    <t>Stefan Baur</t>
+  </si>
+  <si>
+    <t>Schade, die Helden fehlen mir immer noch sehr.</t>
+  </si>
+  <si>
+    <t>Ich freue mich auf alle kommenden Reiseberichte.</t>
+  </si>
+  <si>
+    <t>Super schön geschrieben.</t>
+  </si>
+  <si>
+    <t>Mike Linsenbold</t>
+  </si>
+  <si>
+    <t>Micha</t>
+  </si>
+  <si>
+    <t>Das ist so aufregend.</t>
+  </si>
+  <si>
+    <t>Lea's imperfect photography</t>
+  </si>
+  <si>
+    <t>Ein tolles und mutiges Statement</t>
+  </si>
+  <si>
+    <t>Jonas Caesar</t>
+  </si>
+  <si>
+    <t>Ja gut. Schon einen an der Waffel. Insofern schadet ein Rücktritt nicht.</t>
+  </si>
+  <si>
+    <t>Chris Bloom</t>
+  </si>
+  <si>
+    <t>Ich bin sowas von mit am Start!</t>
+  </si>
+  <si>
+    <t>Telekommanderin</t>
+  </si>
+  <si>
+    <t>wie cool und praktisch, dass dein neues und altes ich den gleichen namen tragen</t>
+  </si>
+  <si>
+    <t>kellners</t>
+  </si>
+  <si>
+    <t>Toll, Du machst den Ziggy Stardust.</t>
+  </si>
+  <si>
+    <t>Woman in the attic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dein Ding wird bestimmt großartig, </t>
+  </si>
+  <si>
+    <t>Dorothea Müller</t>
+  </si>
+  <si>
+    <t>ich freu mich für Dich...Wiese im Herbst ist fantastisch!</t>
+  </si>
+  <si>
+    <t>Frau Hasenherz</t>
+  </si>
+  <si>
+    <t>Die schönste Rücktrittserklärung überhaupt.</t>
+  </si>
+  <si>
+    <t>Charlotte Obermeier</t>
+  </si>
+  <si>
+    <t>Nur der Wandel ist stetig!</t>
+  </si>
+  <si>
+    <t>DerBuddler</t>
+  </si>
+  <si>
+    <t>Herzlichen Glückwunsch und gutes Gelingen!</t>
+  </si>
+  <si>
+    <t>Das wird so geil, yeah!</t>
+  </si>
+  <si>
+    <t>We are the Discovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das liest sich alles sooooo schön. </t>
+  </si>
+  <si>
+    <t>Moritz</t>
+  </si>
+  <si>
+    <t>Wünsche dir alles tolle!!!</t>
+  </si>
+  <si>
+    <t>Ein Mensch</t>
+  </si>
+  <si>
+    <t>immer wieder sich neu erfinden mache ich auch immer</t>
+  </si>
+  <si>
+    <t>Wie überaus bedauerlich.</t>
+  </si>
+  <si>
+    <t>Jörg Karlauf</t>
+  </si>
+  <si>
+    <t>Ich werde die Musikerin Judith Holofernes ganz dolle vermissen...</t>
+  </si>
+  <si>
+    <t>Aber das Video ist ganz schön hart</t>
+  </si>
+  <si>
+    <t>Laila</t>
+  </si>
+  <si>
+    <t>https://twitter.com/unheilig_com/status/1029075613846568961</t>
+  </si>
+  <si>
+    <t>Super Song</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klingt von der Musik her,schon arg nach Unheilig.Nicht schlecht </t>
+  </si>
+  <si>
+    <t>Holger Kupitz</t>
+  </si>
+  <si>
+    <t>Was für ein toller Auftritt von Sotiria beim Schlagerbooom 2018!</t>
+  </si>
+  <si>
+    <t>Ich find Schlager toll</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?time_continue=50&amp;v=p8B7J0YkMro&amp;feature=emb_logo</t>
+  </si>
+  <si>
+    <t>Man merkt einfach das der Graf an dem Lied mitgewirkt hat.</t>
+  </si>
+  <si>
+    <t>Hört sich aber super an.</t>
+  </si>
+  <si>
+    <t>Christian V</t>
+  </si>
+  <si>
+    <t>Absoluter Gänsehaut Titel.</t>
+  </si>
+  <si>
+    <t>Hendrik Schmidt</t>
+  </si>
+  <si>
+    <t>So ein berührendes Lied ein Titel der unter die Haut geht</t>
+  </si>
+  <si>
+    <t>Florian Maier</t>
+  </si>
+  <si>
+    <t>Und den Grafen hört man in jedem Ton - sehr gut!</t>
+  </si>
+  <si>
+    <t>jcdcarsandmusic</t>
+  </si>
+  <si>
+    <t>Wow!! Einfach nur wow!</t>
+  </si>
+  <si>
+    <t>Vivien Kister</t>
+  </si>
+  <si>
+    <t>So ein schönes Lied.</t>
+  </si>
+  <si>
+    <t>wenn der Chor dazukommt Gänsehaut pur</t>
+  </si>
+  <si>
+    <t>Cindy H.</t>
+  </si>
+  <si>
+    <t>Der Graf hat mal wieder eine prima eingebung gehabt und dann super dargestellt einfach</t>
+  </si>
+  <si>
+    <t>Nico Neidthardt</t>
+  </si>
+  <si>
+    <t>Wow was für ein Tolles Lied</t>
+  </si>
+  <si>
+    <t>Lydia Wolff</t>
+  </si>
+  <si>
+    <t>Wunderschönes Lied aber wie Sotiria, Bravo!</t>
+  </si>
+  <si>
+    <t>M.T.K.</t>
+  </si>
+  <si>
+    <t>Einfach eine tolle Sängerin und eine super Frau</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Wunderschön und sehr gefühlsvoll</t>
+  </si>
+  <si>
+    <t>little lamm</t>
+  </si>
+  <si>
+    <t>Das Lied ist soooooo schön</t>
+  </si>
+  <si>
+    <t>Julia Schöfberger</t>
+  </si>
+  <si>
+    <t>Wahnsinn! Dieses Lied ist mega</t>
+  </si>
+  <si>
+    <t>Tinord</t>
+  </si>
+  <si>
+    <t>Ich kannte sie vorher gar nicht...aber der Song hat mich schon berührt</t>
+  </si>
+  <si>
+    <t>Michael Lohmann</t>
+  </si>
+  <si>
+    <t>Diese Lied erinnert mich an ein anderes</t>
+  </si>
+  <si>
+    <t>Ari</t>
+  </si>
+  <si>
+    <t>Playback des Jahres?</t>
+  </si>
+  <si>
+    <t>Akhi</t>
+  </si>
+  <si>
+    <t>Schön aber ich bezweifle ob es wirklich Live ist</t>
+  </si>
+  <si>
+    <t>johan bauwens</t>
+  </si>
+  <si>
+    <t>ja so geht's mir auch manchmal</t>
+  </si>
+  <si>
+    <t>Jürgen Schulze</t>
+  </si>
+  <si>
+    <t>Soooooooooooooooooooo toll</t>
+  </si>
+  <si>
+    <t>Jana</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=uaEiVAODN-A</t>
+  </si>
+  <si>
+    <t>Ich liebe diesen Gitarristen.</t>
+  </si>
+  <si>
+    <t>Hardocore</t>
+  </si>
+  <si>
+    <t>Die Nummer ist so geil.</t>
+  </si>
+  <si>
+    <t>1carnivore1</t>
+  </si>
+  <si>
+    <t>die gnaze band war extraklasse</t>
+  </si>
+  <si>
+    <t>ustwelve</t>
+  </si>
+  <si>
+    <t>Der Drummer war/ist klasse.</t>
+  </si>
+  <si>
+    <t>Mo makes Art</t>
+  </si>
+  <si>
+    <t>immer wieder mega !!!!!</t>
+  </si>
+  <si>
+    <t>Rene Muellers</t>
   </si>
 </sst>
 </file>
@@ -7170,12 +7566,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1331"/>
+  <dimension ref="A1:W1406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1329" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1404" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="P1331" sqref="P1331"/>
+      <selection pane="bottomLeft" activeCell="M1403" sqref="M1403:N1406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -69303,6 +69699,1281 @@
         <v>19</v>
       </c>
     </row>
+    <row r="1332" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1332" t="s">
+        <v>2252</v>
+      </c>
+      <c r="M1332" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1332" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1332" t="s">
+        <v>2251</v>
+      </c>
+      <c r="Q1332" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1333" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1333" t="s">
+        <v>2255</v>
+      </c>
+      <c r="M1333" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1333" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1333" t="s">
+        <v>2254</v>
+      </c>
+      <c r="Q1333" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1334" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1334" t="s">
+        <v>2255</v>
+      </c>
+      <c r="M1334" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1334" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1334" t="s">
+        <v>2256</v>
+      </c>
+      <c r="Q1334" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1335" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1335" t="s">
+        <v>2255</v>
+      </c>
+      <c r="M1335" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1335" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1335" t="s">
+        <v>2257</v>
+      </c>
+      <c r="Q1335" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1336" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1336" t="s">
+        <v>2255</v>
+      </c>
+      <c r="M1336" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1336" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1336" t="s">
+        <v>2258</v>
+      </c>
+      <c r="Q1336" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1337" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1337" t="s">
+        <v>2259</v>
+      </c>
+      <c r="M1337" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1337" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1337" t="s">
+        <v>2260</v>
+      </c>
+      <c r="Q1337" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1338" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1338" t="s">
+        <v>2259</v>
+      </c>
+      <c r="M1338" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1338" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1338" t="s">
+        <v>2261</v>
+      </c>
+      <c r="Q1338" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1339" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1339" t="s">
+        <v>2259</v>
+      </c>
+      <c r="M1339" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1339" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1339" t="s">
+        <v>2262</v>
+      </c>
+      <c r="Q1339" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1340" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1340" t="s">
+        <v>2264</v>
+      </c>
+      <c r="M1340" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1340" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1340" t="s">
+        <v>2263</v>
+      </c>
+      <c r="Q1340" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1341" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1341" t="s">
+        <v>2266</v>
+      </c>
+      <c r="M1341" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1341" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1341" t="s">
+        <v>2265</v>
+      </c>
+      <c r="Q1341" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1342" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1342" t="s">
+        <v>2259</v>
+      </c>
+      <c r="M1342" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1342" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1342" t="s">
+        <v>2267</v>
+      </c>
+      <c r="Q1342" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1343" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1343" t="s">
+        <v>2264</v>
+      </c>
+      <c r="M1343" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1343" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1343" t="s">
+        <v>2268</v>
+      </c>
+      <c r="Q1343" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1344" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1344" t="s">
+        <v>2264</v>
+      </c>
+      <c r="M1344" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1344" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1344" t="s">
+        <v>2269</v>
+      </c>
+      <c r="Q1344" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1345" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1345" t="s">
+        <v>2266</v>
+      </c>
+      <c r="M1345" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1345" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1345" t="s">
+        <v>2270</v>
+      </c>
+      <c r="Q1345" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1346" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1346" t="s">
+        <v>2264</v>
+      </c>
+      <c r="M1346" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1346" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1346" t="s">
+        <v>2271</v>
+      </c>
+      <c r="Q1346" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1347" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1347" t="s">
+        <v>2259</v>
+      </c>
+      <c r="M1347" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1347" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1347" t="s">
+        <v>2272</v>
+      </c>
+      <c r="Q1347" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1348" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1348" t="s">
+        <v>2266</v>
+      </c>
+      <c r="M1348" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1348" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1348" t="s">
+        <v>2273</v>
+      </c>
+      <c r="Q1348" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1349" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1349" t="s">
+        <v>2266</v>
+      </c>
+      <c r="M1349" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1349" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1349" t="s">
+        <v>2274</v>
+      </c>
+      <c r="Q1349" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1350" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1350" t="s">
+        <v>2266</v>
+      </c>
+      <c r="M1350" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1350" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1350" t="s">
+        <v>2275</v>
+      </c>
+      <c r="Q1350" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1351" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1351" t="s">
+        <v>2266</v>
+      </c>
+      <c r="M1351" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1351" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1351" t="s">
+        <v>2276</v>
+      </c>
+      <c r="Q1351" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1352" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1352" t="s">
+        <v>2278</v>
+      </c>
+      <c r="M1352" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1352" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1352" t="s">
+        <v>2277</v>
+      </c>
+      <c r="Q1352" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1353" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1353" t="s">
+        <v>2278</v>
+      </c>
+      <c r="M1353" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1353" t="s">
+        <v>2253</v>
+      </c>
+      <c r="P1353" t="s">
+        <v>2279</v>
+      </c>
+      <c r="Q1353" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1354" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1354" t="s">
+        <v>2281</v>
+      </c>
+      <c r="M1354" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1354" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1354" t="s">
+        <v>2280</v>
+      </c>
+      <c r="Q1354" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1355" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1355" t="s">
+        <v>2281</v>
+      </c>
+      <c r="M1355" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1355" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1355" t="s">
+        <v>2283</v>
+      </c>
+      <c r="Q1355" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1356" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1356" t="s">
+        <v>2285</v>
+      </c>
+      <c r="M1356" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1356" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1356" t="s">
+        <v>2284</v>
+      </c>
+      <c r="Q1356" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1357" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1357" t="s">
+        <v>2286</v>
+      </c>
+      <c r="M1357" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1357" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1357" t="s">
+        <v>2287</v>
+      </c>
+      <c r="Q1357" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1358" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1358" t="s">
+        <v>2291</v>
+      </c>
+      <c r="M1358" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1358" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1358" t="s">
+        <v>2288</v>
+      </c>
+      <c r="Q1358" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1359" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1359" t="s">
+        <v>2290</v>
+      </c>
+      <c r="M1359" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1359" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1359" t="s">
+        <v>2289</v>
+      </c>
+      <c r="Q1359" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1360" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1360" t="s">
+        <v>2293</v>
+      </c>
+      <c r="M1360" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1360" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1360" t="s">
+        <v>2292</v>
+      </c>
+      <c r="Q1360" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1361" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1361" t="s">
+        <v>2295</v>
+      </c>
+      <c r="M1361" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1361" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1361" t="s">
+        <v>2294</v>
+      </c>
+      <c r="Q1361" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1362" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1362" t="s">
+        <v>2297</v>
+      </c>
+      <c r="M1362" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1362" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1362" t="s">
+        <v>2296</v>
+      </c>
+      <c r="Q1362" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1363" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1363" t="s">
+        <v>2299</v>
+      </c>
+      <c r="M1363" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1363" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1363" t="s">
+        <v>2298</v>
+      </c>
+      <c r="Q1363" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1364" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1364" t="s">
+        <v>2301</v>
+      </c>
+      <c r="M1364" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1364" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1364" t="s">
+        <v>2300</v>
+      </c>
+      <c r="Q1364" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1365" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1365" t="s">
+        <v>2303</v>
+      </c>
+      <c r="M1365" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1365" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1365" t="s">
+        <v>2302</v>
+      </c>
+      <c r="Q1365" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1366" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1366" t="s">
+        <v>2305</v>
+      </c>
+      <c r="M1366" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1366" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1366" t="s">
+        <v>2304</v>
+      </c>
+      <c r="Q1366" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1367" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1367" t="s">
+        <v>2307</v>
+      </c>
+      <c r="M1367" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1367" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1367" t="s">
+        <v>2306</v>
+      </c>
+      <c r="Q1367" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1368" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1368" t="s">
+        <v>2309</v>
+      </c>
+      <c r="M1368" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1368" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1368" t="s">
+        <v>2308</v>
+      </c>
+      <c r="Q1368" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1369" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1369" t="s">
+        <v>2311</v>
+      </c>
+      <c r="M1369" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1369" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1369" t="s">
+        <v>2310</v>
+      </c>
+      <c r="Q1369" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1370" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1370" t="s">
+        <v>2314</v>
+      </c>
+      <c r="M1370" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1370" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1370" t="s">
+        <v>2312</v>
+      </c>
+      <c r="Q1370" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1371" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1371" t="s">
+        <v>2314</v>
+      </c>
+      <c r="M1371" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1371" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1371" t="s">
+        <v>2313</v>
+      </c>
+      <c r="Q1371" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1372" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1372" t="s">
+        <v>2316</v>
+      </c>
+      <c r="M1372" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1372" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1372" t="s">
+        <v>2315</v>
+      </c>
+      <c r="Q1372" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1373" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1373" t="s">
+        <v>2316</v>
+      </c>
+      <c r="M1373" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1373" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1373" t="s">
+        <v>2317</v>
+      </c>
+      <c r="Q1373" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1374" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1374" t="s">
+        <v>2318</v>
+      </c>
+      <c r="M1374" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1374" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1374" t="s">
+        <v>2319</v>
+      </c>
+      <c r="Q1374" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1375" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1375" t="s">
+        <v>2321</v>
+      </c>
+      <c r="M1375" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1375" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1375" t="s">
+        <v>2320</v>
+      </c>
+      <c r="Q1375" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1376" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1376" t="s">
+        <v>2321</v>
+      </c>
+      <c r="M1376" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1376" t="s">
+        <v>2282</v>
+      </c>
+      <c r="P1376" t="s">
+        <v>2322</v>
+      </c>
+      <c r="Q1376" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1377" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1377" t="s">
+        <v>2324</v>
+      </c>
+      <c r="M1377" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1377" t="s">
+        <v>2325</v>
+      </c>
+      <c r="P1377" t="s">
+        <v>2323</v>
+      </c>
+      <c r="Q1377" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1378" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1378" t="s">
+        <v>2324</v>
+      </c>
+      <c r="M1378" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1378" t="s">
+        <v>2325</v>
+      </c>
+      <c r="P1378" t="s">
+        <v>2326</v>
+      </c>
+      <c r="Q1378" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1379" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1379" t="s">
+        <v>2328</v>
+      </c>
+      <c r="M1379" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1379" t="s">
+        <v>2325</v>
+      </c>
+      <c r="P1379" t="s">
+        <v>2327</v>
+      </c>
+      <c r="Q1379" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1380" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1380" t="s">
+        <v>2330</v>
+      </c>
+      <c r="M1380" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1380" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1380" t="s">
+        <v>2329</v>
+      </c>
+      <c r="Q1380" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1381" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1381" t="s">
+        <v>2334</v>
+      </c>
+      <c r="M1381" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1381" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1381" t="s">
+        <v>2332</v>
+      </c>
+      <c r="Q1381" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1382" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1382" t="s">
+        <v>2334</v>
+      </c>
+      <c r="M1382" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1382" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1382" t="s">
+        <v>2333</v>
+      </c>
+      <c r="Q1382" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1383" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1383" t="s">
+        <v>2336</v>
+      </c>
+      <c r="M1383" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1383" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1383" t="s">
+        <v>2335</v>
+      </c>
+      <c r="Q1383" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1384" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1384" t="s">
+        <v>2338</v>
+      </c>
+      <c r="M1384" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1384" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1384" t="s">
+        <v>2337</v>
+      </c>
+      <c r="Q1384" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1385" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1385" t="s">
+        <v>2340</v>
+      </c>
+      <c r="M1385" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1385" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1385" t="s">
+        <v>2339</v>
+      </c>
+      <c r="Q1385" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1386" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1386" t="s">
+        <v>2342</v>
+      </c>
+      <c r="M1386" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1386" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1386" t="s">
+        <v>2341</v>
+      </c>
+      <c r="Q1386" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1387" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1387" t="s">
+        <v>2342</v>
+      </c>
+      <c r="M1387" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1387" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1387" t="s">
+        <v>2343</v>
+      </c>
+      <c r="Q1387" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1388" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1388" t="s">
+        <v>2345</v>
+      </c>
+      <c r="M1388" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1388" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1388" t="s">
+        <v>2344</v>
+      </c>
+      <c r="Q1388" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1389" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1389" t="s">
+        <v>2347</v>
+      </c>
+      <c r="M1389" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1389" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1389" t="s">
+        <v>2346</v>
+      </c>
+      <c r="Q1389" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1390" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1390" t="s">
+        <v>2349</v>
+      </c>
+      <c r="M1390" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1390" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1390" t="s">
+        <v>2348</v>
+      </c>
+      <c r="Q1390" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1391" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1391" t="s">
+        <v>2351</v>
+      </c>
+      <c r="M1391" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1391" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1391" t="s">
+        <v>2350</v>
+      </c>
+      <c r="Q1391" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1392" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1392" t="s">
+        <v>2353</v>
+      </c>
+      <c r="M1392" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1392" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1392" t="s">
+        <v>2352</v>
+      </c>
+      <c r="Q1392" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1393" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1393" t="s">
+        <v>2355</v>
+      </c>
+      <c r="M1393" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1393" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1393" t="s">
+        <v>2354</v>
+      </c>
+      <c r="Q1393" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1394" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1394" t="s">
+        <v>2357</v>
+      </c>
+      <c r="M1394" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1394" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1394" t="s">
+        <v>2356</v>
+      </c>
+      <c r="Q1394" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1395" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1395" t="s">
+        <v>2359</v>
+      </c>
+      <c r="M1395" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1395" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1395" t="s">
+        <v>2358</v>
+      </c>
+      <c r="Q1395" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1396" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1396" t="s">
+        <v>2361</v>
+      </c>
+      <c r="M1396" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1396" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1396" t="s">
+        <v>2360</v>
+      </c>
+      <c r="Q1396" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1397" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1397" t="s">
+        <v>2363</v>
+      </c>
+      <c r="M1397" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1397" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1397" t="s">
+        <v>2362</v>
+      </c>
+      <c r="Q1397" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1398" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1398" t="s">
+        <v>2365</v>
+      </c>
+      <c r="M1398" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1398" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1398" t="s">
+        <v>2364</v>
+      </c>
+      <c r="Q1398" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1399" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1399" t="s">
+        <v>2367</v>
+      </c>
+      <c r="M1399" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1399" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1399" t="s">
+        <v>2366</v>
+      </c>
+      <c r="Q1399" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1400" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1400" t="s">
+        <v>2369</v>
+      </c>
+      <c r="M1400" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1400" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1400" t="s">
+        <v>2368</v>
+      </c>
+      <c r="Q1400" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1401" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1401" t="s">
+        <v>2371</v>
+      </c>
+      <c r="M1401" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1401" t="s">
+        <v>2331</v>
+      </c>
+      <c r="P1401" t="s">
+        <v>2370</v>
+      </c>
+      <c r="Q1401" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1402" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1402" t="s">
+        <v>2374</v>
+      </c>
+      <c r="M1402" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1402" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1402" t="s">
+        <v>2373</v>
+      </c>
+      <c r="Q1402" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1403" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1403" t="s">
+        <v>2376</v>
+      </c>
+      <c r="M1403" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1403" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1403" t="s">
+        <v>2375</v>
+      </c>
+      <c r="Q1403" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1404" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1404" t="s">
+        <v>2378</v>
+      </c>
+      <c r="M1404" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1404" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1404" t="s">
+        <v>2377</v>
+      </c>
+      <c r="Q1404" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1405" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1405" t="s">
+        <v>2380</v>
+      </c>
+      <c r="M1405" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1405" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1405" t="s">
+        <v>2379</v>
+      </c>
+      <c r="Q1405" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1406" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1406" t="s">
+        <v>2382</v>
+      </c>
+      <c r="M1406" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1406" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1406" t="s">
+        <v>2381</v>
+      </c>
+      <c r="Q1406" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="P1306" r:id="rId1"/>

</xml_diff>

<commit_message>
TD ML = 1500
</commit_message>
<xml_diff>
--- a/webserver/model_data/TrainingData_ml.xlsx
+++ b/webserver/model_data/TrainingData_ml.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14330" uniqueCount="2383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14868" uniqueCount="2542">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -7199,6 +7199,483 @@
   </si>
   <si>
     <t>Rene Muellers</t>
+  </si>
+  <si>
+    <t>Das ist so ne Rotze zum Schluss die schreit und stönnt ja nur noch rum</t>
+  </si>
+  <si>
+    <t>Mr LackMulex</t>
+  </si>
+  <si>
+    <t>So ein kak Lied!</t>
+  </si>
+  <si>
+    <t>Karin Geiler</t>
+  </si>
+  <si>
+    <t>Bullshit</t>
+  </si>
+  <si>
+    <t>JjSs WERER</t>
+  </si>
+  <si>
+    <t>Die Genialität und die Einzigartigkeit dieses Werks scheint kaum noch Gehör zu finden, geschweige denn den Respekt/die Anerkennung zu erfahren, der ihr gebührt.</t>
+  </si>
+  <si>
+    <t>Alan Ladd seine Katze</t>
+  </si>
+  <si>
+    <t>Das ist kackeeeeeeeeee</t>
+  </si>
+  <si>
+    <t>squaddEmre</t>
+  </si>
+  <si>
+    <t>punk a la card</t>
+  </si>
+  <si>
+    <t>Gregor Bakunin</t>
+  </si>
+  <si>
+    <t>Hinter dieser starken Message geht es beinahe verloren, dass dieses Lied auch musikalisch und gesangstechnisch von einer Qualität ist, die man heute vergeblich sucht.</t>
+  </si>
+  <si>
+    <t>Benno Witter</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GK51vq95j1s</t>
+  </si>
+  <si>
+    <t>Top Sound</t>
+  </si>
+  <si>
+    <t>L Wagner</t>
+  </si>
+  <si>
+    <t>Lyric trifft ins Schwarze.</t>
+  </si>
+  <si>
+    <t>Schöne klare Stimme!</t>
+  </si>
+  <si>
+    <t>Das waren die 80´s toll!</t>
+  </si>
+  <si>
+    <t>Butz Pennymaker</t>
+  </si>
+  <si>
+    <t>So aktuell wie nie !!!</t>
+  </si>
+  <si>
+    <t>Birgit Kröger</t>
+  </si>
+  <si>
+    <t>Tolle Erinnerung an diese Zeit.</t>
+  </si>
+  <si>
+    <t>Vogelweyhde</t>
+  </si>
+  <si>
+    <t>sie hat voll das liebe Lächeln</t>
+  </si>
+  <si>
+    <t>C S</t>
+  </si>
+  <si>
+    <t>da hatte noch jeder seine eigene Kreativität</t>
+  </si>
+  <si>
+    <t>bernie van Halen</t>
+  </si>
+  <si>
+    <t>Schönes Lied in schönen Zeiten.</t>
+  </si>
+  <si>
+    <t>IrudienLentegia</t>
+  </si>
+  <si>
+    <t>Kult</t>
+  </si>
+  <si>
+    <t>Bernd Bratton</t>
+  </si>
+  <si>
+    <t>Soooooooo geil</t>
+  </si>
+  <si>
+    <t>Tanja Busch</t>
+  </si>
+  <si>
+    <t>Das waren Zeiten!</t>
+  </si>
+  <si>
+    <t>Storm Hansen</t>
+  </si>
+  <si>
+    <t>genial die kreative NDW Zeit ....</t>
+  </si>
+  <si>
+    <t>Hab sie gar nicht mehr so hübsch in Erinnerung</t>
+  </si>
+  <si>
+    <t>schreiterkeit</t>
+  </si>
+  <si>
+    <t>Sah echt klasse aus, damals, die Ina.</t>
+  </si>
+  <si>
+    <t>Tolles Lied</t>
+  </si>
+  <si>
+    <t>Carina Stender</t>
+  </si>
+  <si>
+    <t>Kult aus der NDW Zeit</t>
+  </si>
+  <si>
+    <t>Downnumbereight</t>
+  </si>
+  <si>
+    <t>YEEP yeep</t>
+  </si>
+  <si>
+    <t>antje tautkus</t>
+  </si>
+  <si>
+    <t>Der Klassiker</t>
+  </si>
+  <si>
+    <t>DuDie72</t>
+  </si>
+  <si>
+    <t>classic!</t>
+  </si>
+  <si>
+    <t>Gott, was 'ne tolle Frau.</t>
+  </si>
+  <si>
+    <t>Lee La</t>
+  </si>
+  <si>
+    <t>wo sind solche Frauen heute?</t>
+  </si>
+  <si>
+    <t>Ich beneide meine Mama igdwie, daß das ihre Generation ist und sie ihre Jugend in dieser Zeit erlebt hat.</t>
+  </si>
+  <si>
+    <t>Heute ist alles so gleich</t>
+  </si>
+  <si>
+    <t>alle sollen gleich sein und nur Oberflächlichkeiten beherrschen die Köpfe der meisten Frauen.</t>
+  </si>
+  <si>
+    <t>Klasse Musik!</t>
+  </si>
+  <si>
+    <t>hey men</t>
+  </si>
+  <si>
+    <t>Noch echt gute Melodien damals!</t>
+  </si>
+  <si>
+    <t>Solche Frauen wie dich, braucht das Land auch Ina.</t>
+  </si>
+  <si>
+    <t>Beste Version!</t>
+  </si>
+  <si>
+    <t>tolle Version !</t>
+  </si>
+  <si>
+    <t>monika müller</t>
+  </si>
+  <si>
+    <t>ach, schöne alte Zeiten, damals...</t>
+  </si>
+  <si>
+    <t>Adriaan Camambert</t>
+  </si>
+  <si>
+    <t>einfach nur Suuuper</t>
+  </si>
+  <si>
+    <t>ulli wiermann</t>
+  </si>
+  <si>
+    <t>Neue Frauen brauch das Land ihr seid zu verklemmt</t>
+  </si>
+  <si>
+    <t>Christian putzi</t>
+  </si>
+  <si>
+    <t>Unglaublich!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wow - diese Version gefällt mir von allen bisher gehörten am besten! </t>
+  </si>
+  <si>
+    <t>Michael Schiffmann</t>
+  </si>
+  <si>
+    <t>cinderella 0307</t>
+  </si>
+  <si>
+    <t>Da ist richtig Feuer dahinter und es kribbelt einem sofort in den Füßen.</t>
+  </si>
+  <si>
+    <t>Danke für's Einstellen.</t>
+  </si>
+  <si>
+    <t>AIDAsign medienbüro</t>
+  </si>
+  <si>
+    <t>hart aber ehrlich</t>
+  </si>
+  <si>
+    <t>echt handgezufte mucke, passt auf die heutige zeit</t>
+  </si>
+  <si>
+    <t>Diesen Einwurf mit dem Atommüll bei 3:32 finde und fand ich nie gut bei Konzerten</t>
+  </si>
+  <si>
+    <t>Hermes Phettberg</t>
+  </si>
+  <si>
+    <t>gehörte aber zur damaligen Zeit einfach dazu</t>
+  </si>
+  <si>
+    <t>Auf der anderen Seite waren es aber gerade diese Themen, die die Gesellschaft in Bewegung hielten.</t>
+  </si>
+  <si>
+    <t>Nicht immer zum Guten, wenn man den politisch motivierten Terror bedenkt</t>
+  </si>
+  <si>
+    <t>Und trotzdem fehlt mir heute irgendwie das Rotzige von damals</t>
+  </si>
+  <si>
+    <t>Alles uniformiert heute und bei manch einem ist das Ventil unter anderem auch die AFD, leider</t>
+  </si>
+  <si>
+    <t>Aber gut, war toll, diese Zeit mitgemacht zu haben.</t>
+  </si>
+  <si>
+    <t>Oh Gott Nein!</t>
+  </si>
+  <si>
+    <t>Professor Trefusius</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/kultur/musik/2020-02/james-bond-song-billie-eilish-no-time-to-die</t>
+  </si>
+  <si>
+    <t>Nicht Hans Zimmer!</t>
+  </si>
+  <si>
+    <t>Die Zahl der Filme die er mit seinem Lärm ruiniert hat (von Gladiator und bis Interstellar) ist jetzt schon Legion, jetzt bitte nicht noch James Bond!</t>
+  </si>
+  <si>
+    <t>Gegen Billy Eillish, spricht nichts, auch wenn ich sie nicht für das Uebergenie halte, dass manche in Ihr sehen.</t>
+  </si>
+  <si>
+    <t>Skyfall war viel besser.</t>
+  </si>
+  <si>
+    <t>Der Song hat fast gar nichts.</t>
+  </si>
+  <si>
+    <t>ssr</t>
+  </si>
+  <si>
+    <t>Ihre Stimme ist bei weitem nicht so überzeugend und beeindruckend wie die von z.B. Adele.</t>
+  </si>
+  <si>
+    <t>Nein, der nächste kann gerne wieder eine ausdrucksstärkere Stimme haben und origineller sein.</t>
+  </si>
+  <si>
+    <t>Ich fand den Song etwas mager.</t>
+  </si>
+  <si>
+    <t>Eher weniger als mehr.</t>
+  </si>
+  <si>
+    <t>Um Charme gehts schon lange nicht mehr.</t>
+  </si>
+  <si>
+    <t>hairy</t>
+  </si>
+  <si>
+    <t>Sondern ums Marketing.</t>
+  </si>
+  <si>
+    <t>Wenn man irgendwas besser verkaufen will, klebt man vorn noch ein celebrity mehr drauf.</t>
+  </si>
+  <si>
+    <t>Bei allem Respekt vor verschiedenen Meinungen</t>
+  </si>
+  <si>
+    <t>younes1</t>
+  </si>
+  <si>
+    <t>Hans Zimmers Musik als „Lärm“ zu bezeichnen ist wirklich lächerlich.</t>
+  </si>
+  <si>
+    <t>Zuminest einmal Interstallar wäre ohne Zimmers Musik nur halb so gut.</t>
+  </si>
+  <si>
+    <t>Frank-Werner</t>
+  </si>
+  <si>
+    <t>Wenn ich da etwa an die minutenlange Andock-Sequenz an die sich langsam zerstörende Raumstation denke, so war bzw. ist dies ein ganz großer Kino-Moment - auch dank Zimmers Musik.</t>
+  </si>
+  <si>
+    <t>Dies und vor allen Dingen: nicht immer alles so furchtbar ernst nehmen.</t>
+  </si>
+  <si>
+    <t>Dass die Vertreter der Regierung in Berlin von einer neuen DDR Träumen dürfte mittlerweile jedem klar sein.</t>
+  </si>
+  <si>
+    <t>Gelöschter Nutzer 10457</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/politik/deutschland/2019-10/wohnungspolitik-mietendeckel-mietabsenkung-berlin-immobilienmarkt-faq</t>
+  </si>
+  <si>
+    <t>Probleme verbieten, süßes Gift.</t>
+  </si>
+  <si>
+    <t>magnalogger</t>
+  </si>
+  <si>
+    <t>Das ist aber gegen die Menschen, mittelfristig.</t>
+  </si>
+  <si>
+    <t>Beeindruckend, der Mann kommt authentisch rüber und weiß, was Sache ist</t>
+  </si>
+  <si>
+    <t>married to the game</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/sport/2020-02/uli-borowka-alkoholiker-sucht-fussball-nationalspieler</t>
+  </si>
+  <si>
+    <t>Und er handelt und kann helfen</t>
+  </si>
+  <si>
+    <t>Guter Text</t>
+  </si>
+  <si>
+    <t>regreub</t>
+  </si>
+  <si>
+    <t>Herr Borowka, Sie sind der wahre Leistungsträger dieser Gesellschaft!</t>
+  </si>
+  <si>
+    <t>El Capone 2.0</t>
+  </si>
+  <si>
+    <t>Mit allergrößten Respekt verneige ich mich vor Ihnen und schlage Sie für's Bundestverdienstkreuz vor.</t>
+  </si>
+  <si>
+    <t>Auf jeden Fall tolle und wichtige Arbeit, die Uli Borowka da seit geraumer Zeit leistet</t>
+  </si>
+  <si>
+    <t>Ente Willi</t>
+  </si>
+  <si>
+    <t>Kleiner Wermutstropfen: Die Geschichte um den "Eisenfuß" herum hätte meiner Meinung nach auch diskreter gehandhabt werden können</t>
+  </si>
+  <si>
+    <t>Guter Text! Danke Uli und weiter so!</t>
+  </si>
+  <si>
+    <t>Herostratos</t>
+  </si>
+  <si>
+    <t>Beeindruckend und authentisch!</t>
+  </si>
+  <si>
+    <t>Axel T</t>
+  </si>
+  <si>
+    <t>Umso wichtiger, dass es Menschen wie UB gibt, die authentisch sind und unterstützen.</t>
+  </si>
+  <si>
+    <t>tolles Interview. Weiter so!</t>
+  </si>
+  <si>
+    <t>Beasthoven</t>
+  </si>
+  <si>
+    <t>Beeindruckender Artikel in dem ein großartiger Mensch zu Wort kommt.</t>
+  </si>
+  <si>
+    <t>Borsigkreisläufer</t>
+  </si>
+  <si>
+    <t>Selbst im Suchtumfeld beruflich aktiv habe ich größten Respekt vor Menschen die ihre Sucht beherrschen und für andere eine große Hilfe sind.</t>
+  </si>
+  <si>
+    <t>Da weiß man, aus welcher Ecke der ganze Mist stammt.</t>
+  </si>
+  <si>
+    <t>https://jungefreiheit.de/debatte/kommentar/2020/saekularer-tugendwettbewerb/</t>
+  </si>
+  <si>
+    <t>Kersti Wolnow</t>
+  </si>
+  <si>
+    <t>Einen größeren Unsinn kann man nicht verbreiten</t>
+  </si>
+  <si>
+    <t>M.Kratzsch</t>
+  </si>
+  <si>
+    <t>Ideologie ist anscheinend auch für die Lehrer eine Fessel geworden, die das wissenschaftlich Denken, zumindest das Aussprechen von Wahrheiten verhindert</t>
+  </si>
+  <si>
+    <t>Wem vertrauen wir nur unsere Kinder an ?</t>
+  </si>
+  <si>
+    <t>Im Gegenteil, diese Haltung wird als STOLZ, im Sinne von Hybris, verstanden.</t>
+  </si>
+  <si>
+    <t>Veronika Batz-Jevec</t>
+  </si>
+  <si>
+    <t>Sie sind dumm und manipuliert.</t>
+  </si>
+  <si>
+    <t>Erwin der Querdenker</t>
+  </si>
+  <si>
+    <t>Von der Klimaforschung, lassen sie mich raten, haben diese Herrschaften Null Ahnung!</t>
+  </si>
+  <si>
+    <t>Sie begreifen auch nicht, dass sie missbraucht werden.</t>
+  </si>
+  <si>
+    <t>Vermutlich werden sie sehr aggressiv auf Gegenargumente und eine Gegenaufklärung reagieren.</t>
+  </si>
+  <si>
+    <t>Vernunft wird bei dieser glaubensmäßigen Sektiererei völlig ausgeschaltet.</t>
+  </si>
+  <si>
+    <t>Hieran wird deutlich, wie krank manche Ideologien machen und wie sehr diese das menschliche Hirn psychisch vergiften.</t>
+  </si>
+  <si>
+    <t>Zwischen einem paranoiden Schizphrenen gibt es hierbei durchaus erschreckende Parallelen.</t>
+  </si>
+  <si>
+    <t>Deshalb können solche auf Angst und psychischer Kontrolle beruhenden Bewegung als eine ernste Gefahr für unsere Gesellschaft gesehen werden.</t>
+  </si>
+  <si>
+    <t>Da, wo der gesunde Menschenverstand erfolgreich durch eine fortwährende Gehirnwäsche jedoch gelähmt wurde, lässt sich mit Vernunft leider nichts mehr erreichen.</t>
+  </si>
+  <si>
+    <t>Ein solches Vorgehen wirkt bei solchen Menschen immer wie eine Aggression.</t>
+  </si>
+  <si>
+    <t>Entsprechend sind dann ihre Reaktionen.</t>
   </si>
 </sst>
 </file>
@@ -7566,12 +8043,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1406"/>
+  <dimension ref="A1:W1508"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1404" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1484" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="M1403" sqref="M1403:N1406"/>
+      <selection pane="bottomLeft" activeCell="P1509" sqref="P1509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47375,7 +47852,7 @@
         <v>1198</v>
       </c>
       <c r="I714">
-        <v>0.5</v>
+        <v>0.67</v>
       </c>
       <c r="J714">
         <v>0.5</v>
@@ -70972,6 +71449,1824 @@
       </c>
       <c r="Q1406" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="1407" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1407" t="s">
+        <v>2384</v>
+      </c>
+      <c r="M1407" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1407" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1407" t="s">
+        <v>2383</v>
+      </c>
+      <c r="Q1407" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1408" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1408" t="s">
+        <v>2386</v>
+      </c>
+      <c r="M1408" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1408" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1408" t="s">
+        <v>2385</v>
+      </c>
+      <c r="Q1408" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1409" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1409" t="s">
+        <v>2388</v>
+      </c>
+      <c r="M1409" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1409" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1409" t="s">
+        <v>2387</v>
+      </c>
+      <c r="Q1409" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1410" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1410" t="s">
+        <v>2390</v>
+      </c>
+      <c r="M1410" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1410" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1410" t="s">
+        <v>2389</v>
+      </c>
+      <c r="Q1410" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1411" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1411" t="s">
+        <v>2392</v>
+      </c>
+      <c r="M1411" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1411" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1411" t="s">
+        <v>2391</v>
+      </c>
+      <c r="Q1411" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1412" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1412" t="s">
+        <v>2394</v>
+      </c>
+      <c r="M1412" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1412" t="s">
+        <v>2372</v>
+      </c>
+      <c r="P1412" t="s">
+        <v>2393</v>
+      </c>
+      <c r="Q1412" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1413" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1413" t="s">
+        <v>2396</v>
+      </c>
+      <c r="M1413" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1413" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1413" t="s">
+        <v>2395</v>
+      </c>
+      <c r="Q1413" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1414" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1414" t="s">
+        <v>2399</v>
+      </c>
+      <c r="M1414" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1414" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1414" t="s">
+        <v>2398</v>
+      </c>
+      <c r="Q1414" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1415" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1415" t="s">
+        <v>2399</v>
+      </c>
+      <c r="M1415" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1415" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1415" t="s">
+        <v>2400</v>
+      </c>
+      <c r="Q1415" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1416" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1416" t="s">
+        <v>2399</v>
+      </c>
+      <c r="M1416" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1416" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1416" t="s">
+        <v>2401</v>
+      </c>
+      <c r="Q1416" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1417" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1417" t="s">
+        <v>2403</v>
+      </c>
+      <c r="M1417" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1417" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1417" t="s">
+        <v>2402</v>
+      </c>
+      <c r="Q1417" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1418" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1418" t="s">
+        <v>2405</v>
+      </c>
+      <c r="M1418" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1418" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1418" t="s">
+        <v>2404</v>
+      </c>
+      <c r="Q1418" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1419" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1419" t="s">
+        <v>2407</v>
+      </c>
+      <c r="M1419" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1419" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1419" t="s">
+        <v>2406</v>
+      </c>
+      <c r="Q1419" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1420" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1420" t="s">
+        <v>2409</v>
+      </c>
+      <c r="M1420" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1420" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1420" t="s">
+        <v>2408</v>
+      </c>
+      <c r="Q1420" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1421" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1421" t="s">
+        <v>2411</v>
+      </c>
+      <c r="M1421" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1421" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1421" t="s">
+        <v>2410</v>
+      </c>
+      <c r="Q1421" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1422" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1422" t="s">
+        <v>2413</v>
+      </c>
+      <c r="M1422" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1422" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1422" t="s">
+        <v>2412</v>
+      </c>
+      <c r="Q1422" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1423" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1423" t="s">
+        <v>2415</v>
+      </c>
+      <c r="M1423" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1423" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1423" t="s">
+        <v>2414</v>
+      </c>
+      <c r="Q1423" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1424" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1424" t="s">
+        <v>2417</v>
+      </c>
+      <c r="M1424" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1424" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1424" t="s">
+        <v>2416</v>
+      </c>
+      <c r="Q1424" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1425" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1425" t="s">
+        <v>2419</v>
+      </c>
+      <c r="M1425" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1425" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1425" t="s">
+        <v>2418</v>
+      </c>
+      <c r="Q1425" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1426" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1426" t="s">
+        <v>2411</v>
+      </c>
+      <c r="M1426" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1426" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1426" t="s">
+        <v>2420</v>
+      </c>
+      <c r="Q1426" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1427" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1427" t="s">
+        <v>2422</v>
+      </c>
+      <c r="M1427" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1427" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1427" t="s">
+        <v>2421</v>
+      </c>
+      <c r="Q1427" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1428" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1428" t="s">
+        <v>2422</v>
+      </c>
+      <c r="M1428" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1428" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1428" t="s">
+        <v>2423</v>
+      </c>
+      <c r="Q1428" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1429" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1429" t="s">
+        <v>2425</v>
+      </c>
+      <c r="M1429" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1429" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1429" t="s">
+        <v>2424</v>
+      </c>
+      <c r="Q1429" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1430" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1430" t="s">
+        <v>2427</v>
+      </c>
+      <c r="M1430" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1430" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1430" t="s">
+        <v>2426</v>
+      </c>
+      <c r="Q1430" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1431" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1431" t="s">
+        <v>2429</v>
+      </c>
+      <c r="M1431" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1431" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1431" t="s">
+        <v>2428</v>
+      </c>
+      <c r="Q1431" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1432" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="K1432" t="s">
+        <v>2432</v>
+      </c>
+      <c r="L1432" t="s">
+        <v>2431</v>
+      </c>
+      <c r="M1432" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1432" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1432" t="s">
+        <v>2430</v>
+      </c>
+      <c r="Q1432" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1432" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1432" t="s">
+        <v>1645</v>
+      </c>
+      <c r="T1432" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1432" t="s">
+        <v>211</v>
+      </c>
+      <c r="V1432" t="s">
+        <v>72</v>
+      </c>
+      <c r="W1432" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1433" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1433" t="s">
+        <v>2434</v>
+      </c>
+      <c r="M1433" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1433" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1433" t="s">
+        <v>2433</v>
+      </c>
+      <c r="Q1433" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1434" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1434" t="s">
+        <v>2434</v>
+      </c>
+      <c r="M1434" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1434" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1434" t="s">
+        <v>2435</v>
+      </c>
+      <c r="Q1434" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1435" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1435" t="s">
+        <v>2434</v>
+      </c>
+      <c r="M1435" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1435" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1435" t="s">
+        <v>2436</v>
+      </c>
+      <c r="Q1435" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1435" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1435" t="s">
+        <v>142</v>
+      </c>
+      <c r="T1435" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1435" t="s">
+        <v>825</v>
+      </c>
+      <c r="V1435" t="s">
+        <v>542</v>
+      </c>
+      <c r="W1435" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1436" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1436" t="s">
+        <v>2434</v>
+      </c>
+      <c r="M1436" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1436" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1436" t="s">
+        <v>2437</v>
+      </c>
+      <c r="Q1436" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1436" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1436" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1436" t="s">
+        <v>552</v>
+      </c>
+      <c r="U1436" t="s">
+        <v>588</v>
+      </c>
+      <c r="V1436" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1437" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1437" t="s">
+        <v>2434</v>
+      </c>
+      <c r="M1437" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1437" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1437" t="s">
+        <v>2438</v>
+      </c>
+      <c r="Q1437" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1437" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1437" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1437" t="s">
+        <v>1645</v>
+      </c>
+      <c r="U1437" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1437" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1438" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1438" t="s">
+        <v>2440</v>
+      </c>
+      <c r="M1438" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1438" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1438" t="s">
+        <v>2439</v>
+      </c>
+      <c r="Q1438" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1439" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1439" t="s">
+        <v>2440</v>
+      </c>
+      <c r="M1439" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1439" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1439" t="s">
+        <v>2441</v>
+      </c>
+      <c r="Q1439" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1440" spans="11:23" x14ac:dyDescent="0.2">
+      <c r="L1440" t="s">
+        <v>2440</v>
+      </c>
+      <c r="M1440" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1440" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1440" t="s">
+        <v>2442</v>
+      </c>
+      <c r="Q1440" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1441" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1441" t="s">
+        <v>2440</v>
+      </c>
+      <c r="M1441" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1441" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1441" t="s">
+        <v>2443</v>
+      </c>
+      <c r="Q1441" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1442" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1442" t="s">
+        <v>2445</v>
+      </c>
+      <c r="M1442" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1442" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1442" t="s">
+        <v>2444</v>
+      </c>
+      <c r="Q1442" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1443" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1443" t="s">
+        <v>2447</v>
+      </c>
+      <c r="M1443" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1443" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1443" t="s">
+        <v>2446</v>
+      </c>
+      <c r="Q1443" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1444" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1444" t="s">
+        <v>2449</v>
+      </c>
+      <c r="M1444" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1444" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1444" t="s">
+        <v>2448</v>
+      </c>
+      <c r="Q1444" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1445" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1445" t="s">
+        <v>2451</v>
+      </c>
+      <c r="M1445" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1445" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1445" t="s">
+        <v>2450</v>
+      </c>
+      <c r="Q1445" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1446" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1446" t="s">
+        <v>2454</v>
+      </c>
+      <c r="M1446" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1446" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1446" t="s">
+        <v>2452</v>
+      </c>
+      <c r="Q1446" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1446" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1446" t="s">
+        <v>142</v>
+      </c>
+      <c r="T1446" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1446" t="s">
+        <v>350</v>
+      </c>
+      <c r="V1446" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1447" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1447" t="s">
+        <v>2455</v>
+      </c>
+      <c r="M1447" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1447" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1447" t="s">
+        <v>2453</v>
+      </c>
+      <c r="Q1447" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1448" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1448" t="s">
+        <v>2455</v>
+      </c>
+      <c r="M1448" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1448" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1448" t="s">
+        <v>2456</v>
+      </c>
+      <c r="Q1448" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1449" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1449" t="s">
+        <v>2455</v>
+      </c>
+      <c r="M1449" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1449" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1449" t="s">
+        <v>2457</v>
+      </c>
+      <c r="Q1449" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1450" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1450" t="s">
+        <v>2458</v>
+      </c>
+      <c r="M1450" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1450" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1450" t="s">
+        <v>2459</v>
+      </c>
+      <c r="Q1450" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1451" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1451" t="s">
+        <v>2458</v>
+      </c>
+      <c r="M1451" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1451" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1451" t="s">
+        <v>2460</v>
+      </c>
+      <c r="Q1451" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1452" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1452" t="s">
+        <v>2462</v>
+      </c>
+      <c r="M1452" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1452" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1452" t="s">
+        <v>2461</v>
+      </c>
+      <c r="Q1452" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1453" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1453" t="s">
+        <v>2462</v>
+      </c>
+      <c r="M1453" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1453" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1453" t="s">
+        <v>2463</v>
+      </c>
+      <c r="Q1453" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1454" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1454" t="s">
+        <v>2462</v>
+      </c>
+      <c r="M1454" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1454" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1454" t="s">
+        <v>2464</v>
+      </c>
+      <c r="Q1454" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1455" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1455" t="s">
+        <v>2462</v>
+      </c>
+      <c r="M1455" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1455" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1455" t="s">
+        <v>2465</v>
+      </c>
+      <c r="Q1455" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1456" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="L1456" t="s">
+        <v>2462</v>
+      </c>
+      <c r="M1456" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1456" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1456" t="s">
+        <v>2466</v>
+      </c>
+      <c r="Q1456" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1457" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1457" t="s">
+        <v>2462</v>
+      </c>
+      <c r="M1457" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1457" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1457" t="s">
+        <v>2467</v>
+      </c>
+      <c r="Q1457" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1458" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1458" t="s">
+        <v>2462</v>
+      </c>
+      <c r="M1458" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1458" t="s">
+        <v>2397</v>
+      </c>
+      <c r="P1458" t="s">
+        <v>2468</v>
+      </c>
+      <c r="Q1458" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1459" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1459" t="s">
+        <v>2470</v>
+      </c>
+      <c r="M1459" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1459" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1459" t="s">
+        <v>2469</v>
+      </c>
+      <c r="Q1459" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1460" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1460" t="s">
+        <v>2470</v>
+      </c>
+      <c r="M1460" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1460" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1460" t="s">
+        <v>2472</v>
+      </c>
+      <c r="Q1460" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1461" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1461" t="s">
+        <v>2470</v>
+      </c>
+      <c r="M1461" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1461" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1461" t="s">
+        <v>2473</v>
+      </c>
+      <c r="Q1461" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1462" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1462" t="s">
+        <v>2470</v>
+      </c>
+      <c r="M1462" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1462" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1462" t="s">
+        <v>2474</v>
+      </c>
+      <c r="Q1462" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1463" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1463" t="s">
+        <v>2477</v>
+      </c>
+      <c r="M1463" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1463" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1463" t="s">
+        <v>2475</v>
+      </c>
+      <c r="Q1463" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1464" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1464" t="s">
+        <v>2477</v>
+      </c>
+      <c r="M1464" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1464" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1464" t="s">
+        <v>2476</v>
+      </c>
+      <c r="Q1464" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1465" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1465" t="s">
+        <v>1955</v>
+      </c>
+      <c r="M1465" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1465" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1465" t="s">
+        <v>2478</v>
+      </c>
+      <c r="Q1465" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1466" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1466" t="s">
+        <v>1955</v>
+      </c>
+      <c r="M1466" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1466" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1466" t="s">
+        <v>2479</v>
+      </c>
+      <c r="Q1466" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1467" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1467" t="s">
+        <v>1841</v>
+      </c>
+      <c r="M1467" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1467" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1467" t="s">
+        <v>2480</v>
+      </c>
+      <c r="Q1467" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1468" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1468" t="s">
+        <v>1841</v>
+      </c>
+      <c r="M1468" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1468" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1468" t="s">
+        <v>2481</v>
+      </c>
+      <c r="Q1468" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1469" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1469" t="s">
+        <v>2483</v>
+      </c>
+      <c r="M1469" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1469" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1469" t="s">
+        <v>2482</v>
+      </c>
+      <c r="Q1469" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1470" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1470" t="s">
+        <v>2483</v>
+      </c>
+      <c r="M1470" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1470" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1470" t="s">
+        <v>2484</v>
+      </c>
+      <c r="Q1470" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1471" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1471" t="s">
+        <v>2483</v>
+      </c>
+      <c r="M1471" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1471" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1471" t="s">
+        <v>2485</v>
+      </c>
+      <c r="Q1471" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1472" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1472" t="s">
+        <v>2487</v>
+      </c>
+      <c r="M1472" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1472" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1472" t="s">
+        <v>2486</v>
+      </c>
+      <c r="Q1472" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1473" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1473" t="s">
+        <v>2487</v>
+      </c>
+      <c r="M1473" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1473" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1473" t="s">
+        <v>2488</v>
+      </c>
+      <c r="Q1473" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1474" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1474" t="s">
+        <v>2490</v>
+      </c>
+      <c r="M1474" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1474" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1474" t="s">
+        <v>2489</v>
+      </c>
+      <c r="Q1474" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1475" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1475" t="s">
+        <v>2490</v>
+      </c>
+      <c r="M1475" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1475" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1475" t="s">
+        <v>2491</v>
+      </c>
+      <c r="Q1475" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1476" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1476" t="s">
+        <v>2490</v>
+      </c>
+      <c r="M1476" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1476" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P1476" t="s">
+        <v>2492</v>
+      </c>
+      <c r="Q1476" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1477" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1477" t="s">
+        <v>2494</v>
+      </c>
+      <c r="M1477" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1477" t="s">
+        <v>2495</v>
+      </c>
+      <c r="P1477" t="s">
+        <v>2493</v>
+      </c>
+      <c r="Q1477" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1478" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1478" t="s">
+        <v>2497</v>
+      </c>
+      <c r="M1478" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1478" t="s">
+        <v>2495</v>
+      </c>
+      <c r="P1478" t="s">
+        <v>2496</v>
+      </c>
+      <c r="Q1478" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1479" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1479" t="s">
+        <v>2497</v>
+      </c>
+      <c r="M1479" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1479" t="s">
+        <v>2495</v>
+      </c>
+      <c r="P1479" t="s">
+        <v>2498</v>
+      </c>
+      <c r="Q1479" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1480" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1480" t="s">
+        <v>2500</v>
+      </c>
+      <c r="M1480" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1480" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1480" t="s">
+        <v>2499</v>
+      </c>
+      <c r="Q1480" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1481" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1481" t="s">
+        <v>2500</v>
+      </c>
+      <c r="M1481" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1481" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1481" t="s">
+        <v>2502</v>
+      </c>
+      <c r="Q1481" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1482" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1482" t="s">
+        <v>2504</v>
+      </c>
+      <c r="M1482" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1482" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1482" t="s">
+        <v>2503</v>
+      </c>
+      <c r="Q1482" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1483" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1483" t="s">
+        <v>2506</v>
+      </c>
+      <c r="M1483" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1483" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1483" t="s">
+        <v>2505</v>
+      </c>
+      <c r="Q1483" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1484" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1484" t="s">
+        <v>2506</v>
+      </c>
+      <c r="M1484" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1484" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1484" t="s">
+        <v>2507</v>
+      </c>
+      <c r="Q1484" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1485" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1485" t="s">
+        <v>2509</v>
+      </c>
+      <c r="M1485" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1485" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1485" t="s">
+        <v>2508</v>
+      </c>
+      <c r="Q1485" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1486" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1486" t="s">
+        <v>2509</v>
+      </c>
+      <c r="M1486" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1486" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1486" t="s">
+        <v>2510</v>
+      </c>
+      <c r="Q1486" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1487" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1487" t="s">
+        <v>2512</v>
+      </c>
+      <c r="M1487" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1487" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1487" t="s">
+        <v>2511</v>
+      </c>
+      <c r="Q1487" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1488" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1488" t="s">
+        <v>2514</v>
+      </c>
+      <c r="M1488" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1488" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1488" t="s">
+        <v>2513</v>
+      </c>
+      <c r="Q1488" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1489" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1489" t="s">
+        <v>2514</v>
+      </c>
+      <c r="M1489" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1489" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1489" t="s">
+        <v>2515</v>
+      </c>
+      <c r="Q1489" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1490" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1490" t="s">
+        <v>2517</v>
+      </c>
+      <c r="M1490" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1490" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1490" t="s">
+        <v>2516</v>
+      </c>
+      <c r="Q1490" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1491" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1491" t="s">
+        <v>2519</v>
+      </c>
+      <c r="M1491" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1491" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1491" t="s">
+        <v>2518</v>
+      </c>
+      <c r="Q1491" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1492" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1492" t="s">
+        <v>2519</v>
+      </c>
+      <c r="M1492" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1492" t="s">
+        <v>2501</v>
+      </c>
+      <c r="P1492" t="s">
+        <v>2520</v>
+      </c>
+      <c r="Q1492" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1493" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1493" t="s">
+        <v>2523</v>
+      </c>
+      <c r="M1493" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1493" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1493" t="s">
+        <v>2521</v>
+      </c>
+      <c r="Q1493" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1494" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1494" t="s">
+        <v>2525</v>
+      </c>
+      <c r="M1494" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1494" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1494" t="s">
+        <v>2524</v>
+      </c>
+      <c r="Q1494" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1495" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1495" t="s">
+        <v>2525</v>
+      </c>
+      <c r="M1495" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1495" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1495" t="s">
+        <v>2526</v>
+      </c>
+      <c r="Q1495" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1496" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1496" t="s">
+        <v>2525</v>
+      </c>
+      <c r="M1496" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1496" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1496" t="s">
+        <v>2527</v>
+      </c>
+      <c r="Q1496" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1497" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1497" t="s">
+        <v>2529</v>
+      </c>
+      <c r="M1497" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1497" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1497" t="s">
+        <v>2528</v>
+      </c>
+      <c r="Q1497" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1498" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1498" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1498" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1498" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1498" t="s">
+        <v>2530</v>
+      </c>
+      <c r="Q1498" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1499" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1499" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1499" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1499" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1499" t="s">
+        <v>2532</v>
+      </c>
+      <c r="Q1499" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1500" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1500" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1500" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1500" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1500" t="s">
+        <v>2533</v>
+      </c>
+      <c r="Q1500" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1501" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1501" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1501" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1501" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1501" t="s">
+        <v>2534</v>
+      </c>
+      <c r="Q1501" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1502" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1502" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1502" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1502" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1502" t="s">
+        <v>2535</v>
+      </c>
+      <c r="Q1502" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1503" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1503" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1503" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1503" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1503" t="s">
+        <v>2536</v>
+      </c>
+      <c r="Q1503" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1504" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1504" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1504" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1504" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1504" t="s">
+        <v>2537</v>
+      </c>
+      <c r="Q1504" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1505" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1505" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1505" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1505" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1505" t="s">
+        <v>2538</v>
+      </c>
+      <c r="Q1505" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1506" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1506" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1506" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1506" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1506" t="s">
+        <v>2539</v>
+      </c>
+      <c r="Q1506" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1507" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1507" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1507" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1507" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1507" t="s">
+        <v>2540</v>
+      </c>
+      <c r="Q1507" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1508" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1508" t="s">
+        <v>2531</v>
+      </c>
+      <c r="M1508" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1508" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1508" t="s">
+        <v>2541</v>
+      </c>
+      <c r="Q1508" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -70980,6 +73275,7 @@
     <hyperlink ref="P1308" r:id="rId2"/>
     <hyperlink ref="P1323" r:id="rId3"/>
     <hyperlink ref="P1327" r:id="rId4"/>
+    <hyperlink ref="P1452" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
TD ML = 1600
</commit_message>
<xml_diff>
--- a/webserver/model_data/TrainingData_ml.xlsx
+++ b/webserver/model_data/TrainingData_ml.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14868" uniqueCount="2542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15338" uniqueCount="2690">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -7677,12 +7677,456 @@
   <si>
     <t>Entsprechend sind dann ihre Reaktionen.</t>
   </si>
+  <si>
+    <t>Die Klimabewegung ist eine Kampagne der Anhänger der Linken Weltanschauung.</t>
+  </si>
+  <si>
+    <t>Diogenes</t>
+  </si>
+  <si>
+    <t>Das war so , das ist so und das wird auch so bleiben.</t>
+  </si>
+  <si>
+    <t>Heinrich Seidelbast</t>
+  </si>
+  <si>
+    <t>Die Meinung ist kritisch, ich teile sie nicht unbedingt, aber er hat schon einen Punkt.</t>
+  </si>
+  <si>
+    <t>Alex Bruckes</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=f7JXQfT9ou0</t>
+  </si>
+  <si>
+    <t>Respekt vor euch beiden</t>
+  </si>
+  <si>
+    <t>Volcom2712</t>
+  </si>
+  <si>
+    <t>Sehr gutes Interview, sehr angenehme Gesprächsführung und sehr wichtiger Dialog</t>
+  </si>
+  <si>
+    <t>Relativ neutrales Interview</t>
+  </si>
+  <si>
+    <t>Loki Wassolls</t>
+  </si>
+  <si>
+    <t>Ein sehr wissenswertes interview</t>
+  </si>
+  <si>
+    <t>Zeigt durchaus auch, dass, wenn ich auch in sehr vielen Dingen nicht seiner Meinung bin, es total falsch ist, jeden per se als Nazi abzustempeln</t>
+  </si>
+  <si>
+    <t>LunnarisLP</t>
+  </si>
+  <si>
+    <t>Igitt!!! Wie kann man nur so miesepetrig und gleichzeitig hochnäsig sein.</t>
+  </si>
+  <si>
+    <t>quiscit</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/zeit-magazin/essen-trinken/2020-02/wermule-wermut-moscow-mule-cocktail-rezept</t>
+  </si>
+  <si>
+    <t>So, jetzt will ich sie aber nicht länger von ihrer guten Tasse Malventee abhalten</t>
+  </si>
+  <si>
+    <t>Sie kennen sich offenbar genauso gut aus wie die Autorin.</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/mobilitaet/2020-02/verkehrslaerm-hannover-laermblitzer-stadtverkehr-raser</t>
+  </si>
+  <si>
+    <t>Du Kati</t>
+  </si>
+  <si>
+    <t>Vielleicht einfach mal mit den aktuellen (und angekündigten) Zulassungsvorschriften beschäftigen</t>
+  </si>
+  <si>
+    <t>Nebenbei: schon mal mit Bussen, LKW, Flugzeugen und Bahnen beschäftigt?</t>
+  </si>
+  <si>
+    <t>Ja, der Lärm ist inzwischen Teil des „Sound-Designs“</t>
+  </si>
+  <si>
+    <t>Es ist echt unglaublich, dass so etwas überhaupt zugelassen wird</t>
+  </si>
+  <si>
+    <t>Man schafft damit für Wohlhabende, besonders Rücksichtslose oder einfach nur Machoidioten bewusst eine Möglichkeit andere zu schädigen und zu belästigen</t>
+  </si>
+  <si>
+    <t>ohdochnein</t>
+  </si>
+  <si>
+    <t>Dort zeugt ein lauter Auspuff von der universellen Potenz des Fahrers bzw. sehr selten: der Fahrerin</t>
+  </si>
+  <si>
+    <t>Zumindest nach Ansicht des Fahrers</t>
+  </si>
+  <si>
+    <t>1200KG</t>
+  </si>
+  <si>
+    <t>Und die sollte man zu Ende lesen, ob der vielen Ausnahmen die da drin stehen</t>
+  </si>
+  <si>
+    <t>Entenschorsch</t>
+  </si>
+  <si>
+    <t>es ist genau anders herum wie Sie es beschreiben</t>
+  </si>
+  <si>
+    <t>Und erst Recht blöde</t>
+  </si>
+  <si>
+    <t>Aha..der gute alte Whataboutism</t>
+  </si>
+  <si>
+    <t>Best Friend Tabitha</t>
+  </si>
+  <si>
+    <t>Auch Poser, wa?</t>
+  </si>
+  <si>
+    <t>Dinge, die die Welt nicht braucht</t>
+  </si>
+  <si>
+    <t>GlobalTraveler</t>
+  </si>
+  <si>
+    <t>dumme Antwort ist dumm</t>
+  </si>
+  <si>
+    <t>JanGoldbeck</t>
+  </si>
+  <si>
+    <t>Wohn mal in einer verkehrsberuhigten Seitenstraße für ne Weile und du kannst verstehen warum viele Menschen Autolärm verringern wollen</t>
+  </si>
+  <si>
+    <t>Kenne ich. Weiß man aber auch vor dem Einzug</t>
+  </si>
+  <si>
+    <t>Ich finde die Idee gut</t>
+  </si>
+  <si>
+    <t>diametral3.0</t>
+  </si>
+  <si>
+    <t>Sie haben wohl den Artikel nicht gelesen</t>
+  </si>
+  <si>
+    <t>raflix</t>
+  </si>
+  <si>
+    <t>Der gemeine Mortorradfahrer ist meist älter, gutsituiertm gehört zur Gruppe der Zahnwälte oder Beamten auf Midlifecrisis</t>
+  </si>
+  <si>
+    <t>yamxs1</t>
+  </si>
+  <si>
+    <t>und ist gleichzeitig auch der, der sich am meisten im eigenem Wohngebiet über den Lärm der Anderen aufregt</t>
+  </si>
+  <si>
+    <t>Mich nervt diese permanente Rücksichtslosigkeit und Poserei auf Kosten seiner Mitmenschen</t>
+  </si>
+  <si>
+    <t>Schneeregen</t>
+  </si>
+  <si>
+    <t>Was ist das denn für eine schwache Argumentation?</t>
+  </si>
+  <si>
+    <t>aderz</t>
+  </si>
+  <si>
+    <t>Es geht hier ja nicht um den normalen Lärm des Straßenverkehrs, sondern um Leute die absichtlich Lärm verursachen</t>
+  </si>
+  <si>
+    <t>Es sind einfach nur Regeln und Maßnahmen um Menschen vor unnötigen Lärm zu schützen</t>
+  </si>
+  <si>
+    <t>Schade, ich bin von Ihnen eigentlich eine bessere Argumentation gewohnt</t>
+  </si>
+  <si>
+    <t>Lies - den - Artikel - bevor - du - kommentierst!</t>
+  </si>
+  <si>
+    <t>Südvorstadt</t>
+  </si>
+  <si>
+    <t>Zieht - aufs - Land!</t>
+  </si>
+  <si>
+    <t>serdna</t>
+  </si>
+  <si>
+    <t>https://www.tagesspiegel.de/politik/us-demokraten-vor-dem-super-tuesday-es-laeuft-die-operation-bernie-verhindern/25603238.html</t>
+  </si>
+  <si>
+    <t>Bernie Sanders will eine Krankenversicherung für alle</t>
+  </si>
+  <si>
+    <t>Das kann man höchst vernünftig finden</t>
+  </si>
+  <si>
+    <t>Also die Aussage, dass es lediglich auf Personen ankommt, ist umfassender, totaler Schwachsinn.</t>
+  </si>
+  <si>
+    <t>hanebutt</t>
+  </si>
+  <si>
+    <t>Die Kulissenschieber bei den Demokraten sind wieder gefragt.</t>
+  </si>
+  <si>
+    <t>Nicht nur Trump beherrscht dieses Metier</t>
+  </si>
+  <si>
+    <t>auch die Demokraten sind darin bewandert</t>
+  </si>
+  <si>
+    <t>Sie sind leiser.</t>
+  </si>
+  <si>
+    <t>... die Innenpolitik ist unterschiedlich, alles andere gleich.</t>
+  </si>
+  <si>
+    <t>Er ist schriller, ansonsten ein ganz normaler Politiker der USA.</t>
+  </si>
+  <si>
+    <t>maxost</t>
+  </si>
+  <si>
+    <t>Es zählt wer am Ende gewinnt</t>
+  </si>
+  <si>
+    <t>Sanders ist eine politische Vogelscheuche außerhalb eines linken innerparteilichen Spektrums</t>
+  </si>
+  <si>
+    <t>2010ff</t>
+  </si>
+  <si>
+    <t>Hier wird deutlich: Der Begriff "moderat" für Leute wie Biden ist "Fake-News".</t>
+  </si>
+  <si>
+    <t>teesieb</t>
+  </si>
+  <si>
+    <t>"Bernie verhindern" heißt, Trump die Präsidentschaft zu sichern.</t>
+  </si>
+  <si>
+    <t>ist schon lange, daß die etablierten Dems sich gut mit Trump arrangiert haben</t>
+  </si>
+  <si>
+    <t>Das war auch schon 2016 bei der intrigant vorgehenden Clinton und den sie unterstützenden Medien so.</t>
+  </si>
+  <si>
+    <t>Es darf halt nicht dazu kommen, dass der gesetzliche Mindestlohn steigt.</t>
+  </si>
+  <si>
+    <t>Ja, Demokratie ist in den USA eine in jeder Hinsicht extreme Sache.</t>
+  </si>
+  <si>
+    <t>derbergruft</t>
+  </si>
+  <si>
+    <t>https://www.tagesspiegel.de/wirtschaft/entscheidung-ueber-automobil-ausstellung-iaa-soll-nach-muenchen-gehen/25603462.html</t>
+  </si>
+  <si>
+    <t>Super!</t>
+  </si>
+  <si>
+    <t>Gute Entscheidung für Berlin</t>
+  </si>
+  <si>
+    <t>Stimmt auch wieder, muß ja keiner müssen.</t>
+  </si>
+  <si>
+    <t>Anarc</t>
+  </si>
+  <si>
+    <t>In keinem Bundesland sitzt die Autolobby derart deutlich mit in der Regierung als in Bayern.</t>
+  </si>
+  <si>
+    <t>Die IAA paßt dorthin.</t>
+  </si>
+  <si>
+    <t>Eine gute Entscheidung.</t>
+  </si>
+  <si>
+    <t>In Berlin wollen wir die stinkenden Kisten nicht mehr.</t>
+  </si>
+  <si>
+    <t>Berliner8000</t>
+  </si>
+  <si>
+    <t>Also Leute bin ich der Einzige, der die Standortwahl nicht versteht im Moment?</t>
+  </si>
+  <si>
+    <t>Eine Neuausrichtung, wie behauptet, weshalb man eigtl. von Frankfurt wegzog, sind eindeutig anders aus.</t>
+  </si>
+  <si>
+    <t>W.Wang</t>
+  </si>
+  <si>
+    <t>Die autogerechte Stadt war das Modell des 20. Jahrhunderts.</t>
+  </si>
+  <si>
+    <t>Viel Spaß nach München mit der IAA.</t>
+  </si>
+  <si>
+    <t>Thalmayr</t>
+  </si>
+  <si>
+    <t>Hoffentlich stimmt diese Meldung auch.</t>
+  </si>
+  <si>
+    <t>sciaridae</t>
+  </si>
+  <si>
+    <t>Ein Segen, dass dieser Schwachsinn nicht in Berlin veranstaltet wird.</t>
+  </si>
+  <si>
+    <t>Null Substanz, wie gewohnt.</t>
+  </si>
+  <si>
+    <t>Getiton</t>
+  </si>
+  <si>
+    <t>Hier werden Waren und Menschen nach Berlin gebracht.</t>
+  </si>
+  <si>
+    <t>Alles CO2 schädlich.</t>
+  </si>
+  <si>
+    <t>Wirtschaft/Geldverdienen ist hier auch verpönt.</t>
+  </si>
+  <si>
+    <t>Täglich kann man im TV beobachten, mit welchen Karossen die Herrschaften durch die Lande fahren.</t>
+  </si>
+  <si>
+    <t>Und dann ist es auch richtig, wenn Bayern die IAA bekommt.</t>
+  </si>
+  <si>
+    <t>hedgehog</t>
+  </si>
+  <si>
+    <t>Da spielt wohl auch Tesla eine Rolle.</t>
+  </si>
+  <si>
+    <t>mitte31</t>
+  </si>
+  <si>
+    <t>Eine nachvollziehbare Entscheidung.</t>
+  </si>
+  <si>
+    <t>Die Berliner Regierung sowie ein Teil der Berliner Bevölkerung sind Autofeinde.</t>
+  </si>
+  <si>
+    <t>StolzwieBolle</t>
+  </si>
+  <si>
+    <t>...die Messe Berlin macht einen guten Job,</t>
+  </si>
+  <si>
+    <t>Die verkraftet das problemlos.</t>
+  </si>
+  <si>
+    <t>Netiew</t>
+  </si>
+  <si>
+    <t>https://www.tagesspiegel.de/kultur/mailaender-lehrer-schreibt-brief-an-schueler-das-groesste-risiko-ist-nicht-das-coronavirus/25601804.html#</t>
+  </si>
+  <si>
+    <t>Diesen wunderbaren Brief ...</t>
+  </si>
+  <si>
+    <t>herjeh</t>
+  </si>
+  <si>
+    <t>https://www.tagesspiegel.de/kultur/neuer-james-bond-song-so-klingt-no-time-to-die-von-billie-eilish/25546338.html</t>
+  </si>
+  <si>
+    <t>Hier wird mal wieder deutlich, dass man keine Stimme haben muß um Erfolg zu haben.</t>
+  </si>
+  <si>
+    <t>devvkon</t>
+  </si>
+  <si>
+    <t>Einverstanden!</t>
+  </si>
+  <si>
+    <t>... klingt aber wie der vierte Aufguss Grüntee schmeckt:...</t>
+  </si>
+  <si>
+    <t>Stimmt aber nicht immer.</t>
+  </si>
+  <si>
+    <t>margard</t>
+  </si>
+  <si>
+    <t>Dito, sieht man aber auch am ESC</t>
+  </si>
+  <si>
+    <t>JuergenHockensberg</t>
+  </si>
+  <si>
+    <t>Sorry, da möchte ich Ihnen widersprechen, ...</t>
+  </si>
+  <si>
+    <t>klaus14513</t>
+  </si>
+  <si>
+    <t>... aber wissen sie überhaupt wer Billie Eilish ist?</t>
+  </si>
+  <si>
+    <t>carnet</t>
+  </si>
+  <si>
+    <t>https://www.tagesspiegel.de/kultur/justin-biebers-comebackalbum-changes-gesang-ohne-emotionen-lyrics-zum-fremdschaemen/25551754.html</t>
+  </si>
+  <si>
+    <t>Bieber ist und bleibt ein Proll.</t>
+  </si>
+  <si>
+    <t>Tja, und? :)</t>
+  </si>
+  <si>
+    <t>turbo_p</t>
+  </si>
+  <si>
+    <t>https://www.tagesspiegel.de/berlin/vorbereitung-auf-das-coronavirus-aerzte-suchen-schon-im-baumarkt-nach-einem-mundschutz/25598504.html</t>
+  </si>
+  <si>
+    <t>Eine Schande ist das.</t>
+  </si>
+  <si>
+    <t>Korsowolf</t>
+  </si>
+  <si>
+    <t>Man sollte sich nicht an der Nase herumführen lassen.</t>
+  </si>
+  <si>
+    <t>Auch in Deutschland.</t>
+  </si>
+  <si>
+    <t>Ist doch wohl lachhaft,</t>
+  </si>
+  <si>
+    <t>Ja blöde, dass ...</t>
+  </si>
+  <si>
+    <t>berit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7702,6 +8146,29 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -7736,16 +8203,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8043,12 +8516,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1508"/>
+  <dimension ref="A1:W1602"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1484" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1583" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="P1509" sqref="P1509"/>
+      <selection pane="bottomLeft" activeCell="B1548" sqref="B1548:B1602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -73269,6 +73742,1660 @@
         <v>18</v>
       </c>
     </row>
+    <row r="1509" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1509" t="s">
+        <v>2543</v>
+      </c>
+      <c r="M1509" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1509" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1509" t="s">
+        <v>2542</v>
+      </c>
+      <c r="Q1509" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1510" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1510" t="s">
+        <v>2545</v>
+      </c>
+      <c r="M1510" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1510" t="s">
+        <v>2522</v>
+      </c>
+      <c r="P1510" t="s">
+        <v>2544</v>
+      </c>
+      <c r="Q1510" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1511" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1511" t="s">
+        <v>2547</v>
+      </c>
+      <c r="M1511" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1511" t="s">
+        <v>2548</v>
+      </c>
+      <c r="P1511" t="s">
+        <v>2546</v>
+      </c>
+      <c r="Q1511" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1512" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1512" t="s">
+        <v>2550</v>
+      </c>
+      <c r="M1512" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1512" t="s">
+        <v>2548</v>
+      </c>
+      <c r="P1512" t="s">
+        <v>2549</v>
+      </c>
+      <c r="Q1512" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1513" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1513" t="s">
+        <v>2550</v>
+      </c>
+      <c r="M1513" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1513" t="s">
+        <v>2548</v>
+      </c>
+      <c r="P1513" t="s">
+        <v>2551</v>
+      </c>
+      <c r="Q1513" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1514" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1514" t="s">
+        <v>2553</v>
+      </c>
+      <c r="M1514" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1514" t="s">
+        <v>2548</v>
+      </c>
+      <c r="P1514" t="s">
+        <v>2552</v>
+      </c>
+      <c r="Q1514" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1515" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1515" t="s">
+        <v>2556</v>
+      </c>
+      <c r="M1515" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1515" t="s">
+        <v>2548</v>
+      </c>
+      <c r="P1515" t="s">
+        <v>2554</v>
+      </c>
+      <c r="Q1515" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1516" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1516" t="s">
+        <v>2556</v>
+      </c>
+      <c r="M1516" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1516" t="s">
+        <v>2548</v>
+      </c>
+      <c r="P1516" t="s">
+        <v>2555</v>
+      </c>
+      <c r="Q1516" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1517" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1517" t="s">
+        <v>2558</v>
+      </c>
+      <c r="M1517" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1517" t="s">
+        <v>2559</v>
+      </c>
+      <c r="P1517" t="s">
+        <v>2557</v>
+      </c>
+      <c r="Q1517" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1518" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1518" t="s">
+        <v>2558</v>
+      </c>
+      <c r="M1518" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N1518" t="s">
+        <v>2559</v>
+      </c>
+      <c r="P1518" t="s">
+        <v>2560</v>
+      </c>
+      <c r="Q1518" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1519" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1519" t="s">
+        <v>2563</v>
+      </c>
+      <c r="M1519" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1519" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1519" t="s">
+        <v>2561</v>
+      </c>
+      <c r="Q1519" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1520" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1520" t="s">
+        <v>2563</v>
+      </c>
+      <c r="M1520" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1520" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1520" t="s">
+        <v>2564</v>
+      </c>
+      <c r="Q1520" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1521" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1521" t="s">
+        <v>2563</v>
+      </c>
+      <c r="M1521" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1521" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1521" t="s">
+        <v>2565</v>
+      </c>
+      <c r="Q1521" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1522" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1522" t="s">
+        <v>1380</v>
+      </c>
+      <c r="M1522" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1522" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1522" t="s">
+        <v>2566</v>
+      </c>
+      <c r="Q1522" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1523" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1523" t="s">
+        <v>1380</v>
+      </c>
+      <c r="M1523" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1523" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1523" t="s">
+        <v>2567</v>
+      </c>
+      <c r="Q1523" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1524" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1524" t="s">
+        <v>2569</v>
+      </c>
+      <c r="M1524" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1524" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1524" t="s">
+        <v>2568</v>
+      </c>
+      <c r="Q1524" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1525" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1525" t="s">
+        <v>2572</v>
+      </c>
+      <c r="M1525" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1525" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1525" t="s">
+        <v>2570</v>
+      </c>
+      <c r="Q1525" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1526" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1526" t="s">
+        <v>2572</v>
+      </c>
+      <c r="M1526" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1526" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1526" t="s">
+        <v>2571</v>
+      </c>
+      <c r="Q1526" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1527" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1527" t="s">
+        <v>2574</v>
+      </c>
+      <c r="M1527" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1527" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1527" t="s">
+        <v>2573</v>
+      </c>
+      <c r="Q1527" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1528" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1528" t="s">
+        <v>2574</v>
+      </c>
+      <c r="M1528" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1528" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1528" t="s">
+        <v>2575</v>
+      </c>
+      <c r="Q1528" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1529" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1529" t="s">
+        <v>2574</v>
+      </c>
+      <c r="M1529" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1529" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1529" t="s">
+        <v>2576</v>
+      </c>
+      <c r="Q1529" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1530" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1530" t="s">
+        <v>2578</v>
+      </c>
+      <c r="M1530" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1530" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1530" t="s">
+        <v>2577</v>
+      </c>
+      <c r="Q1530" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1531" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1531" t="s">
+        <v>2578</v>
+      </c>
+      <c r="M1531" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1531" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1531" t="s">
+        <v>2579</v>
+      </c>
+      <c r="Q1531" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1532" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1532" t="s">
+        <v>2581</v>
+      </c>
+      <c r="M1532" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1532" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1532" t="s">
+        <v>2580</v>
+      </c>
+      <c r="Q1532" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1533" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1533" t="s">
+        <v>2583</v>
+      </c>
+      <c r="M1533" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1533" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1533" t="s">
+        <v>2582</v>
+      </c>
+      <c r="Q1533" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1534" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1534" t="s">
+        <v>2583</v>
+      </c>
+      <c r="M1534" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1534" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1534" t="s">
+        <v>2584</v>
+      </c>
+      <c r="Q1534" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1535" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1535" t="s">
+        <v>2581</v>
+      </c>
+      <c r="M1535" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1535" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1535" t="s">
+        <v>2585</v>
+      </c>
+      <c r="Q1535" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1536" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L1536" t="s">
+        <v>2587</v>
+      </c>
+      <c r="M1536" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1536" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1536" t="s">
+        <v>2586</v>
+      </c>
+      <c r="Q1536" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1537" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L1537" t="s">
+        <v>2589</v>
+      </c>
+      <c r="M1537" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1537" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1537" t="s">
+        <v>2588</v>
+      </c>
+      <c r="Q1537" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1538" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L1538" t="s">
+        <v>2591</v>
+      </c>
+      <c r="M1538" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1538" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1538" t="s">
+        <v>2590</v>
+      </c>
+      <c r="Q1538" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1539" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L1539" t="s">
+        <v>2591</v>
+      </c>
+      <c r="M1539" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1539" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1539" t="s">
+        <v>2592</v>
+      </c>
+      <c r="Q1539" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1540" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L1540" t="s">
+        <v>2594</v>
+      </c>
+      <c r="M1540" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1540" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1540" t="s">
+        <v>2593</v>
+      </c>
+      <c r="Q1540" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1541" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L1541" t="s">
+        <v>2596</v>
+      </c>
+      <c r="M1541" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1541" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1541" t="s">
+        <v>2595</v>
+      </c>
+      <c r="Q1541" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1542" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L1542" t="s">
+        <v>2596</v>
+      </c>
+      <c r="M1542" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1542" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1542" t="s">
+        <v>2597</v>
+      </c>
+      <c r="Q1542" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1543" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L1543" t="s">
+        <v>2596</v>
+      </c>
+      <c r="M1543" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1543" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1543" t="s">
+        <v>2598</v>
+      </c>
+      <c r="Q1543" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1544" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L1544" t="s">
+        <v>2596</v>
+      </c>
+      <c r="M1544" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1544" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1544" t="s">
+        <v>2599</v>
+      </c>
+      <c r="Q1544" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1545" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L1545" t="s">
+        <v>2601</v>
+      </c>
+      <c r="M1545" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1545" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1545" t="s">
+        <v>2600</v>
+      </c>
+      <c r="Q1545" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1546" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L1546" t="s">
+        <v>2581</v>
+      </c>
+      <c r="M1546" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1546" t="s">
+        <v>2562</v>
+      </c>
+      <c r="P1546" t="s">
+        <v>2602</v>
+      </c>
+      <c r="Q1546" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1547" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B1547" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1547" s="2" t="s">
+        <v>2603</v>
+      </c>
+      <c r="M1547" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1547" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1547" s="2"/>
+      <c r="P1547" s="4" t="s">
+        <v>2605</v>
+      </c>
+    </row>
+    <row r="1548" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B1548" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1548" s="2" t="s">
+        <v>2603</v>
+      </c>
+      <c r="M1548" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1548" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1548" s="2"/>
+      <c r="P1548" s="4" t="s">
+        <v>2606</v>
+      </c>
+    </row>
+    <row r="1549" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B1549" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1549" s="2" t="s">
+        <v>2603</v>
+      </c>
+      <c r="M1549" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1549" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1549" s="2"/>
+      <c r="P1549" s="4" t="s">
+        <v>2607</v>
+      </c>
+    </row>
+    <row r="1550" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B1550" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1550" s="2" t="s">
+        <v>2608</v>
+      </c>
+      <c r="M1550" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1550" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1550" s="2"/>
+      <c r="P1550" s="4" t="s">
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="1551" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B1551" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1551" s="2" t="s">
+        <v>2608</v>
+      </c>
+      <c r="M1551" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1551" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1551" s="2"/>
+      <c r="P1551" s="4" t="s">
+        <v>2610</v>
+      </c>
+    </row>
+    <row r="1552" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B1552" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1552" s="2" t="s">
+        <v>2608</v>
+      </c>
+      <c r="M1552" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1552" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1552" s="2"/>
+      <c r="P1552" s="2" t="s">
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="1553" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1553" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1553" s="2" t="s">
+        <v>2608</v>
+      </c>
+      <c r="M1553" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1553" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1553" s="2"/>
+      <c r="P1553" s="4" t="s">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="1554" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1554" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1554" s="5" t="s">
+        <v>2608</v>
+      </c>
+      <c r="M1554" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1554" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1554" s="2"/>
+      <c r="P1554" s="4" t="s">
+        <v>2613</v>
+      </c>
+    </row>
+    <row r="1555" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1555" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1555" s="5" t="s">
+        <v>2608</v>
+      </c>
+      <c r="M1555" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1555" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1555" s="2"/>
+      <c r="P1555" s="4" t="s">
+        <v>2614</v>
+      </c>
+    </row>
+    <row r="1556" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1556" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1556" s="2" t="s">
+        <v>2615</v>
+      </c>
+      <c r="M1556" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1556" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1556" s="2"/>
+      <c r="P1556" s="4" t="s">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="1557" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1557" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1557" s="2" t="s">
+        <v>2615</v>
+      </c>
+      <c r="M1557" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1557" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1557" s="2"/>
+      <c r="P1557" s="4" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="1558" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1558" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1558" s="2" t="s">
+        <v>2618</v>
+      </c>
+      <c r="M1558" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1558" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1558" s="2"/>
+      <c r="P1558" s="4" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="1559" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1559" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1559" s="2" t="s">
+        <v>2620</v>
+      </c>
+      <c r="M1559" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1559" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1559" s="2"/>
+      <c r="P1559" s="4" t="s">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="1560" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1560" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1560" s="5" t="s">
+        <v>2620</v>
+      </c>
+      <c r="M1560" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1560" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1560" s="2"/>
+      <c r="P1560" s="4" t="s">
+        <v>2622</v>
+      </c>
+    </row>
+    <row r="1561" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1561" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1561" s="5" t="s">
+        <v>2618</v>
+      </c>
+      <c r="M1561" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1561" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1561" s="2"/>
+      <c r="P1561" s="4" t="s">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="1562" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1562" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1562" s="2" t="s">
+        <v>2618</v>
+      </c>
+      <c r="M1562" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1562" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1562" s="2"/>
+      <c r="P1562" s="4" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="1563" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1563" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1563" s="5" t="s">
+        <v>2618</v>
+      </c>
+      <c r="M1563" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1563" s="3" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O1563" s="2"/>
+      <c r="P1563" s="4" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="1564" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1564" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1564" s="2" t="s">
+        <v>2626</v>
+      </c>
+      <c r="M1564" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1564" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1564" s="2"/>
+      <c r="P1564" s="4" t="s">
+        <v>2628</v>
+      </c>
+    </row>
+    <row r="1565" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1565" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1565" s="5" t="s">
+        <v>2626</v>
+      </c>
+      <c r="M1565" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1565" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1565" s="2"/>
+      <c r="P1565" s="2" t="s">
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="1566" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1566" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1566" s="5" t="s">
+        <v>2626</v>
+      </c>
+      <c r="M1566" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1566" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1566" s="2"/>
+      <c r="P1566" s="4" t="s">
+        <v>2630</v>
+      </c>
+    </row>
+    <row r="1567" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1567" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1567" s="2" t="s">
+        <v>2631</v>
+      </c>
+      <c r="M1567" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1567" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1567" s="2"/>
+      <c r="P1567" s="4" t="s">
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="1568" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1568" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1568" s="5" t="s">
+        <v>2631</v>
+      </c>
+      <c r="M1568" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1568" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1568" s="2"/>
+      <c r="P1568" s="4" t="s">
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="1569" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1569" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1569" s="5" t="s">
+        <v>2631</v>
+      </c>
+      <c r="M1569" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1569" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1569" s="2"/>
+      <c r="P1569" s="4" t="s">
+        <v>2634</v>
+      </c>
+    </row>
+    <row r="1570" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1570" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1570" s="5" t="s">
+        <v>2631</v>
+      </c>
+      <c r="M1570" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1570" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1570" s="2"/>
+      <c r="P1570" s="4" t="s">
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="1571" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1571" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1571" s="2" t="s">
+        <v>2636</v>
+      </c>
+      <c r="M1571" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1571" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1571" s="2"/>
+      <c r="P1571" s="4" t="s">
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="1572" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1572" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1572" s="2" t="s">
+        <v>2636</v>
+      </c>
+      <c r="M1572" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1572" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1572" s="2"/>
+      <c r="P1572" s="4" t="s">
+        <v>2638</v>
+      </c>
+    </row>
+    <row r="1573" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1573" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1573" s="2" t="s">
+        <v>2639</v>
+      </c>
+      <c r="M1573" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1573" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1573" s="2"/>
+      <c r="P1573" s="4" t="s">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="1574" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1574" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1574" s="2" t="s">
+        <v>2639</v>
+      </c>
+      <c r="M1574" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1574" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1574" s="2"/>
+      <c r="P1574" s="4" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="1575" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1575" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1575" s="2" t="s">
+        <v>2642</v>
+      </c>
+      <c r="M1575" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1575" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1575" s="2"/>
+      <c r="P1575" s="4" t="s">
+        <v>2643</v>
+      </c>
+    </row>
+    <row r="1576" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1576" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1576" s="2" t="s">
+        <v>2644</v>
+      </c>
+      <c r="M1576" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1576" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1576" s="2"/>
+      <c r="P1576" s="4" t="s">
+        <v>2645</v>
+      </c>
+    </row>
+    <row r="1577" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1577" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1577" s="2" t="s">
+        <v>2644</v>
+      </c>
+      <c r="M1577" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1577" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1577" s="2"/>
+      <c r="P1577" s="4" t="s">
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="1578" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1578" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1578" s="2" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M1578" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1578" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1578" s="2"/>
+      <c r="P1578" s="4" t="s">
+        <v>2648</v>
+      </c>
+    </row>
+    <row r="1579" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1579" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1579" s="5" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M1579" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1579" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1579" s="2"/>
+      <c r="P1579" s="4" t="s">
+        <v>2649</v>
+      </c>
+    </row>
+    <row r="1580" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1580" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1580" s="5" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M1580" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1580" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1580" s="2"/>
+      <c r="P1580" s="4" t="s">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="1581" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1581" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1581" s="5" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M1581" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1581" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1581" s="2"/>
+      <c r="P1581" s="4" t="s">
+        <v>2651</v>
+      </c>
+    </row>
+    <row r="1582" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1582" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1582" s="2" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M1582" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1582" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1582" s="2"/>
+      <c r="P1582" s="4" t="s">
+        <v>2652</v>
+      </c>
+    </row>
+    <row r="1583" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1583" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1583" s="2" t="s">
+        <v>2653</v>
+      </c>
+      <c r="M1583" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1583" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1583" s="2"/>
+      <c r="P1583" s="4" t="s">
+        <v>2654</v>
+      </c>
+    </row>
+    <row r="1584" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1584" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1584" s="2" t="s">
+        <v>2655</v>
+      </c>
+      <c r="M1584" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1584" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1584" s="2"/>
+      <c r="P1584" s="4" t="s">
+        <v>2656</v>
+      </c>
+    </row>
+    <row r="1585" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1585" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1585" s="2" t="s">
+        <v>2655</v>
+      </c>
+      <c r="M1585" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1585" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1585" s="2"/>
+      <c r="P1585" s="4" t="s">
+        <v>2657</v>
+      </c>
+    </row>
+    <row r="1586" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1586" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1586" s="2" t="s">
+        <v>2658</v>
+      </c>
+      <c r="M1586" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1586" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1586" s="2"/>
+      <c r="P1586" s="4" t="s">
+        <v>2659</v>
+      </c>
+    </row>
+    <row r="1587" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1587" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1587" s="2" t="s">
+        <v>2658</v>
+      </c>
+      <c r="M1587" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1587" s="3" t="s">
+        <v>2627</v>
+      </c>
+      <c r="O1587" s="2"/>
+      <c r="P1587" s="4" t="s">
+        <v>2660</v>
+      </c>
+    </row>
+    <row r="1588" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1588" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1588" s="2" t="s">
+        <v>2661</v>
+      </c>
+      <c r="M1588" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1588" s="3" t="s">
+        <v>2662</v>
+      </c>
+      <c r="O1588" s="2"/>
+      <c r="P1588" s="4" t="s">
+        <v>2663</v>
+      </c>
+    </row>
+    <row r="1589" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1589" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1589" s="2" t="s">
+        <v>2664</v>
+      </c>
+      <c r="M1589" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1589" s="3" t="s">
+        <v>2665</v>
+      </c>
+      <c r="O1589" s="2"/>
+      <c r="P1589" s="4" t="s">
+        <v>2666</v>
+      </c>
+    </row>
+    <row r="1590" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1590" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1590" s="2" t="s">
+        <v>2667</v>
+      </c>
+      <c r="M1590" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1590" s="3" t="s">
+        <v>2665</v>
+      </c>
+      <c r="O1590" s="2"/>
+      <c r="P1590" s="4" t="s">
+        <v>2668</v>
+      </c>
+    </row>
+    <row r="1591" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1591" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1591" s="2" t="s">
+        <v>2667</v>
+      </c>
+      <c r="M1591" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1591" s="3" t="s">
+        <v>2665</v>
+      </c>
+      <c r="O1591" s="2"/>
+      <c r="P1591" s="4" t="s">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="1592" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1592" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1592" s="2" t="s">
+        <v>2664</v>
+      </c>
+      <c r="M1592" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1592" s="3" t="s">
+        <v>2665</v>
+      </c>
+      <c r="O1592" s="2"/>
+      <c r="P1592" s="4" t="s">
+        <v>2670</v>
+      </c>
+    </row>
+    <row r="1593" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1593" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1593" s="2" t="s">
+        <v>2671</v>
+      </c>
+      <c r="M1593" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1593" s="3" t="s">
+        <v>2665</v>
+      </c>
+      <c r="O1593" s="2"/>
+      <c r="P1593" s="4" t="s">
+        <v>2672</v>
+      </c>
+    </row>
+    <row r="1594" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1594" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1594" s="2" t="s">
+        <v>2673</v>
+      </c>
+      <c r="M1594" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1594" s="3" t="s">
+        <v>2665</v>
+      </c>
+      <c r="O1594" s="2"/>
+      <c r="P1594" s="4" t="s">
+        <v>2674</v>
+      </c>
+    </row>
+    <row r="1595" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1595" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1595" s="2" t="s">
+        <v>2675</v>
+      </c>
+      <c r="M1595" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1595" s="3" t="s">
+        <v>2665</v>
+      </c>
+      <c r="O1595" s="2"/>
+      <c r="P1595" s="4" t="s">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="1596" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1596" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1596" s="2" t="s">
+        <v>2677</v>
+      </c>
+      <c r="M1596" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1596" s="3" t="s">
+        <v>2678</v>
+      </c>
+      <c r="O1596" s="2"/>
+      <c r="P1596" s="4" t="s">
+        <v>2679</v>
+      </c>
+    </row>
+    <row r="1597" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1597" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1597" s="2" t="s">
+        <v>2644</v>
+      </c>
+      <c r="M1597" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="N1597" s="3" t="s">
+        <v>2678</v>
+      </c>
+      <c r="O1597" s="2"/>
+      <c r="P1597" s="4" t="s">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="1598" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1598" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1598" s="2" t="s">
+        <v>2681</v>
+      </c>
+      <c r="M1598" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1598" s="3" t="s">
+        <v>2682</v>
+      </c>
+      <c r="O1598" s="2"/>
+      <c r="P1598" s="4" t="s">
+        <v>2683</v>
+      </c>
+    </row>
+    <row r="1599" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1599" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1599" s="2" t="s">
+        <v>2684</v>
+      </c>
+      <c r="M1599" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1599" s="3" t="s">
+        <v>2682</v>
+      </c>
+      <c r="O1599" s="2"/>
+      <c r="P1599" s="4" t="s">
+        <v>2685</v>
+      </c>
+    </row>
+    <row r="1600" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1600" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1600" s="5" t="s">
+        <v>2684</v>
+      </c>
+      <c r="M1600" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1600" s="3" t="s">
+        <v>2682</v>
+      </c>
+      <c r="O1600" s="2"/>
+      <c r="P1600" s="4" t="s">
+        <v>2686</v>
+      </c>
+    </row>
+    <row r="1601" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1601" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1601" s="2" t="s">
+        <v>2684</v>
+      </c>
+      <c r="M1601" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1601" s="3" t="s">
+        <v>2682</v>
+      </c>
+      <c r="O1601" s="2"/>
+      <c r="P1601" s="4" t="s">
+        <v>2687</v>
+      </c>
+    </row>
+    <row r="1602" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B1602" t="s">
+        <v>2689</v>
+      </c>
+      <c r="L1602" s="2" t="s">
+        <v>2615</v>
+      </c>
+      <c r="M1602" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="N1602" s="3" t="s">
+        <v>2682</v>
+      </c>
+      <c r="O1602" s="2"/>
+      <c r="P1602" s="4" t="s">
+        <v>2688</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="P1306" r:id="rId1"/>
@@ -73276,6 +75403,62 @@
     <hyperlink ref="P1323" r:id="rId3"/>
     <hyperlink ref="P1327" r:id="rId4"/>
     <hyperlink ref="P1452" r:id="rId5"/>
+    <hyperlink ref="N1547" r:id="rId6"/>
+    <hyperlink ref="N1548" r:id="rId7"/>
+    <hyperlink ref="N1549" r:id="rId8"/>
+    <hyperlink ref="N1550" r:id="rId9"/>
+    <hyperlink ref="N1551" r:id="rId10"/>
+    <hyperlink ref="N1552" r:id="rId11"/>
+    <hyperlink ref="N1553" r:id="rId12"/>
+    <hyperlink ref="N1554" r:id="rId13"/>
+    <hyperlink ref="N1555" r:id="rId14"/>
+    <hyperlink ref="N1556" r:id="rId15"/>
+    <hyperlink ref="N1557" r:id="rId16"/>
+    <hyperlink ref="N1558" r:id="rId17"/>
+    <hyperlink ref="N1559" r:id="rId18"/>
+    <hyperlink ref="N1560" r:id="rId19"/>
+    <hyperlink ref="N1561" r:id="rId20"/>
+    <hyperlink ref="N1562" r:id="rId21"/>
+    <hyperlink ref="N1563" r:id="rId22"/>
+    <hyperlink ref="N1564" r:id="rId23"/>
+    <hyperlink ref="N1565" r:id="rId24"/>
+    <hyperlink ref="N1566" r:id="rId25"/>
+    <hyperlink ref="N1567" r:id="rId26"/>
+    <hyperlink ref="N1568" r:id="rId27"/>
+    <hyperlink ref="N1569" r:id="rId28"/>
+    <hyperlink ref="N1570" r:id="rId29"/>
+    <hyperlink ref="N1571" r:id="rId30"/>
+    <hyperlink ref="N1572" r:id="rId31"/>
+    <hyperlink ref="N1573" r:id="rId32"/>
+    <hyperlink ref="N1574" r:id="rId33"/>
+    <hyperlink ref="N1575" r:id="rId34"/>
+    <hyperlink ref="N1576" r:id="rId35"/>
+    <hyperlink ref="N1577" r:id="rId36"/>
+    <hyperlink ref="N1578" r:id="rId37"/>
+    <hyperlink ref="N1579" r:id="rId38"/>
+    <hyperlink ref="N1580" r:id="rId39"/>
+    <hyperlink ref="N1581" r:id="rId40"/>
+    <hyperlink ref="N1582" r:id="rId41"/>
+    <hyperlink ref="N1583" r:id="rId42"/>
+    <hyperlink ref="N1584" r:id="rId43"/>
+    <hyperlink ref="N1585" r:id="rId44"/>
+    <hyperlink ref="N1586" r:id="rId45"/>
+    <hyperlink ref="N1587" r:id="rId46"/>
+    <hyperlink ref="N1588" r:id="rId47"/>
+    <hyperlink ref="N1589" r:id="rId48"/>
+    <hyperlink ref="N1590" r:id="rId49"/>
+    <hyperlink ref="N1591" r:id="rId50"/>
+    <hyperlink ref="N1592" r:id="rId51"/>
+    <hyperlink ref="N1593" r:id="rId52"/>
+    <hyperlink ref="N1594" r:id="rId53"/>
+    <hyperlink ref="N1595" r:id="rId54"/>
+    <hyperlink ref="N1596" r:id="rId55"/>
+    <hyperlink ref="N1597" r:id="rId56"/>
+    <hyperlink ref="N1598" r:id="rId57"/>
+    <hyperlink ref="N1599" r:id="rId58"/>
+    <hyperlink ref="N1600" r:id="rId59"/>
+    <hyperlink ref="N1601" r:id="rId60"/>
+    <hyperlink ref="N1602" r:id="rId61"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>